<commit_message>
* Updated Time spent per member per week and activity.docx and Graphs.xlsx * Modified Time Management Account.docx : Finished Part 4.1, moved to 4.2
</commit_message>
<xml_diff>
--- a/doc/End of Project Report/Graphs.xlsx
+++ b/doc/End of Project Report/Graphs.xlsx
@@ -16,196 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="83">
-  <si>
-    <t>Process / Member</t>
-  </si>
-  <si>
-    <t>Edward</t>
-  </si>
-  <si>
-    <t>Kristian</t>
-  </si>
-  <si>
-    <t>Brian</t>
-  </si>
-  <si>
-    <t>Oscar</t>
-  </si>
-  <si>
-    <t>Kelvin</t>
-  </si>
-  <si>
-    <t>Week 1 : 19.5 hours</t>
-  </si>
-  <si>
-    <t>Project Plan : 19.5 hours</t>
-  </si>
-  <si>
-    <t>Gantt Chart and Work Breakdown</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Risk Analysis </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Budget </t>
-  </si>
-  <si>
-    <t>Project Management</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reviewing </t>
-  </si>
-  <si>
-    <t>Week 2 : 6.5 hours</t>
-  </si>
-  <si>
-    <t>Analysis, Design and Testing  : 6.5 hours</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Title, Introduction and Revision History </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description of Approach </t>
-  </si>
-  <si>
-    <t xml:space="preserve">UML for Requirements </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Human Computer Interaction </t>
-  </si>
-  <si>
-    <t>Week 3 : 26 hours</t>
-  </si>
-  <si>
-    <t>Analysis, Design and Testing : 16.25 hours</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UML for Design </t>
-  </si>
-  <si>
-    <t>Programming : 9.75 hours</t>
-  </si>
-  <si>
-    <t>Model</t>
-  </si>
-  <si>
-    <t>View</t>
-  </si>
-  <si>
-    <t>Week 4 : 15.5 hours</t>
-  </si>
-  <si>
-    <t>Analysis, Design and Testing : 2.5 hours</t>
-  </si>
-  <si>
-    <t>Test plan</t>
-  </si>
-  <si>
-    <t>Programming : 13 hours</t>
-  </si>
-  <si>
-    <t>Subtotal</t>
-  </si>
-  <si>
-    <t>Week 5 : 38 hours</t>
-  </si>
-  <si>
-    <t>Programming : 5.5 hours</t>
-  </si>
-  <si>
-    <t>Presentation : 30 hours</t>
-  </si>
-  <si>
-    <t>Discussion and Group Preparation</t>
-  </si>
-  <si>
-    <t>Prepare Slides</t>
-  </si>
-  <si>
-    <t>Rehearsal</t>
-  </si>
-  <si>
-    <t>Week 6 : 6 hours</t>
-  </si>
-  <si>
-    <t>Programming : 6 hours</t>
-  </si>
-  <si>
-    <t>Controller</t>
-  </si>
-  <si>
-    <t>Week 7 : 9.5 hours</t>
-  </si>
-  <si>
-    <t>Programming : 9.5 hours</t>
-  </si>
-  <si>
-    <t>Week 8 : 27.25</t>
-  </si>
-  <si>
-    <t>Analysis, Design and Testing : 4 hours</t>
-  </si>
-  <si>
-    <t>UML</t>
-  </si>
-  <si>
-    <t>Programming : 15.75 hours</t>
-  </si>
-  <si>
-    <t>Integration</t>
-  </si>
-  <si>
-    <t>Testing : 2.5 hours</t>
-  </si>
-  <si>
-    <t>Unit testing</t>
-  </si>
-  <si>
-    <t>Final Report : 6.5 hours</t>
-  </si>
-  <si>
-    <t>Final Report</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Week 9 : </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Analysis, Design and Testing </t>
-  </si>
-  <si>
-    <t>UML for Requirements</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Programming </t>
-  </si>
-  <si>
-    <t>Formal &amp; informal meetings</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Breakdown</t>
-  </si>
-  <si>
-    <t>Project Plan : 19.5 h</t>
-  </si>
-  <si>
-    <t>Analysis, Design &amp; Testing : 38.75 h</t>
-  </si>
-  <si>
-    <t>Programming : 75.5 h</t>
-  </si>
-  <si>
-    <t>Testing : 2.5 h</t>
-  </si>
-  <si>
-    <t>First Presentation : 30 h</t>
-  </si>
-  <si>
-    <t>Final Report : 10.5 h</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>Edward</t>
     <phoneticPr fontId="10" type="noConversion"/>
@@ -292,7 +103,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="180" formatCode="m&quot;月&quot;d&quot;日&quot;"/>
+    <numFmt numFmtId="176" formatCode="m&quot;月&quot;d&quot;日&quot;"/>
   </numFmts>
   <fonts count="11">
     <font>
@@ -389,7 +200,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -473,13 +284,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -549,28 +375,10 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -600,37 +408,85 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -756,7 +612,7 @@
                   <c:v>12.25</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.5</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -845,7 +701,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -934,7 +790,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.5</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1023,7 +879,7 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1123,31 +979,31 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10</c:v>
+                  <c:v>16.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="76927744"/>
-        <c:axId val="76929280"/>
+        <c:axId val="42738048"/>
+        <c:axId val="42739584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="76927744"/>
+        <c:axId val="42738048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76929280"/>
+        <c:crossAx val="42739584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76929280"/>
+        <c:axId val="42739584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1155,7 +1011,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0_);\(#,##0\)" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76927744"/>
+        <c:crossAx val="42738048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1168,7 +1024,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1261,10 +1117,13 @@
                   <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.75</c:v>
+                  <c:v>29.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1323,7 +1182,7 @@
                   <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>6</c:v>
@@ -1385,13 +1244,13 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1447,16 +1306,19 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.5</c:v>
+                  <c:v>7.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1515,41 +1377,41 @@
                   <c:v>3.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11</c:v>
+                  <c:v>17.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="71132288"/>
-        <c:axId val="71164288"/>
+        <c:axId val="42788352"/>
+        <c:axId val="42789888"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="71132288"/>
+        <c:axId val="42788352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71164288"/>
+        <c:crossAx val="42789888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71164288"/>
+        <c:axId val="42789888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1557,7 +1419,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71132288"/>
+        <c:crossAx val="42788352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1570,7 +1432,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1928,8 +1790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="O85" sqref="O85"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Y10" sqref="Y10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1945,684 +1807,507 @@
     <row r="2" spans="1:21" ht="17.25" thickBot="1">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="J2" s="49" t="s">
-        <v>63</v>
-      </c>
-      <c r="K2" s="49" t="s">
-        <v>73</v>
-      </c>
-      <c r="L2" s="49" t="s">
-        <v>74</v>
-      </c>
-      <c r="M2" s="49" t="s">
-        <v>75</v>
-      </c>
-      <c r="N2" s="49" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q2" s="49" t="s">
-        <v>63</v>
-      </c>
-      <c r="R2" s="49" t="s">
-        <v>73</v>
-      </c>
-      <c r="S2" s="49" t="s">
-        <v>74</v>
-      </c>
-      <c r="T2" s="49" t="s">
-        <v>75</v>
-      </c>
-      <c r="U2" s="49" t="s">
-        <v>76</v>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="J2" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="R2" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="S2" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="T2" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="U2" s="37" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="17.25" thickBot="1">
       <c r="A3" s="6"/>
-      <c r="B3" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="8">
+      <c r="B3" s="7"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="I3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J3" s="34">
         <v>5</v>
       </c>
-      <c r="D3" s="8">
+      <c r="K3" s="34">
         <v>5</v>
       </c>
-      <c r="E3" s="8">
+      <c r="L3" s="34">
         <v>3.5</v>
       </c>
-      <c r="F3" s="8">
+      <c r="M3" s="34">
         <v>3</v>
       </c>
-      <c r="G3" s="8">
+      <c r="N3" s="34">
         <v>3</v>
       </c>
-      <c r="I3" t="s">
-        <v>64</v>
-      </c>
-      <c r="J3" s="50">
+      <c r="P3" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q3" s="38">
         <v>5</v>
       </c>
-      <c r="K3" s="50">
+      <c r="R3" s="39">
         <v>5</v>
       </c>
-      <c r="L3" s="50">
+      <c r="S3" s="40">
         <v>3.5</v>
       </c>
-      <c r="M3" s="50">
+      <c r="T3" s="40">
         <v>3</v>
       </c>
-      <c r="N3" s="50">
+      <c r="U3" s="40">
         <v>3</v>
       </c>
-      <c r="P3" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q3" s="36">
-        <v>5</v>
-      </c>
-      <c r="R3" s="36">
-        <v>5</v>
-      </c>
-      <c r="S3" s="37">
-        <v>3.5</v>
-      </c>
-      <c r="T3" s="37">
-        <v>3</v>
-      </c>
-      <c r="U3" s="37">
-        <v>3</v>
-      </c>
     </row>
     <row r="4" spans="1:21" ht="17.25" thickBot="1">
-      <c r="A4" s="9">
+      <c r="A4" s="9"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="51"/>
+      <c r="I4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="35">
         <v>1</v>
       </c>
-      <c r="B4" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="25"/>
-      <c r="I4" t="s">
-        <v>65</v>
-      </c>
-      <c r="J4">
+      <c r="K4" s="35">
+        <v>1.5</v>
+      </c>
+      <c r="L4" s="35">
         <v>1</v>
       </c>
-      <c r="K4">
-        <v>1.5</v>
-      </c>
-      <c r="L4">
+      <c r="M4" s="35">
+        <v>2</v>
+      </c>
+      <c r="N4" s="35">
         <v>1</v>
       </c>
-      <c r="M4">
-        <v>2</v>
-      </c>
-      <c r="N4">
-        <v>1</v>
-      </c>
-      <c r="P4" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q4" s="36">
+      <c r="P4" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q4" s="41">
         <v>16</v>
       </c>
-      <c r="R4" s="36">
+      <c r="R4" s="30">
         <v>4.5</v>
       </c>
-      <c r="S4" s="37">
+      <c r="S4" s="31">
         <v>8</v>
       </c>
-      <c r="T4" s="37">
-        <v>6</v>
-      </c>
-      <c r="U4" s="37">
+      <c r="T4" s="31">
+        <v>7.5</v>
+      </c>
+      <c r="U4" s="31">
         <v>3.25</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="17.25" thickBot="1">
-      <c r="A5" s="10">
-        <v>2</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="12">
-        <v>4</v>
-      </c>
-      <c r="D5" s="12">
-        <v>4</v>
-      </c>
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
       <c r="I5" t="s">
-        <v>66</v>
-      </c>
-      <c r="J5">
+        <v>3</v>
+      </c>
+      <c r="J5" s="35">
         <v>7</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="35">
         <v>3</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="35">
         <v>2</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="35">
         <v>8.75</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="35">
         <v>5.25</v>
       </c>
-      <c r="P5" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q5" s="33">
-        <v>17.75</v>
-      </c>
-      <c r="R5" s="33">
+      <c r="P5" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="S5" s="34">
-        <v>15</v>
-      </c>
-      <c r="T5" s="34">
-        <v>15</v>
-      </c>
-      <c r="U5" s="34">
-        <v>11</v>
+      <c r="Q5" s="42">
+        <v>29.5</v>
+      </c>
+      <c r="R5" s="27">
+        <v>23</v>
+      </c>
+      <c r="S5" s="28">
+        <v>18</v>
+      </c>
+      <c r="T5" s="28">
+        <v>17</v>
+      </c>
+      <c r="U5" s="28">
+        <v>17.25</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="17.25" thickBot="1">
-      <c r="A6" s="14">
-        <v>3</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>9</v>
-      </c>
+      <c r="A6" s="14"/>
+      <c r="B6" s="15"/>
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
       <c r="E6" s="13"/>
-      <c r="F6" s="16">
-        <v>2</v>
-      </c>
+      <c r="F6" s="16"/>
       <c r="G6" s="13"/>
       <c r="I6" t="s">
-        <v>67</v>
-      </c>
-      <c r="J6">
+        <v>4</v>
+      </c>
+      <c r="J6" s="35">
         <v>1</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="35">
         <v>7</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="35">
         <v>1.5</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="35">
         <v>2.5</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="35">
         <v>3.5</v>
       </c>
-      <c r="P6" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q6" s="33"/>
-      <c r="R6" s="33"/>
-      <c r="S6" s="34"/>
-      <c r="T6" s="34"/>
-      <c r="U6" s="34">
-        <v>2.5</v>
+      <c r="P6" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q6" s="42"/>
+      <c r="R6" s="27"/>
+      <c r="S6" s="28"/>
+      <c r="T6" s="28">
+        <v>2</v>
+      </c>
+      <c r="U6" s="28">
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="17.25" thickBot="1">
-      <c r="A7" s="14">
-        <v>4</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>10</v>
-      </c>
+      <c r="A7" s="14"/>
+      <c r="B7" s="15"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
-      <c r="G7" s="16">
-        <v>2</v>
-      </c>
+      <c r="G7" s="16"/>
       <c r="I7" t="s">
-        <v>68</v>
-      </c>
-      <c r="J7">
+        <v>5</v>
+      </c>
+      <c r="J7" s="35">
         <v>11</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="35">
         <v>7</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="35">
         <v>6</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="35">
         <v>7.75</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="35">
         <v>7.25</v>
       </c>
-      <c r="P7" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q7" s="33">
+      <c r="P7" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q7" s="42">
         <v>6</v>
       </c>
-      <c r="R7" s="33">
+      <c r="R7" s="27">
         <v>6</v>
       </c>
-      <c r="S7" s="34">
+      <c r="S7" s="28">
         <v>6</v>
       </c>
-      <c r="T7" s="34">
+      <c r="T7" s="28">
         <v>6</v>
       </c>
-      <c r="U7" s="34">
+      <c r="U7" s="28">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="17.25" thickBot="1">
-      <c r="A8" s="14">
-        <v>5</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="A8" s="14"/>
+      <c r="B8" s="15"/>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
-      <c r="E8" s="16">
-        <v>2.5</v>
-      </c>
+      <c r="E8" s="16"/>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
       <c r="I8" t="s">
-        <v>69</v>
-      </c>
-      <c r="J8">
+        <v>6</v>
+      </c>
+      <c r="J8" s="35">
         <v>0</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="35">
         <v>0</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="35">
         <v>6</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="35">
         <v>0</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="35">
         <v>0</v>
       </c>
-      <c r="P8" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q8" s="33"/>
-      <c r="R8" s="33"/>
-      <c r="S8" s="34">
-        <v>1</v>
-      </c>
-      <c r="T8" s="34">
-        <v>2.5</v>
-      </c>
-      <c r="U8" s="34">
-        <v>10</v>
+      <c r="P8" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q8" s="42">
+        <v>5.75</v>
+      </c>
+      <c r="R8" s="27"/>
+      <c r="S8" s="28">
+        <v>5.5</v>
+      </c>
+      <c r="T8" s="28">
+        <v>7.5</v>
+      </c>
+      <c r="U8" s="28">
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="17.25" thickBot="1">
-      <c r="A9" s="14">
+      <c r="A9" s="14"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="I9" t="s">
+        <v>7</v>
+      </c>
+      <c r="J9" s="34">
+        <v>0</v>
+      </c>
+      <c r="K9" s="35">
+        <v>0</v>
+      </c>
+      <c r="L9" s="35">
         <v>6</v>
       </c>
-      <c r="B9" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="12">
-        <v>1</v>
-      </c>
-      <c r="D9" s="12">
-        <v>1</v>
-      </c>
-      <c r="E9" s="16">
-        <v>1</v>
-      </c>
-      <c r="F9" s="16">
-        <v>1</v>
-      </c>
-      <c r="G9" s="16">
-        <v>1</v>
-      </c>
-      <c r="I9" t="s">
-        <v>70</v>
-      </c>
-      <c r="J9" s="49">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>6</v>
-      </c>
-      <c r="M9">
+      <c r="M9" s="35">
         <v>3.5</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="35">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="17.25" thickBot="1">
       <c r="A10" s="17"/>
-      <c r="B10" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="19">
-        <v>1</v>
-      </c>
-      <c r="D10" s="19">
-        <v>1.5</v>
-      </c>
-      <c r="E10" s="8">
-        <v>1</v>
-      </c>
-      <c r="F10" s="8">
+      <c r="B10" s="18"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="I10" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10" s="34">
+        <v>12.25</v>
+      </c>
+      <c r="K10" s="34">
+        <v>0</v>
+      </c>
+      <c r="L10" s="34">
         <v>2</v>
       </c>
-      <c r="G10" s="8">
-        <v>1</v>
-      </c>
-      <c r="I10" t="s">
-        <v>71</v>
-      </c>
-      <c r="J10" s="50">
-        <v>12.25</v>
-      </c>
-      <c r="K10" s="50">
-        <v>0</v>
-      </c>
-      <c r="L10" s="50">
-        <v>2</v>
-      </c>
-      <c r="M10" s="50">
+      <c r="M10" s="34">
         <v>5</v>
       </c>
-      <c r="N10" s="50">
+      <c r="N10" s="34">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="17.25" thickBot="1">
-      <c r="A11" s="20">
-        <v>7</v>
-      </c>
-      <c r="B11" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="28"/>
+      <c r="A11" s="20"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="48"/>
       <c r="I11" t="s">
-        <v>72</v>
-      </c>
-      <c r="J11">
-        <v>9.5</v>
-      </c>
-      <c r="K11">
         <v>9</v>
       </c>
-      <c r="L11">
-        <v>5.5</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11">
-        <v>10</v>
+      <c r="J11" s="58">
+        <v>22</v>
+      </c>
+      <c r="K11" s="59">
+        <v>15</v>
+      </c>
+      <c r="L11" s="60">
+        <v>12.5</v>
+      </c>
+      <c r="M11" s="60">
+        <v>9</v>
+      </c>
+      <c r="N11" s="60">
+        <v>16.25</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="17.25" thickBot="1">
-      <c r="A12" s="14">
-        <v>8</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="12">
-        <v>1</v>
-      </c>
+      <c r="A12" s="14"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="12"/>
       <c r="D12" s="12"/>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
     </row>
     <row r="13" spans="1:21" ht="17.25" thickBot="1">
-      <c r="A13" s="14">
-        <v>9</v>
-      </c>
-      <c r="B13" s="15" t="s">
-        <v>16</v>
-      </c>
+      <c r="A13" s="14"/>
+      <c r="B13" s="15"/>
       <c r="C13" s="12"/>
-      <c r="D13" s="12">
-        <v>1.5</v>
-      </c>
+      <c r="D13" s="12"/>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
     </row>
     <row r="14" spans="1:21" ht="17.25" thickBot="1">
-      <c r="A14" s="14">
-        <v>10</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>17</v>
-      </c>
+      <c r="A14" s="14"/>
+      <c r="B14" s="15"/>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
-      <c r="E14" s="16">
-        <v>1</v>
-      </c>
+      <c r="E14" s="16"/>
       <c r="F14" s="13"/>
-      <c r="G14" s="16">
-        <v>1</v>
-      </c>
+      <c r="G14" s="16"/>
     </row>
     <row r="15" spans="1:21" ht="17.25" thickBot="1">
-      <c r="A15" s="14">
-        <v>12</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>18</v>
-      </c>
+      <c r="A15" s="14"/>
+      <c r="B15" s="15"/>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="13"/>
-      <c r="F15" s="16">
-        <v>2</v>
-      </c>
+      <c r="F15" s="16"/>
       <c r="G15" s="13"/>
     </row>
     <row r="16" spans="1:21" ht="17.25" thickBot="1">
       <c r="A16" s="17"/>
-      <c r="B16" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="19">
-        <v>7</v>
-      </c>
-      <c r="D16" s="19">
-        <v>3</v>
-      </c>
-      <c r="E16" s="8">
-        <v>2</v>
-      </c>
-      <c r="F16" s="8">
-        <v>8.75</v>
-      </c>
-      <c r="G16" s="8">
-        <v>5.25</v>
-      </c>
+      <c r="B16" s="18"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
     </row>
     <row r="17" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A17" s="20">
-        <v>7</v>
-      </c>
-      <c r="B17" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="28"/>
+      <c r="A17" s="20"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="48"/>
     </row>
     <row r="18" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A18" s="14">
-        <v>8</v>
-      </c>
-      <c r="B18" s="15" t="s">
-        <v>15</v>
-      </c>
+      <c r="A18" s="14"/>
+      <c r="B18" s="15"/>
       <c r="C18" s="12"/>
       <c r="D18" s="12"/>
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
-      <c r="G18" s="16">
-        <v>0.25</v>
-      </c>
+      <c r="G18" s="16"/>
     </row>
     <row r="19" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A19" s="14">
-        <v>9</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>16</v>
-      </c>
+      <c r="A19" s="14"/>
+      <c r="B19" s="15"/>
       <c r="C19" s="12"/>
-      <c r="D19" s="12">
-        <v>1</v>
-      </c>
+      <c r="D19" s="12"/>
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
     </row>
     <row r="20" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A20" s="14">
-        <v>11</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="12">
-        <v>1</v>
-      </c>
+      <c r="A20" s="14"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="12"/>
       <c r="D20" s="12"/>
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
     </row>
     <row r="21" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A21" s="14">
-        <v>12</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="12">
-        <v>2</v>
-      </c>
+      <c r="A21" s="14"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="12"/>
       <c r="D21" s="12"/>
       <c r="E21" s="13"/>
-      <c r="F21" s="16">
-        <v>2</v>
-      </c>
+      <c r="F21" s="16"/>
       <c r="G21" s="13"/>
     </row>
     <row r="22" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A22" s="14">
-        <v>15</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" s="12">
-        <v>2</v>
-      </c>
-      <c r="D22" s="12">
-        <v>2</v>
-      </c>
-      <c r="E22" s="16">
-        <v>2</v>
-      </c>
-      <c r="F22" s="16">
-        <v>2</v>
-      </c>
-      <c r="G22" s="16">
-        <v>2</v>
-      </c>
+      <c r="A22" s="14"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
     </row>
     <row r="23" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A23" s="20">
-        <v>16</v>
-      </c>
-      <c r="B23" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="28"/>
+      <c r="A23" s="20"/>
+      <c r="B23" s="46"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="48"/>
     </row>
     <row r="24" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A24" s="14">
-        <v>17</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>23</v>
-      </c>
+      <c r="A24" s="14"/>
+      <c r="B24" s="15"/>
       <c r="C24" s="12"/>
       <c r="D24" s="12"/>
       <c r="E24" s="13"/>
-      <c r="F24" s="16">
-        <v>4.75</v>
-      </c>
-      <c r="G24" s="16">
-        <v>3</v>
-      </c>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
     </row>
     <row r="25" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A25" s="14">
-        <v>18</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" s="12">
-        <v>2</v>
-      </c>
+      <c r="A25" s="14"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="12"/>
       <c r="D25" s="12"/>
       <c r="E25" s="13"/>
       <c r="F25" s="13"/>
@@ -2630,783 +2315,433 @@
     </row>
     <row r="26" spans="1:7" ht="17.25" thickBot="1">
       <c r="A26" s="17"/>
-      <c r="B26" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" s="19">
-        <v>1</v>
-      </c>
-      <c r="D26" s="19">
-        <v>7</v>
-      </c>
-      <c r="E26" s="8">
-        <v>1.5</v>
-      </c>
-      <c r="F26" s="8">
-        <v>2.5</v>
-      </c>
-      <c r="G26" s="8">
-        <v>3.5</v>
-      </c>
+      <c r="B26" s="18"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
     </row>
     <row r="27" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A27" s="20">
-        <v>7</v>
-      </c>
-      <c r="B27" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="28"/>
+      <c r="A27" s="20"/>
+      <c r="B27" s="46"/>
+      <c r="C27" s="47"/>
+      <c r="D27" s="47"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="48"/>
     </row>
     <row r="28" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A28" s="14">
-        <v>12</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28" s="12">
-        <v>1</v>
-      </c>
+      <c r="A28" s="14"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="12"/>
       <c r="D28" s="12"/>
       <c r="E28" s="13"/>
       <c r="F28" s="13"/>
       <c r="G28" s="13"/>
     </row>
     <row r="29" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A29" s="14">
-        <v>13</v>
-      </c>
-      <c r="B29" s="21" t="s">
-        <v>27</v>
-      </c>
+      <c r="A29" s="14"/>
+      <c r="B29" s="21"/>
       <c r="C29" s="12"/>
       <c r="D29" s="12"/>
-      <c r="E29" s="16">
-        <v>1.5</v>
-      </c>
+      <c r="E29" s="16"/>
       <c r="F29" s="13"/>
       <c r="G29" s="13"/>
     </row>
     <row r="30" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A30" s="20">
-        <v>16</v>
-      </c>
-      <c r="B30" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="28"/>
+      <c r="A30" s="20"/>
+      <c r="B30" s="46"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="48"/>
     </row>
     <row r="31" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A31" s="14">
-        <v>17</v>
-      </c>
-      <c r="B31" s="15" t="s">
-        <v>23</v>
-      </c>
+      <c r="A31" s="14"/>
+      <c r="B31" s="15"/>
       <c r="C31" s="12"/>
       <c r="D31" s="12"/>
       <c r="E31" s="13"/>
-      <c r="F31" s="16">
-        <v>2.5</v>
-      </c>
-      <c r="G31" s="16">
-        <v>3.5</v>
-      </c>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
     </row>
     <row r="32" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A32" s="14">
-        <v>18</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>24</v>
-      </c>
+      <c r="A32" s="14"/>
+      <c r="B32" s="15"/>
       <c r="C32" s="12"/>
-      <c r="D32" s="12">
-        <v>7</v>
-      </c>
+      <c r="D32" s="12"/>
       <c r="E32" s="13"/>
       <c r="F32" s="13"/>
       <c r="G32" s="13"/>
     </row>
     <row r="33" spans="1:7" ht="17.25" thickBot="1">
       <c r="A33" s="17"/>
-      <c r="B33" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C33" s="19">
-        <v>14</v>
-      </c>
-      <c r="D33" s="19">
-        <v>16.5</v>
-      </c>
-      <c r="E33" s="8">
-        <v>8</v>
-      </c>
-      <c r="F33" s="8">
-        <v>16.25</v>
-      </c>
-      <c r="G33" s="8">
-        <v>12.75</v>
-      </c>
+      <c r="B33" s="22"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
     </row>
     <row r="34" spans="1:7" ht="17.25" thickBot="1">
       <c r="A34" s="2"/>
     </row>
     <row r="35" spans="1:7" ht="17.25" thickBot="1">
       <c r="A35" s="3"/>
-      <c r="B35" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>5</v>
-      </c>
+      <c r="B35" s="4"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
     </row>
     <row r="36" spans="1:7" ht="17.25" thickBot="1">
       <c r="A36" s="6"/>
-      <c r="B36" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C36" s="8">
-        <v>11</v>
-      </c>
-      <c r="D36" s="8">
-        <v>7</v>
-      </c>
-      <c r="E36" s="8">
-        <v>6</v>
-      </c>
-      <c r="F36" s="8">
-        <v>7.75</v>
-      </c>
-      <c r="G36" s="8">
-        <v>7.25</v>
-      </c>
+      <c r="B36" s="7"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+      <c r="F36" s="8"/>
+      <c r="G36" s="8"/>
     </row>
     <row r="37" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A37" s="29">
-        <v>7</v>
-      </c>
-      <c r="B37" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="C37" s="41"/>
-      <c r="D37" s="41"/>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
-      <c r="G37" s="42"/>
+      <c r="A37" s="23"/>
+      <c r="B37" s="52"/>
+      <c r="C37" s="53"/>
+      <c r="D37" s="53"/>
+      <c r="E37" s="53"/>
+      <c r="F37" s="53"/>
+      <c r="G37" s="54"/>
     </row>
     <row r="38" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A38" s="14">
-        <v>12</v>
-      </c>
-      <c r="B38" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C38" s="12">
-        <v>2.5</v>
-      </c>
+      <c r="A38" s="14"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="12"/>
       <c r="D38" s="12"/>
       <c r="E38" s="13"/>
       <c r="F38" s="13"/>
       <c r="G38" s="13"/>
     </row>
     <row r="39" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A39" s="20">
-        <v>16</v>
-      </c>
-      <c r="B39" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="C39" s="27"/>
-      <c r="D39" s="27"/>
-      <c r="E39" s="27"/>
-      <c r="F39" s="27"/>
-      <c r="G39" s="28"/>
+      <c r="A39" s="20"/>
+      <c r="B39" s="46"/>
+      <c r="C39" s="47"/>
+      <c r="D39" s="47"/>
+      <c r="E39" s="47"/>
+      <c r="F39" s="47"/>
+      <c r="G39" s="48"/>
     </row>
     <row r="40" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A40" s="14">
-        <v>17</v>
-      </c>
-      <c r="B40" s="15" t="s">
-        <v>23</v>
-      </c>
+      <c r="A40" s="14"/>
+      <c r="B40" s="15"/>
       <c r="C40" s="12"/>
       <c r="D40" s="12"/>
       <c r="E40" s="16"/>
-      <c r="F40" s="16">
-        <v>1.75</v>
-      </c>
-      <c r="G40" s="16">
-        <v>0.5</v>
-      </c>
+      <c r="F40" s="16"/>
+      <c r="G40" s="16"/>
     </row>
     <row r="41" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A41" s="14">
-        <v>18</v>
-      </c>
-      <c r="B41" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C41" s="12">
-        <v>2.5</v>
-      </c>
-      <c r="D41" s="12">
-        <v>1</v>
-      </c>
+      <c r="A41" s="14"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
       <c r="E41" s="16"/>
       <c r="F41" s="16"/>
       <c r="G41" s="16"/>
     </row>
     <row r="42" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A42" s="20">
-        <v>24</v>
-      </c>
-      <c r="B42" s="43" t="s">
-        <v>32</v>
-      </c>
-      <c r="C42" s="44"/>
-      <c r="D42" s="44"/>
-      <c r="E42" s="44"/>
-      <c r="F42" s="44"/>
-      <c r="G42" s="45"/>
+      <c r="A42" s="20"/>
+      <c r="B42" s="55"/>
+      <c r="C42" s="56"/>
+      <c r="D42" s="56"/>
+      <c r="E42" s="56"/>
+      <c r="F42" s="56"/>
+      <c r="G42" s="57"/>
     </row>
     <row r="43" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A43" s="14">
-        <v>25</v>
-      </c>
-      <c r="B43" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C43" s="12">
-        <v>4</v>
-      </c>
-      <c r="D43" s="12">
-        <v>4</v>
-      </c>
-      <c r="E43" s="16">
-        <v>4</v>
-      </c>
-      <c r="F43" s="16">
-        <v>4</v>
-      </c>
-      <c r="G43" s="16">
-        <v>4</v>
-      </c>
+      <c r="A43" s="14"/>
+      <c r="B43" s="15"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="16"/>
     </row>
     <row r="44" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A44" s="14">
-        <v>26</v>
-      </c>
-      <c r="B44" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="C44" s="12">
-        <v>1</v>
-      </c>
-      <c r="D44" s="12">
-        <v>1</v>
-      </c>
-      <c r="E44" s="16">
-        <v>1</v>
-      </c>
-      <c r="F44" s="16">
-        <v>1</v>
-      </c>
-      <c r="G44" s="16">
-        <v>2</v>
-      </c>
+      <c r="A44" s="14"/>
+      <c r="B44" s="15"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="16"/>
+      <c r="G44" s="16"/>
     </row>
     <row r="45" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A45" s="14">
-        <v>27</v>
-      </c>
-      <c r="B45" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="C45" s="12">
-        <v>1</v>
-      </c>
-      <c r="D45" s="12">
-        <v>1</v>
-      </c>
-      <c r="E45" s="16">
-        <v>1</v>
-      </c>
-      <c r="F45" s="16">
-        <v>1</v>
-      </c>
-      <c r="G45" s="16">
-        <v>1</v>
-      </c>
+      <c r="A45" s="14"/>
+      <c r="B45" s="15"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="16"/>
     </row>
     <row r="46" spans="1:7" ht="17.25" thickBot="1">
       <c r="A46" s="17"/>
-      <c r="B46" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="C46" s="19">
-        <v>0</v>
-      </c>
-      <c r="D46" s="19">
-        <v>0</v>
-      </c>
-      <c r="E46" s="8">
-        <v>6</v>
-      </c>
-      <c r="F46" s="8">
-        <v>0</v>
-      </c>
-      <c r="G46" s="8">
-        <v>0</v>
-      </c>
+      <c r="B46" s="18"/>
+      <c r="C46" s="19"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
     </row>
     <row r="47" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A47" s="20">
-        <v>16</v>
-      </c>
-      <c r="B47" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="C47" s="27"/>
-      <c r="D47" s="27"/>
-      <c r="E47" s="27"/>
-      <c r="F47" s="27"/>
-      <c r="G47" s="28"/>
+      <c r="A47" s="20"/>
+      <c r="B47" s="46"/>
+      <c r="C47" s="47"/>
+      <c r="D47" s="47"/>
+      <c r="E47" s="47"/>
+      <c r="F47" s="47"/>
+      <c r="G47" s="48"/>
     </row>
     <row r="48" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A48" s="14">
-        <v>18</v>
-      </c>
-      <c r="B48" s="15" t="s">
-        <v>24</v>
-      </c>
+      <c r="A48" s="14"/>
+      <c r="B48" s="15"/>
       <c r="C48" s="12"/>
       <c r="D48" s="12"/>
-      <c r="E48" s="16">
-        <v>2</v>
-      </c>
+      <c r="E48" s="16"/>
       <c r="F48" s="16"/>
       <c r="G48" s="16"/>
     </row>
     <row r="49" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A49" s="14">
-        <v>19</v>
-      </c>
-      <c r="B49" s="15" t="s">
-        <v>38</v>
-      </c>
+      <c r="A49" s="14"/>
+      <c r="B49" s="15"/>
       <c r="C49" s="12"/>
       <c r="D49" s="12"/>
-      <c r="E49" s="16">
-        <v>4</v>
-      </c>
+      <c r="E49" s="16"/>
       <c r="F49" s="16"/>
       <c r="G49" s="16"/>
     </row>
     <row r="50" spans="1:7" ht="17.25" thickBot="1">
       <c r="A50" s="17"/>
-      <c r="B50" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="C50" s="19">
-        <v>0</v>
-      </c>
-      <c r="D50" s="19">
-        <v>0</v>
-      </c>
-      <c r="E50" s="8">
-        <v>6</v>
-      </c>
-      <c r="F50" s="8">
-        <v>3.5</v>
-      </c>
-      <c r="G50" s="8">
-        <v>0</v>
-      </c>
+      <c r="B50" s="18"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="8"/>
     </row>
     <row r="51" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A51" s="20">
-        <v>16</v>
-      </c>
-      <c r="B51" s="26" t="s">
-        <v>40</v>
-      </c>
-      <c r="C51" s="27"/>
-      <c r="D51" s="27"/>
-      <c r="E51" s="27"/>
-      <c r="F51" s="27"/>
-      <c r="G51" s="28"/>
+      <c r="A51" s="20"/>
+      <c r="B51" s="46"/>
+      <c r="C51" s="47"/>
+      <c r="D51" s="47"/>
+      <c r="E51" s="47"/>
+      <c r="F51" s="47"/>
+      <c r="G51" s="48"/>
     </row>
     <row r="52" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A52" s="14">
-        <v>17</v>
-      </c>
-      <c r="B52" s="15" t="s">
-        <v>23</v>
-      </c>
+      <c r="A52" s="14"/>
+      <c r="B52" s="15"/>
       <c r="C52" s="12"/>
       <c r="D52" s="12"/>
       <c r="E52" s="16"/>
-      <c r="F52" s="16">
-        <v>3.5</v>
-      </c>
+      <c r="F52" s="16"/>
       <c r="G52" s="16"/>
     </row>
     <row r="53" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A53" s="14">
-        <v>19</v>
-      </c>
-      <c r="B53" s="15" t="s">
-        <v>38</v>
-      </c>
+      <c r="A53" s="14"/>
+      <c r="B53" s="15"/>
       <c r="C53" s="12"/>
       <c r="D53" s="12"/>
-      <c r="E53" s="16">
-        <v>6</v>
-      </c>
+      <c r="E53" s="16"/>
       <c r="F53" s="16"/>
       <c r="G53" s="16"/>
     </row>
     <row r="54" spans="1:7" ht="17.25" thickBot="1">
       <c r="A54" s="17"/>
-      <c r="B54" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C54" s="19">
-        <v>12.25</v>
-      </c>
-      <c r="D54" s="19">
-        <v>0</v>
-      </c>
-      <c r="E54" s="8">
-        <v>2</v>
-      </c>
-      <c r="F54" s="8">
-        <v>5</v>
-      </c>
-      <c r="G54" s="8">
-        <v>8</v>
-      </c>
+      <c r="B54" s="18"/>
+      <c r="C54" s="19"/>
+      <c r="D54" s="19"/>
+      <c r="E54" s="8"/>
+      <c r="F54" s="8"/>
+      <c r="G54" s="8"/>
     </row>
     <row r="55" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A55" s="20">
-        <v>7</v>
-      </c>
-      <c r="B55" s="26" t="s">
-        <v>42</v>
-      </c>
-      <c r="C55" s="27"/>
-      <c r="D55" s="27"/>
-      <c r="E55" s="27"/>
-      <c r="F55" s="27"/>
-      <c r="G55" s="28"/>
+      <c r="A55" s="20"/>
+      <c r="B55" s="46"/>
+      <c r="C55" s="47"/>
+      <c r="D55" s="47"/>
+      <c r="E55" s="47"/>
+      <c r="F55" s="47"/>
+      <c r="G55" s="48"/>
     </row>
     <row r="56" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A56" s="14">
-        <v>9</v>
-      </c>
-      <c r="B56" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C56" s="12">
-        <v>1.5</v>
-      </c>
+      <c r="A56" s="14"/>
+      <c r="B56" s="15"/>
+      <c r="C56" s="12"/>
       <c r="D56" s="12"/>
       <c r="E56" s="16"/>
       <c r="F56" s="16"/>
       <c r="G56" s="16"/>
     </row>
     <row r="57" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A57" s="30">
-        <v>41223</v>
-      </c>
-      <c r="B57" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C57" s="12">
-        <v>0.5</v>
-      </c>
+      <c r="A57" s="24"/>
+      <c r="B57" s="15"/>
+      <c r="C57" s="12"/>
       <c r="D57" s="12"/>
       <c r="E57" s="16"/>
       <c r="F57" s="16"/>
       <c r="G57" s="16"/>
     </row>
     <row r="58" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A58" s="14">
-        <v>13</v>
-      </c>
-      <c r="B58" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C58" s="12">
-        <v>1</v>
-      </c>
+      <c r="A58" s="14"/>
+      <c r="B58" s="15"/>
+      <c r="C58" s="12"/>
       <c r="D58" s="12"/>
-      <c r="E58" s="16">
-        <v>2</v>
-      </c>
+      <c r="E58" s="16"/>
       <c r="F58" s="16"/>
       <c r="G58" s="16"/>
     </row>
     <row r="59" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A59" s="20">
-        <v>16</v>
-      </c>
-      <c r="B59" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="C59" s="27"/>
-      <c r="D59" s="27"/>
-      <c r="E59" s="27"/>
-      <c r="F59" s="27"/>
-      <c r="G59" s="28"/>
+      <c r="A59" s="20"/>
+      <c r="B59" s="46"/>
+      <c r="C59" s="47"/>
+      <c r="D59" s="47"/>
+      <c r="E59" s="47"/>
+      <c r="F59" s="47"/>
+      <c r="G59" s="48"/>
     </row>
     <row r="60" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A60" s="14">
-        <v>17</v>
-      </c>
-      <c r="B60" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C60" s="12">
-        <v>0.5</v>
-      </c>
+      <c r="A60" s="14"/>
+      <c r="B60" s="15"/>
+      <c r="C60" s="12"/>
       <c r="D60" s="12"/>
       <c r="E60" s="16"/>
-      <c r="F60" s="16">
-        <v>2.5</v>
-      </c>
-      <c r="G60" s="16">
-        <v>4</v>
-      </c>
+      <c r="F60" s="16"/>
+      <c r="G60" s="16"/>
     </row>
     <row r="61" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A61" s="14">
-        <v>18</v>
-      </c>
-      <c r="B61" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C61" s="12">
-        <v>2</v>
-      </c>
+      <c r="A61" s="14"/>
+      <c r="B61" s="15"/>
+      <c r="C61" s="12"/>
       <c r="D61" s="12"/>
       <c r="E61" s="16"/>
       <c r="F61" s="16"/>
       <c r="G61" s="16"/>
     </row>
     <row r="62" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A62" s="14">
-        <v>19</v>
-      </c>
-      <c r="B62" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C62" s="12">
-        <v>2.5</v>
-      </c>
+      <c r="A62" s="14"/>
+      <c r="B62" s="15"/>
+      <c r="C62" s="12"/>
       <c r="D62" s="12"/>
       <c r="E62" s="16"/>
       <c r="F62" s="16"/>
       <c r="G62" s="16"/>
     </row>
     <row r="63" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A63" s="14">
-        <v>20</v>
-      </c>
-      <c r="B63" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="C63" s="12">
-        <v>4.25</v>
-      </c>
+      <c r="A63" s="14"/>
+      <c r="B63" s="15"/>
+      <c r="C63" s="12"/>
       <c r="D63" s="12"/>
       <c r="E63" s="16"/>
       <c r="F63" s="16"/>
       <c r="G63" s="16"/>
     </row>
     <row r="64" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A64" s="20">
-        <v>21</v>
-      </c>
-      <c r="B64" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="C64" s="27"/>
-      <c r="D64" s="27"/>
-      <c r="E64" s="27"/>
-      <c r="F64" s="27"/>
-      <c r="G64" s="28"/>
+      <c r="A64" s="20"/>
+      <c r="B64" s="46"/>
+      <c r="C64" s="47"/>
+      <c r="D64" s="47"/>
+      <c r="E64" s="47"/>
+      <c r="F64" s="47"/>
+      <c r="G64" s="48"/>
     </row>
     <row r="65" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A65" s="14">
-        <v>22</v>
-      </c>
-      <c r="B65" s="15" t="s">
-        <v>47</v>
-      </c>
+      <c r="A65" s="14"/>
+      <c r="B65" s="15"/>
       <c r="C65" s="12"/>
       <c r="D65" s="12"/>
       <c r="E65" s="16"/>
       <c r="F65" s="16"/>
-      <c r="G65" s="16">
-        <v>2.5</v>
-      </c>
+      <c r="G65" s="16"/>
     </row>
     <row r="66" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A66" s="20">
-        <v>32</v>
-      </c>
-      <c r="B66" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="C66" s="27"/>
-      <c r="D66" s="27"/>
-      <c r="E66" s="27"/>
-      <c r="F66" s="27"/>
-      <c r="G66" s="28"/>
+      <c r="A66" s="20"/>
+      <c r="B66" s="46"/>
+      <c r="C66" s="47"/>
+      <c r="D66" s="47"/>
+      <c r="E66" s="47"/>
+      <c r="F66" s="47"/>
+      <c r="G66" s="48"/>
     </row>
     <row r="67" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A67" s="14">
-        <v>32</v>
-      </c>
-      <c r="B67" s="15" t="s">
-        <v>49</v>
-      </c>
+      <c r="A67" s="14"/>
+      <c r="B67" s="15"/>
       <c r="C67" s="12"/>
       <c r="D67" s="12"/>
       <c r="E67" s="16"/>
-      <c r="F67" s="16">
-        <v>2.5</v>
-      </c>
-      <c r="G67" s="16">
-        <v>4</v>
-      </c>
+      <c r="F67" s="16"/>
+      <c r="G67" s="16"/>
     </row>
     <row r="68" spans="1:7" ht="17.25" thickBot="1">
       <c r="A68" s="17"/>
-      <c r="B68" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="C68" s="19">
-        <v>9.5</v>
-      </c>
-      <c r="D68" s="19">
-        <v>9</v>
-      </c>
-      <c r="E68" s="8">
-        <v>5.5</v>
-      </c>
-      <c r="F68" s="8">
-        <v>0</v>
-      </c>
-      <c r="G68" s="8">
-        <v>3</v>
-      </c>
+      <c r="B68" s="18"/>
+      <c r="C68" s="19"/>
+      <c r="D68" s="19"/>
+      <c r="E68" s="8"/>
+      <c r="F68" s="8"/>
+      <c r="G68" s="8"/>
     </row>
     <row r="69" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A69" s="20">
-        <v>7</v>
-      </c>
-      <c r="B69" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="C69" s="27"/>
-      <c r="D69" s="27"/>
-      <c r="E69" s="27"/>
-      <c r="F69" s="27"/>
-      <c r="G69" s="28"/>
+      <c r="A69" s="20"/>
+      <c r="B69" s="46"/>
+      <c r="C69" s="47"/>
+      <c r="D69" s="47"/>
+      <c r="E69" s="47"/>
+      <c r="F69" s="47"/>
+      <c r="G69" s="48"/>
     </row>
     <row r="70" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A70" s="14">
-        <v>9</v>
-      </c>
-      <c r="B70" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C70" s="12">
-        <v>1.5</v>
-      </c>
+      <c r="A70" s="14"/>
+      <c r="B70" s="15"/>
+      <c r="C70" s="12"/>
       <c r="D70" s="12"/>
       <c r="E70" s="16"/>
       <c r="F70" s="16"/>
       <c r="G70" s="16"/>
     </row>
     <row r="71" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A71" s="14">
-        <v>10</v>
-      </c>
-      <c r="B71" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="C71" s="12">
-        <v>1</v>
-      </c>
+      <c r="A71" s="14"/>
+      <c r="B71" s="15"/>
+      <c r="C71" s="12"/>
       <c r="D71" s="12"/>
       <c r="E71" s="16"/>
       <c r="F71" s="16"/>
       <c r="G71" s="16"/>
     </row>
     <row r="72" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A72" s="14">
-        <v>11</v>
-      </c>
-      <c r="B72" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="C72" s="12">
-        <v>2</v>
-      </c>
+      <c r="A72" s="14"/>
+      <c r="B72" s="15"/>
+      <c r="C72" s="12"/>
       <c r="D72" s="12"/>
       <c r="E72" s="16"/>
       <c r="F72" s="16"/>
       <c r="G72" s="16"/>
     </row>
     <row r="73" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A73" s="14">
-        <v>12</v>
-      </c>
-      <c r="B73" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C73" s="12">
-        <v>1</v>
-      </c>
+      <c r="A73" s="14"/>
+      <c r="B73" s="15"/>
+      <c r="C73" s="12"/>
       <c r="D73" s="12"/>
-      <c r="E73" s="16">
-        <v>1.5</v>
-      </c>
+      <c r="E73" s="16"/>
       <c r="F73" s="16"/>
       <c r="G73" s="16"/>
     </row>
     <row r="74" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A74" s="14">
-        <v>13</v>
-      </c>
-      <c r="B74" s="15" t="s">
-        <v>12</v>
-      </c>
+      <c r="A74" s="14"/>
+      <c r="B74" s="15"/>
       <c r="C74" s="12"/>
       <c r="D74" s="12"/>
       <c r="E74" s="16"/>
@@ -3414,277 +2749,157 @@
       <c r="G74" s="16"/>
     </row>
     <row r="75" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A75" s="20">
-        <v>16</v>
-      </c>
-      <c r="B75" s="26" t="s">
-        <v>53</v>
-      </c>
-      <c r="C75" s="27"/>
-      <c r="D75" s="27"/>
-      <c r="E75" s="27"/>
-      <c r="F75" s="27"/>
-      <c r="G75" s="28"/>
+      <c r="A75" s="20"/>
+      <c r="B75" s="46"/>
+      <c r="C75" s="47"/>
+      <c r="D75" s="47"/>
+      <c r="E75" s="47"/>
+      <c r="F75" s="47"/>
+      <c r="G75" s="48"/>
     </row>
     <row r="76" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A76" s="14">
-        <v>18</v>
-      </c>
-      <c r="B76" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C76" s="12">
-        <v>2</v>
-      </c>
-      <c r="D76" s="12">
-        <v>9</v>
-      </c>
+      <c r="A76" s="14"/>
+      <c r="B76" s="15"/>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
       <c r="E76" s="16"/>
       <c r="F76" s="16"/>
       <c r="G76" s="16"/>
     </row>
     <row r="77" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A77" s="14">
-        <v>19</v>
-      </c>
-      <c r="B77" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C77" s="12">
-        <v>2</v>
-      </c>
+      <c r="A77" s="14"/>
+      <c r="B77" s="15"/>
+      <c r="C77" s="12"/>
       <c r="D77" s="12"/>
-      <c r="E77" s="16">
-        <v>3</v>
-      </c>
+      <c r="E77" s="16"/>
       <c r="F77" s="16"/>
       <c r="G77" s="16"/>
     </row>
     <row r="78" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A78" s="20">
-        <v>32</v>
-      </c>
-      <c r="B78" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="C78" s="27"/>
-      <c r="D78" s="27"/>
-      <c r="E78" s="27"/>
-      <c r="F78" s="27"/>
-      <c r="G78" s="28"/>
+      <c r="A78" s="20"/>
+      <c r="B78" s="46"/>
+      <c r="C78" s="47"/>
+      <c r="D78" s="47"/>
+      <c r="E78" s="47"/>
+      <c r="F78" s="47"/>
+      <c r="G78" s="48"/>
     </row>
     <row r="79" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A79" s="14">
-        <v>32</v>
-      </c>
-      <c r="B79" s="15" t="s">
-        <v>49</v>
-      </c>
+      <c r="A79" s="14"/>
+      <c r="B79" s="15"/>
       <c r="C79" s="12"/>
       <c r="D79" s="12"/>
-      <c r="E79" s="16">
-        <v>1</v>
-      </c>
+      <c r="E79" s="16"/>
       <c r="F79" s="16"/>
-      <c r="G79" s="16">
-        <v>6.5</v>
-      </c>
+      <c r="G79" s="16"/>
     </row>
     <row r="80" spans="1:7" ht="17.25" thickBot="1">
       <c r="A80" s="17"/>
-      <c r="B80" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C80" s="19">
-        <v>46.75</v>
-      </c>
-      <c r="D80" s="19">
-        <v>31.5</v>
-      </c>
-      <c r="E80" s="8">
-        <v>27</v>
-      </c>
-      <c r="F80" s="8">
-        <v>32.5</v>
-      </c>
-      <c r="G80" s="8">
-        <v>37</v>
-      </c>
+      <c r="B80" s="22"/>
+      <c r="C80" s="19"/>
+      <c r="D80" s="19"/>
+      <c r="E80" s="8"/>
+      <c r="F80" s="8"/>
+      <c r="G80" s="8"/>
     </row>
     <row r="81" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A81" s="31"/>
-      <c r="B81" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="C81" s="33">
-        <v>14</v>
-      </c>
-      <c r="D81" s="33">
-        <v>14</v>
-      </c>
-      <c r="E81" s="34">
-        <v>14</v>
-      </c>
-      <c r="F81" s="34">
-        <v>14</v>
-      </c>
-      <c r="G81" s="34">
-        <v>14</v>
-      </c>
+      <c r="A81" s="25"/>
+      <c r="B81" s="26"/>
+      <c r="C81" s="27"/>
+      <c r="D81" s="27"/>
+      <c r="E81" s="28"/>
+      <c r="F81" s="28"/>
+      <c r="G81" s="28"/>
     </row>
     <row r="82" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A82" s="31"/>
-      <c r="B82" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="C82" s="33"/>
-      <c r="D82" s="33"/>
-      <c r="E82" s="34"/>
-      <c r="F82" s="34"/>
-      <c r="G82" s="34"/>
+      <c r="A82" s="25"/>
+      <c r="B82" s="29"/>
+      <c r="C82" s="27"/>
+      <c r="D82" s="27"/>
+      <c r="E82" s="28"/>
+      <c r="F82" s="28"/>
+      <c r="G82" s="28"/>
     </row>
     <row r="83" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A83" s="31"/>
-      <c r="B83" s="46" t="s">
-        <v>56</v>
-      </c>
-      <c r="C83" s="47"/>
-      <c r="D83" s="47"/>
-      <c r="E83" s="47"/>
-      <c r="F83" s="47"/>
-      <c r="G83" s="48"/>
+      <c r="A83" s="25"/>
+      <c r="B83" s="43"/>
+      <c r="C83" s="44"/>
+      <c r="D83" s="44"/>
+      <c r="E83" s="44"/>
+      <c r="F83" s="44"/>
+      <c r="G83" s="45"/>
     </row>
     <row r="84" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A84" s="9">
-        <v>1</v>
-      </c>
-      <c r="B84" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="C84" s="36">
-        <v>5</v>
-      </c>
-      <c r="D84" s="36">
-        <v>5</v>
-      </c>
-      <c r="E84" s="37">
-        <v>3.5</v>
-      </c>
-      <c r="F84" s="37">
-        <v>3</v>
-      </c>
-      <c r="G84" s="37">
-        <v>3</v>
-      </c>
+      <c r="A84" s="9"/>
+      <c r="B84" s="29"/>
+      <c r="C84" s="30"/>
+      <c r="D84" s="30"/>
+      <c r="E84" s="31"/>
+      <c r="F84" s="31"/>
+      <c r="G84" s="31"/>
     </row>
     <row r="85" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A85" s="29">
-        <v>7</v>
-      </c>
-      <c r="B85" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="C85" s="36">
-        <v>16</v>
-      </c>
-      <c r="D85" s="36">
-        <v>4.5</v>
-      </c>
-      <c r="E85" s="37">
-        <v>8</v>
-      </c>
-      <c r="F85" s="37">
-        <v>6</v>
-      </c>
-      <c r="G85" s="37">
-        <v>3.25</v>
-      </c>
+      <c r="A85" s="23"/>
+      <c r="B85" s="32"/>
+      <c r="C85" s="30"/>
+      <c r="D85" s="30"/>
+      <c r="E85" s="31"/>
+      <c r="F85" s="31"/>
+      <c r="G85" s="31"/>
     </row>
     <row r="86" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A86" s="29">
-        <v>16</v>
-      </c>
-      <c r="B86" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="C86" s="33">
-        <v>17.75</v>
-      </c>
-      <c r="D86" s="33">
-        <v>17</v>
-      </c>
-      <c r="E86" s="34">
-        <v>15</v>
-      </c>
-      <c r="F86" s="34">
-        <v>15</v>
-      </c>
-      <c r="G86" s="34">
-        <v>11</v>
-      </c>
+      <c r="A86" s="23"/>
+      <c r="B86" s="32"/>
+      <c r="C86" s="27"/>
+      <c r="D86" s="27"/>
+      <c r="E86" s="28"/>
+      <c r="F86" s="28"/>
+      <c r="G86" s="28"/>
     </row>
     <row r="87" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A87" s="29">
-        <v>21</v>
-      </c>
-      <c r="B87" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="C87" s="33"/>
-      <c r="D87" s="33"/>
-      <c r="E87" s="34"/>
-      <c r="F87" s="34"/>
-      <c r="G87" s="34">
-        <v>2.5</v>
-      </c>
+      <c r="A87" s="23"/>
+      <c r="B87" s="32"/>
+      <c r="C87" s="27"/>
+      <c r="D87" s="27"/>
+      <c r="E87" s="28"/>
+      <c r="F87" s="28"/>
+      <c r="G87" s="28"/>
     </row>
     <row r="88" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A88" s="29">
-        <v>24</v>
-      </c>
-      <c r="B88" s="39" t="s">
-        <v>61</v>
-      </c>
-      <c r="C88" s="33">
-        <v>6</v>
-      </c>
-      <c r="D88" s="33">
-        <v>6</v>
-      </c>
-      <c r="E88" s="34">
-        <v>6</v>
-      </c>
-      <c r="F88" s="34">
-        <v>6</v>
-      </c>
-      <c r="G88" s="34">
-        <v>6</v>
-      </c>
+      <c r="A88" s="23"/>
+      <c r="B88" s="33"/>
+      <c r="C88" s="27"/>
+      <c r="D88" s="27"/>
+      <c r="E88" s="28"/>
+      <c r="F88" s="28"/>
+      <c r="G88" s="28"/>
     </row>
     <row r="89" spans="1:7" ht="17.25" thickBot="1">
-      <c r="A89" s="29">
-        <v>32</v>
-      </c>
-      <c r="B89" s="38" t="s">
-        <v>62</v>
-      </c>
-      <c r="C89" s="33"/>
-      <c r="D89" s="33"/>
-      <c r="E89" s="34">
-        <v>1</v>
-      </c>
-      <c r="F89" s="34">
-        <v>2.5</v>
-      </c>
-      <c r="G89" s="34">
-        <v>10</v>
-      </c>
+      <c r="A89" s="23"/>
+      <c r="B89" s="32"/>
+      <c r="C89" s="27"/>
+      <c r="D89" s="27"/>
+      <c r="E89" s="28"/>
+      <c r="F89" s="28"/>
+      <c r="G89" s="28"/>
     </row>
     <row r="90" spans="1:7">
       <c r="A90" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B55:G55"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B11:G11"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B27:G27"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="B37:G37"/>
+    <mergeCell ref="B39:G39"/>
+    <mergeCell ref="B42:G42"/>
+    <mergeCell ref="B47:G47"/>
+    <mergeCell ref="B51:G51"/>
     <mergeCell ref="B83:G83"/>
     <mergeCell ref="B59:G59"/>
     <mergeCell ref="B64:G64"/>
@@ -3692,18 +2907,6 @@
     <mergeCell ref="B69:G69"/>
     <mergeCell ref="B75:G75"/>
     <mergeCell ref="B78:G78"/>
-    <mergeCell ref="B37:G37"/>
-    <mergeCell ref="B39:G39"/>
-    <mergeCell ref="B42:G42"/>
-    <mergeCell ref="B47:G47"/>
-    <mergeCell ref="B51:G51"/>
-    <mergeCell ref="B55:G55"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B11:G11"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B27:G27"/>
-    <mergeCell ref="B30:G30"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
* Updated Graphs.xlsx and Time spent per member per week and activity.docx * Modified Time Management Account.docx : Added description of the first graph
</commit_message>
<xml_diff>
--- a/doc/End of Project Report/Graphs.xlsx
+++ b/doc/End of Project Report/Graphs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>Edward</t>
     <phoneticPr fontId="10" type="noConversion"/>
@@ -95,6 +95,10 @@
   </si>
   <si>
     <t>Final Report</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Week 10</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
 </sst>
@@ -305,7 +309,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -408,12 +412,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -480,14 +478,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -548,9 +543,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$I$3:$I$11</c:f>
+              <c:f>Sheet1!$I$3:$I$12</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Week 1</c:v>
                 </c:pt>
@@ -577,16 +572,19 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Week 9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Week 10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$3:$J$11</c:f>
+              <c:f>Sheet1!$J$3:$J$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -613,6 +611,9 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -637,9 +638,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$I$3:$I$11</c:f>
+              <c:f>Sheet1!$I$3:$I$12</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Week 1</c:v>
                 </c:pt>
@@ -666,16 +667,19 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Week 9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Week 10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$3:$K$11</c:f>
+              <c:f>Sheet1!$K$3:$K$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -726,9 +730,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$I$3:$I$11</c:f>
+              <c:f>Sheet1!$I$3:$I$12</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Week 1</c:v>
                 </c:pt>
@@ -755,16 +759,19 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Week 9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Week 10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$3:$L$11</c:f>
+              <c:f>Sheet1!$L$3:$L$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>3.5</c:v>
                 </c:pt>
@@ -791,6 +798,9 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -815,9 +825,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$I$3:$I$11</c:f>
+              <c:f>Sheet1!$I$3:$I$12</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Week 1</c:v>
                 </c:pt>
@@ -844,16 +854,19 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Week 9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Week 10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$M$3:$M$11</c:f>
+              <c:f>Sheet1!$M$3:$M$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -915,9 +928,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$I$3:$I$11</c:f>
+              <c:f>Sheet1!$I$3:$I$12</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Week 1</c:v>
                 </c:pt>
@@ -944,16 +957,19 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>Week 9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Week 10</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$3:$N$11</c:f>
+              <c:f>Sheet1!$N$3:$N$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -980,6 +996,9 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>16.25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1117,7 +1136,7 @@
                   <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29.5</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>6</c:v>
@@ -1383,10 +1402,10 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11</c:v>
+                  <c:v>13.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1443,15 +1462,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>9524</xdr:rowOff>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>619125</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>171449</xdr:rowOff>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>219074</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1790,8 +1809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="Y10" sqref="Y10"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1812,35 +1831,36 @@
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
-      <c r="J2" s="34" t="s">
+      <c r="I2" s="34"/>
+      <c r="J2" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="34" t="s">
+      <c r="K2" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="34" t="s">
+      <c r="L2" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="34" t="s">
+      <c r="M2" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="34" t="s">
+      <c r="N2" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="37" t="s">
+      <c r="P2" s="34"/>
+      <c r="Q2" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="R2" s="37" t="s">
+      <c r="R2" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="S2" s="37" t="s">
+      <c r="S2" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="T2" s="37" t="s">
+      <c r="T2" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="U2" s="37" t="s">
+      <c r="U2" s="35" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1852,73 +1872,73 @@
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
-      <c r="I3" t="s">
+      <c r="I3" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="34">
+      <c r="J3" s="35">
         <v>5</v>
       </c>
-      <c r="K3" s="34">
+      <c r="K3" s="35">
         <v>5</v>
       </c>
-      <c r="L3" s="34">
+      <c r="L3" s="35">
         <v>3.5</v>
       </c>
-      <c r="M3" s="34">
+      <c r="M3" s="35">
         <v>3</v>
       </c>
-      <c r="N3" s="34">
+      <c r="N3" s="35">
         <v>3</v>
       </c>
-      <c r="P3" s="36" t="s">
+      <c r="P3" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="Q3" s="38">
+      <c r="Q3" s="36">
         <v>5</v>
       </c>
-      <c r="R3" s="39">
+      <c r="R3" s="37">
         <v>5</v>
       </c>
-      <c r="S3" s="40">
+      <c r="S3" s="38">
         <v>3.5</v>
       </c>
-      <c r="T3" s="40">
+      <c r="T3" s="38">
         <v>3</v>
       </c>
-      <c r="U3" s="40">
+      <c r="U3" s="38">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="17.25" thickBot="1">
       <c r="A4" s="9"/>
-      <c r="B4" s="49"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="51"/>
-      <c r="I4" t="s">
+      <c r="B4" s="47"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="49"/>
+      <c r="I4" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="35">
+      <c r="J4" s="56">
         <v>1</v>
       </c>
-      <c r="K4" s="35">
+      <c r="K4" s="56">
         <v>1.5</v>
       </c>
-      <c r="L4" s="35">
+      <c r="L4" s="56">
         <v>1</v>
       </c>
-      <c r="M4" s="35">
+      <c r="M4" s="56">
         <v>2</v>
       </c>
-      <c r="N4" s="35">
+      <c r="N4" s="56">
         <v>1</v>
       </c>
-      <c r="P4" s="36" t="s">
+      <c r="P4" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="Q4" s="41">
+      <c r="Q4" s="39">
         <v>16</v>
       </c>
       <c r="R4" s="30">
@@ -1942,29 +1962,29 @@
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
-      <c r="I5" t="s">
+      <c r="I5" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="35">
+      <c r="J5" s="56">
         <v>7</v>
       </c>
-      <c r="K5" s="35">
+      <c r="K5" s="56">
         <v>3</v>
       </c>
-      <c r="L5" s="35">
+      <c r="L5" s="56">
         <v>2</v>
       </c>
-      <c r="M5" s="35">
+      <c r="M5" s="56">
         <v>8.75</v>
       </c>
-      <c r="N5" s="35">
+      <c r="N5" s="56">
         <v>5.25</v>
       </c>
-      <c r="P5" s="36" t="s">
+      <c r="P5" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="Q5" s="42">
-        <v>29.5</v>
+      <c r="Q5" s="40">
+        <v>33</v>
       </c>
       <c r="R5" s="27">
         <v>23</v>
@@ -1987,28 +2007,28 @@
       <c r="E6" s="13"/>
       <c r="F6" s="16"/>
       <c r="G6" s="13"/>
-      <c r="I6" t="s">
+      <c r="I6" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="35">
+      <c r="J6" s="56">
         <v>1</v>
       </c>
-      <c r="K6" s="35">
+      <c r="K6" s="56">
         <v>7</v>
       </c>
-      <c r="L6" s="35">
+      <c r="L6" s="56">
         <v>1.5</v>
       </c>
-      <c r="M6" s="35">
+      <c r="M6" s="56">
         <v>2.5</v>
       </c>
-      <c r="N6" s="35">
+      <c r="N6" s="56">
         <v>3.5</v>
       </c>
-      <c r="P6" s="36" t="s">
+      <c r="P6" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="Q6" s="42"/>
+      <c r="Q6" s="40"/>
       <c r="R6" s="27"/>
       <c r="S6" s="28"/>
       <c r="T6" s="28">
@@ -2026,28 +2046,28 @@
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
       <c r="G7" s="16"/>
-      <c r="I7" t="s">
+      <c r="I7" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="35">
+      <c r="J7" s="56">
         <v>11</v>
       </c>
-      <c r="K7" s="35">
+      <c r="K7" s="56">
         <v>7</v>
       </c>
-      <c r="L7" s="35">
+      <c r="L7" s="56">
         <v>6</v>
       </c>
-      <c r="M7" s="35">
+      <c r="M7" s="56">
         <v>7.75</v>
       </c>
-      <c r="N7" s="35">
+      <c r="N7" s="56">
         <v>7.25</v>
       </c>
-      <c r="P7" s="36" t="s">
+      <c r="P7" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="Q7" s="42">
+      <c r="Q7" s="40">
         <v>6</v>
       </c>
       <c r="R7" s="27">
@@ -2060,7 +2080,7 @@
         <v>6</v>
       </c>
       <c r="U7" s="28">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="17.25" thickBot="1">
@@ -2071,28 +2091,28 @@
       <c r="E8" s="16"/>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
-      <c r="I8" t="s">
+      <c r="I8" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="J8" s="35">
+      <c r="J8" s="56">
         <v>0</v>
       </c>
-      <c r="K8" s="35">
+      <c r="K8" s="56">
         <v>0</v>
       </c>
-      <c r="L8" s="35">
+      <c r="L8" s="56">
         <v>6</v>
       </c>
-      <c r="M8" s="35">
+      <c r="M8" s="56">
         <v>0</v>
       </c>
-      <c r="N8" s="35">
+      <c r="N8" s="56">
         <v>0</v>
       </c>
-      <c r="P8" s="36" t="s">
+      <c r="P8" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="Q8" s="42">
+      <c r="Q8" s="40">
         <v>5.75</v>
       </c>
       <c r="R8" s="27"/>
@@ -2103,7 +2123,7 @@
         <v>7.5</v>
       </c>
       <c r="U8" s="28">
-        <v>11</v>
+        <v>13.25</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="17.25" thickBot="1">
@@ -2114,22 +2134,22 @@
       <c r="E9" s="16"/>
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
-      <c r="I9" t="s">
+      <c r="I9" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="34">
+      <c r="J9" s="35">
         <v>0</v>
       </c>
-      <c r="K9" s="35">
+      <c r="K9" s="56">
         <v>0</v>
       </c>
-      <c r="L9" s="35">
+      <c r="L9" s="56">
         <v>6</v>
       </c>
-      <c r="M9" s="35">
+      <c r="M9" s="56">
         <v>3.5</v>
       </c>
-      <c r="N9" s="35">
+      <c r="N9" s="56">
         <v>0</v>
       </c>
     </row>
@@ -2141,49 +2161,49 @@
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
-      <c r="I10" t="s">
+      <c r="I10" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="J10" s="34">
+      <c r="J10" s="35">
         <v>12.25</v>
       </c>
-      <c r="K10" s="34">
+      <c r="K10" s="35">
         <v>0</v>
       </c>
-      <c r="L10" s="34">
+      <c r="L10" s="35">
         <v>2</v>
       </c>
-      <c r="M10" s="34">
+      <c r="M10" s="35">
         <v>5</v>
       </c>
-      <c r="N10" s="34">
+      <c r="N10" s="35">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="17.25" thickBot="1">
       <c r="A11" s="20"/>
-      <c r="B11" s="46"/>
-      <c r="C11" s="47"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="48"/>
-      <c r="I11" t="s">
+      <c r="B11" s="44"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="46"/>
+      <c r="I11" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="J11" s="58">
+      <c r="J11" s="57">
         <v>22</v>
       </c>
-      <c r="K11" s="59">
+      <c r="K11" s="57">
         <v>15</v>
       </c>
-      <c r="L11" s="60">
+      <c r="L11" s="35">
         <v>12.5</v>
       </c>
-      <c r="M11" s="60">
+      <c r="M11" s="35">
         <v>9</v>
       </c>
-      <c r="N11" s="60">
+      <c r="N11" s="35">
         <v>16.25</v>
       </c>
     </row>
@@ -2195,6 +2215,20 @@
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
+      <c r="I12" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="J12" s="57">
+        <v>7.25</v>
+      </c>
+      <c r="K12" s="57"/>
+      <c r="L12" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="M12" s="35"/>
+      <c r="N12" s="35">
+        <v>2.25</v>
+      </c>
     </row>
     <row r="13" spans="1:21" ht="17.25" thickBot="1">
       <c r="A13" s="14"/>
@@ -2234,12 +2268,12 @@
     </row>
     <row r="17" spans="1:7" ht="17.25" thickBot="1">
       <c r="A17" s="20"/>
-      <c r="B17" s="46"/>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="48"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="46"/>
     </row>
     <row r="18" spans="1:7" ht="17.25" thickBot="1">
       <c r="A18" s="14"/>
@@ -2288,12 +2322,12 @@
     </row>
     <row r="23" spans="1:7" ht="17.25" thickBot="1">
       <c r="A23" s="20"/>
-      <c r="B23" s="46"/>
-      <c r="C23" s="47"/>
-      <c r="D23" s="47"/>
-      <c r="E23" s="47"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="48"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="46"/>
     </row>
     <row r="24" spans="1:7" ht="17.25" thickBot="1">
       <c r="A24" s="14"/>
@@ -2324,12 +2358,12 @@
     </row>
     <row r="27" spans="1:7" ht="17.25" thickBot="1">
       <c r="A27" s="20"/>
-      <c r="B27" s="46"/>
-      <c r="C27" s="47"/>
-      <c r="D27" s="47"/>
-      <c r="E27" s="47"/>
-      <c r="F27" s="47"/>
-      <c r="G27" s="48"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="46"/>
     </row>
     <row r="28" spans="1:7" ht="17.25" thickBot="1">
       <c r="A28" s="14"/>
@@ -2351,12 +2385,12 @@
     </row>
     <row r="30" spans="1:7" ht="17.25" thickBot="1">
       <c r="A30" s="20"/>
-      <c r="B30" s="46"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="48"/>
+      <c r="B30" s="44"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="46"/>
     </row>
     <row r="31" spans="1:7" ht="17.25" thickBot="1">
       <c r="A31" s="14"/>
@@ -2408,12 +2442,12 @@
     </row>
     <row r="37" spans="1:7" ht="17.25" thickBot="1">
       <c r="A37" s="23"/>
-      <c r="B37" s="52"/>
-      <c r="C37" s="53"/>
-      <c r="D37" s="53"/>
-      <c r="E37" s="53"/>
-      <c r="F37" s="53"/>
-      <c r="G37" s="54"/>
+      <c r="B37" s="50"/>
+      <c r="C37" s="51"/>
+      <c r="D37" s="51"/>
+      <c r="E37" s="51"/>
+      <c r="F37" s="51"/>
+      <c r="G37" s="52"/>
     </row>
     <row r="38" spans="1:7" ht="17.25" thickBot="1">
       <c r="A38" s="14"/>
@@ -2426,12 +2460,12 @@
     </row>
     <row r="39" spans="1:7" ht="17.25" thickBot="1">
       <c r="A39" s="20"/>
-      <c r="B39" s="46"/>
-      <c r="C39" s="47"/>
-      <c r="D39" s="47"/>
-      <c r="E39" s="47"/>
-      <c r="F39" s="47"/>
-      <c r="G39" s="48"/>
+      <c r="B39" s="44"/>
+      <c r="C39" s="45"/>
+      <c r="D39" s="45"/>
+      <c r="E39" s="45"/>
+      <c r="F39" s="45"/>
+      <c r="G39" s="46"/>
     </row>
     <row r="40" spans="1:7" ht="17.25" thickBot="1">
       <c r="A40" s="14"/>
@@ -2453,12 +2487,12 @@
     </row>
     <row r="42" spans="1:7" ht="17.25" thickBot="1">
       <c r="A42" s="20"/>
-      <c r="B42" s="55"/>
-      <c r="C42" s="56"/>
-      <c r="D42" s="56"/>
-      <c r="E42" s="56"/>
-      <c r="F42" s="56"/>
-      <c r="G42" s="57"/>
+      <c r="B42" s="53"/>
+      <c r="C42" s="54"/>
+      <c r="D42" s="54"/>
+      <c r="E42" s="54"/>
+      <c r="F42" s="54"/>
+      <c r="G42" s="55"/>
     </row>
     <row r="43" spans="1:7" ht="17.25" thickBot="1">
       <c r="A43" s="14"/>
@@ -2498,12 +2532,12 @@
     </row>
     <row r="47" spans="1:7" ht="17.25" thickBot="1">
       <c r="A47" s="20"/>
-      <c r="B47" s="46"/>
-      <c r="C47" s="47"/>
-      <c r="D47" s="47"/>
-      <c r="E47" s="47"/>
-      <c r="F47" s="47"/>
-      <c r="G47" s="48"/>
+      <c r="B47" s="44"/>
+      <c r="C47" s="45"/>
+      <c r="D47" s="45"/>
+      <c r="E47" s="45"/>
+      <c r="F47" s="45"/>
+      <c r="G47" s="46"/>
     </row>
     <row r="48" spans="1:7" ht="17.25" thickBot="1">
       <c r="A48" s="14"/>
@@ -2534,12 +2568,12 @@
     </row>
     <row r="51" spans="1:7" ht="17.25" thickBot="1">
       <c r="A51" s="20"/>
-      <c r="B51" s="46"/>
-      <c r="C51" s="47"/>
-      <c r="D51" s="47"/>
-      <c r="E51" s="47"/>
-      <c r="F51" s="47"/>
-      <c r="G51" s="48"/>
+      <c r="B51" s="44"/>
+      <c r="C51" s="45"/>
+      <c r="D51" s="45"/>
+      <c r="E51" s="45"/>
+      <c r="F51" s="45"/>
+      <c r="G51" s="46"/>
     </row>
     <row r="52" spans="1:7" ht="17.25" thickBot="1">
       <c r="A52" s="14"/>
@@ -2570,12 +2604,12 @@
     </row>
     <row r="55" spans="1:7" ht="17.25" thickBot="1">
       <c r="A55" s="20"/>
-      <c r="B55" s="46"/>
-      <c r="C55" s="47"/>
-      <c r="D55" s="47"/>
-      <c r="E55" s="47"/>
-      <c r="F55" s="47"/>
-      <c r="G55" s="48"/>
+      <c r="B55" s="44"/>
+      <c r="C55" s="45"/>
+      <c r="D55" s="45"/>
+      <c r="E55" s="45"/>
+      <c r="F55" s="45"/>
+      <c r="G55" s="46"/>
     </row>
     <row r="56" spans="1:7" ht="17.25" thickBot="1">
       <c r="A56" s="14"/>
@@ -2606,12 +2640,12 @@
     </row>
     <row r="59" spans="1:7" ht="17.25" thickBot="1">
       <c r="A59" s="20"/>
-      <c r="B59" s="46"/>
-      <c r="C59" s="47"/>
-      <c r="D59" s="47"/>
-      <c r="E59" s="47"/>
-      <c r="F59" s="47"/>
-      <c r="G59" s="48"/>
+      <c r="B59" s="44"/>
+      <c r="C59" s="45"/>
+      <c r="D59" s="45"/>
+      <c r="E59" s="45"/>
+      <c r="F59" s="45"/>
+      <c r="G59" s="46"/>
     </row>
     <row r="60" spans="1:7" ht="17.25" thickBot="1">
       <c r="A60" s="14"/>
@@ -2651,12 +2685,12 @@
     </row>
     <row r="64" spans="1:7" ht="17.25" thickBot="1">
       <c r="A64" s="20"/>
-      <c r="B64" s="46"/>
-      <c r="C64" s="47"/>
-      <c r="D64" s="47"/>
-      <c r="E64" s="47"/>
-      <c r="F64" s="47"/>
-      <c r="G64" s="48"/>
+      <c r="B64" s="44"/>
+      <c r="C64" s="45"/>
+      <c r="D64" s="45"/>
+      <c r="E64" s="45"/>
+      <c r="F64" s="45"/>
+      <c r="G64" s="46"/>
     </row>
     <row r="65" spans="1:7" ht="17.25" thickBot="1">
       <c r="A65" s="14"/>
@@ -2669,12 +2703,12 @@
     </row>
     <row r="66" spans="1:7" ht="17.25" thickBot="1">
       <c r="A66" s="20"/>
-      <c r="B66" s="46"/>
-      <c r="C66" s="47"/>
-      <c r="D66" s="47"/>
-      <c r="E66" s="47"/>
-      <c r="F66" s="47"/>
-      <c r="G66" s="48"/>
+      <c r="B66" s="44"/>
+      <c r="C66" s="45"/>
+      <c r="D66" s="45"/>
+      <c r="E66" s="45"/>
+      <c r="F66" s="45"/>
+      <c r="G66" s="46"/>
     </row>
     <row r="67" spans="1:7" ht="17.25" thickBot="1">
       <c r="A67" s="14"/>
@@ -2696,12 +2730,12 @@
     </row>
     <row r="69" spans="1:7" ht="17.25" thickBot="1">
       <c r="A69" s="20"/>
-      <c r="B69" s="46"/>
-      <c r="C69" s="47"/>
-      <c r="D69" s="47"/>
-      <c r="E69" s="47"/>
-      <c r="F69" s="47"/>
-      <c r="G69" s="48"/>
+      <c r="B69" s="44"/>
+      <c r="C69" s="45"/>
+      <c r="D69" s="45"/>
+      <c r="E69" s="45"/>
+      <c r="F69" s="45"/>
+      <c r="G69" s="46"/>
     </row>
     <row r="70" spans="1:7" ht="17.25" thickBot="1">
       <c r="A70" s="14"/>
@@ -2750,12 +2784,12 @@
     </row>
     <row r="75" spans="1:7" ht="17.25" thickBot="1">
       <c r="A75" s="20"/>
-      <c r="B75" s="46"/>
-      <c r="C75" s="47"/>
-      <c r="D75" s="47"/>
-      <c r="E75" s="47"/>
-      <c r="F75" s="47"/>
-      <c r="G75" s="48"/>
+      <c r="B75" s="44"/>
+      <c r="C75" s="45"/>
+      <c r="D75" s="45"/>
+      <c r="E75" s="45"/>
+      <c r="F75" s="45"/>
+      <c r="G75" s="46"/>
     </row>
     <row r="76" spans="1:7" ht="17.25" thickBot="1">
       <c r="A76" s="14"/>
@@ -2777,12 +2811,12 @@
     </row>
     <row r="78" spans="1:7" ht="17.25" thickBot="1">
       <c r="A78" s="20"/>
-      <c r="B78" s="46"/>
-      <c r="C78" s="47"/>
-      <c r="D78" s="47"/>
-      <c r="E78" s="47"/>
-      <c r="F78" s="47"/>
-      <c r="G78" s="48"/>
+      <c r="B78" s="44"/>
+      <c r="C78" s="45"/>
+      <c r="D78" s="45"/>
+      <c r="E78" s="45"/>
+      <c r="F78" s="45"/>
+      <c r="G78" s="46"/>
     </row>
     <row r="79" spans="1:7" ht="17.25" thickBot="1">
       <c r="A79" s="14"/>
@@ -2822,12 +2856,12 @@
     </row>
     <row r="83" spans="1:7" ht="17.25" thickBot="1">
       <c r="A83" s="25"/>
-      <c r="B83" s="43"/>
-      <c r="C83" s="44"/>
-      <c r="D83" s="44"/>
-      <c r="E83" s="44"/>
-      <c r="F83" s="44"/>
-      <c r="G83" s="45"/>
+      <c r="B83" s="41"/>
+      <c r="C83" s="42"/>
+      <c r="D83" s="42"/>
+      <c r="E83" s="42"/>
+      <c r="F83" s="42"/>
+      <c r="G83" s="43"/>
     </row>
     <row r="84" spans="1:7" ht="17.25" thickBot="1">
       <c r="A84" s="9"/>

</xml_diff>

<commit_message>
* Updated Graphs.xlsx and Time spent per member per week and activity.docx * Modified Time Management Account.docx : Added descriptions on first 3 graphs, 1 left
</commit_message>
<xml_diff>
--- a/doc/End of Project Report/Graphs.xlsx
+++ b/doc/End of Project Report/Graphs.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="30" windowWidth="19395" windowHeight="7830"/>
@@ -309,7 +309,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -433,6 +433,12 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -478,11 +484,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -613,7 +622,7 @@
                   <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7.25</c:v>
+                  <c:v>11.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -707,6 +716,9 @@
                 <c:pt idx="8">
                   <c:v>15</c:v>
                 </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -800,7 +812,7 @@
                   <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.5</c:v>
+                  <c:v>1.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -893,6 +905,9 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -998,31 +1013,31 @@
                   <c:v>16.25</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.25</c:v>
+                  <c:v>5.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="42738048"/>
-        <c:axId val="42739584"/>
+        <c:axId val="58925440"/>
+        <c:axId val="58926976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="42738048"/>
+        <c:axId val="58925440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42739584"/>
+        <c:crossAx val="58926976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="42739584"/>
+        <c:axId val="58926976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1030,7 +1045,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0_);\(#,##0\)" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42738048"/>
+        <c:crossAx val="58925440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1043,7 +1058,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1136,7 +1151,10 @@
                   <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33</c:v>
+                  <c:v>35.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>6</c:v>
@@ -1265,6 +1283,9 @@
                 <c:pt idx="2">
                   <c:v>18</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.75</c:v>
+                </c:pt>
                 <c:pt idx="4">
                   <c:v>6</c:v>
                 </c:pt>
@@ -1325,13 +1346,13 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.5</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17</c:v>
+                  <c:v>19.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>6</c:v>
@@ -1396,7 +1417,7 @@
                   <c:v>3.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.25</c:v>
+                  <c:v>18.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>6</c:v>
@@ -1405,32 +1426,32 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13.25</c:v>
+                  <c:v>15.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="42788352"/>
-        <c:axId val="42789888"/>
+        <c:axId val="58975744"/>
+        <c:axId val="58977280"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="42788352"/>
+        <c:axId val="58975744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42789888"/>
+        <c:crossAx val="58977280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="42789888"/>
+        <c:axId val="58977280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1438,7 +1459,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42788352"/>
+        <c:crossAx val="58975744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1451,7 +1472,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1809,8 +1830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="P33" sqref="P33"/>
+    <sheetView tabSelected="1" topLeftCell="I16" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1911,28 +1932,28 @@
     </row>
     <row r="4" spans="1:21" ht="17.25" thickBot="1">
       <c r="A4" s="9"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="49"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="51"/>
       <c r="I4" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="56">
+      <c r="J4" s="41">
         <v>1</v>
       </c>
-      <c r="K4" s="56">
+      <c r="K4" s="41">
         <v>1.5</v>
       </c>
-      <c r="L4" s="56">
+      <c r="L4" s="41">
         <v>1</v>
       </c>
-      <c r="M4" s="56">
+      <c r="M4" s="41">
         <v>2</v>
       </c>
-      <c r="N4" s="56">
+      <c r="N4" s="41">
         <v>1</v>
       </c>
       <c r="P4" s="34" t="s">
@@ -1948,7 +1969,7 @@
         <v>8</v>
       </c>
       <c r="T4" s="31">
-        <v>7.5</v>
+        <v>8.5</v>
       </c>
       <c r="U4" s="31">
         <v>3.25</v>
@@ -1965,26 +1986,26 @@
       <c r="I5" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="56">
+      <c r="J5" s="41">
         <v>7</v>
       </c>
-      <c r="K5" s="56">
+      <c r="K5" s="41">
         <v>3</v>
       </c>
-      <c r="L5" s="56">
+      <c r="L5" s="41">
         <v>2</v>
       </c>
-      <c r="M5" s="56">
+      <c r="M5" s="41">
         <v>8.75</v>
       </c>
-      <c r="N5" s="56">
+      <c r="N5" s="41">
         <v>5.25</v>
       </c>
       <c r="P5" s="34" t="s">
         <v>17</v>
       </c>
       <c r="Q5" s="40">
-        <v>33</v>
+        <v>35.5</v>
       </c>
       <c r="R5" s="27">
         <v>23</v>
@@ -1993,10 +2014,10 @@
         <v>18</v>
       </c>
       <c r="T5" s="28">
-        <v>17</v>
+        <v>19.5</v>
       </c>
       <c r="U5" s="28">
-        <v>17.25</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="17.25" thickBot="1">
@@ -2010,29 +2031,33 @@
       <c r="I6" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="56">
+      <c r="J6" s="41">
         <v>1</v>
       </c>
-      <c r="K6" s="56">
+      <c r="K6" s="41">
         <v>7</v>
       </c>
-      <c r="L6" s="56">
+      <c r="L6" s="41">
         <v>1.5</v>
       </c>
-      <c r="M6" s="56">
+      <c r="M6" s="41">
         <v>2.5</v>
       </c>
-      <c r="N6" s="56">
+      <c r="N6" s="41">
         <v>3.5</v>
       </c>
       <c r="P6" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="Q6" s="40"/>
+      <c r="Q6" s="40">
+        <v>3</v>
+      </c>
       <c r="R6" s="27"/>
-      <c r="S6" s="28"/>
+      <c r="S6" s="28">
+        <v>0.75</v>
+      </c>
       <c r="T6" s="28">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="U6" s="28">
         <v>6</v>
@@ -2049,19 +2074,19 @@
       <c r="I7" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="56">
+      <c r="J7" s="41">
         <v>11</v>
       </c>
-      <c r="K7" s="56">
+      <c r="K7" s="41">
         <v>7</v>
       </c>
-      <c r="L7" s="56">
+      <c r="L7" s="41">
         <v>6</v>
       </c>
-      <c r="M7" s="56">
+      <c r="M7" s="41">
         <v>7.75</v>
       </c>
-      <c r="N7" s="56">
+      <c r="N7" s="41">
         <v>7.25</v>
       </c>
       <c r="P7" s="34" t="s">
@@ -2094,19 +2119,19 @@
       <c r="I8" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="J8" s="56">
+      <c r="J8" s="41">
         <v>0</v>
       </c>
-      <c r="K8" s="56">
+      <c r="K8" s="41">
         <v>0</v>
       </c>
-      <c r="L8" s="56">
+      <c r="L8" s="41">
         <v>6</v>
       </c>
-      <c r="M8" s="56">
+      <c r="M8" s="41">
         <v>0</v>
       </c>
-      <c r="N8" s="56">
+      <c r="N8" s="41">
         <v>0</v>
       </c>
       <c r="P8" s="34" t="s">
@@ -2123,7 +2148,7 @@
         <v>7.5</v>
       </c>
       <c r="U8" s="28">
-        <v>13.25</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="17.25" thickBot="1">
@@ -2140,16 +2165,16 @@
       <c r="J9" s="35">
         <v>0</v>
       </c>
-      <c r="K9" s="56">
+      <c r="K9" s="41">
         <v>0</v>
       </c>
-      <c r="L9" s="56">
+      <c r="L9" s="41">
         <v>6</v>
       </c>
-      <c r="M9" s="56">
+      <c r="M9" s="41">
         <v>3.5</v>
       </c>
-      <c r="N9" s="56">
+      <c r="N9" s="41">
         <v>0</v>
       </c>
     </row>
@@ -2182,19 +2207,19 @@
     </row>
     <row r="11" spans="1:21" ht="17.25" thickBot="1">
       <c r="A11" s="20"/>
-      <c r="B11" s="44"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="46"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="48"/>
       <c r="I11" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="J11" s="57">
+      <c r="J11" s="42">
         <v>22</v>
       </c>
-      <c r="K11" s="57">
+      <c r="K11" s="42">
         <v>15</v>
       </c>
       <c r="L11" s="35">
@@ -2218,16 +2243,20 @@
       <c r="I12" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="J12" s="57">
-        <v>7.25</v>
-      </c>
-      <c r="K12" s="57"/>
-      <c r="L12" s="35">
-        <v>0.5</v>
-      </c>
-      <c r="M12" s="35"/>
-      <c r="N12" s="35">
-        <v>2.25</v>
+      <c r="J12" s="58">
+        <v>11.75</v>
+      </c>
+      <c r="K12" s="59">
+        <v>0</v>
+      </c>
+      <c r="L12" s="60">
+        <v>1.25</v>
+      </c>
+      <c r="M12" s="60">
+        <v>5.5</v>
+      </c>
+      <c r="N12" s="60">
+        <v>5.75</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="17.25" thickBot="1">
@@ -2268,12 +2297,12 @@
     </row>
     <row r="17" spans="1:7" ht="17.25" thickBot="1">
       <c r="A17" s="20"/>
-      <c r="B17" s="44"/>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="46"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="48"/>
     </row>
     <row r="18" spans="1:7" ht="17.25" thickBot="1">
       <c r="A18" s="14"/>
@@ -2322,12 +2351,12 @@
     </row>
     <row r="23" spans="1:7" ht="17.25" thickBot="1">
       <c r="A23" s="20"/>
-      <c r="B23" s="44"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="45"/>
-      <c r="G23" s="46"/>
+      <c r="B23" s="46"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="48"/>
     </row>
     <row r="24" spans="1:7" ht="17.25" thickBot="1">
       <c r="A24" s="14"/>
@@ -2358,12 +2387,12 @@
     </row>
     <row r="27" spans="1:7" ht="17.25" thickBot="1">
       <c r="A27" s="20"/>
-      <c r="B27" s="44"/>
-      <c r="C27" s="45"/>
-      <c r="D27" s="45"/>
-      <c r="E27" s="45"/>
-      <c r="F27" s="45"/>
-      <c r="G27" s="46"/>
+      <c r="B27" s="46"/>
+      <c r="C27" s="47"/>
+      <c r="D27" s="47"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="47"/>
+      <c r="G27" s="48"/>
     </row>
     <row r="28" spans="1:7" ht="17.25" thickBot="1">
       <c r="A28" s="14"/>
@@ -2385,12 +2414,12 @@
     </row>
     <row r="30" spans="1:7" ht="17.25" thickBot="1">
       <c r="A30" s="20"/>
-      <c r="B30" s="44"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="46"/>
+      <c r="B30" s="46"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="48"/>
     </row>
     <row r="31" spans="1:7" ht="17.25" thickBot="1">
       <c r="A31" s="14"/>
@@ -2442,12 +2471,12 @@
     </row>
     <row r="37" spans="1:7" ht="17.25" thickBot="1">
       <c r="A37" s="23"/>
-      <c r="B37" s="50"/>
-      <c r="C37" s="51"/>
-      <c r="D37" s="51"/>
-      <c r="E37" s="51"/>
-      <c r="F37" s="51"/>
-      <c r="G37" s="52"/>
+      <c r="B37" s="52"/>
+      <c r="C37" s="53"/>
+      <c r="D37" s="53"/>
+      <c r="E37" s="53"/>
+      <c r="F37" s="53"/>
+      <c r="G37" s="54"/>
     </row>
     <row r="38" spans="1:7" ht="17.25" thickBot="1">
       <c r="A38" s="14"/>
@@ -2460,12 +2489,12 @@
     </row>
     <row r="39" spans="1:7" ht="17.25" thickBot="1">
       <c r="A39" s="20"/>
-      <c r="B39" s="44"/>
-      <c r="C39" s="45"/>
-      <c r="D39" s="45"/>
-      <c r="E39" s="45"/>
-      <c r="F39" s="45"/>
-      <c r="G39" s="46"/>
+      <c r="B39" s="46"/>
+      <c r="C39" s="47"/>
+      <c r="D39" s="47"/>
+      <c r="E39" s="47"/>
+      <c r="F39" s="47"/>
+      <c r="G39" s="48"/>
     </row>
     <row r="40" spans="1:7" ht="17.25" thickBot="1">
       <c r="A40" s="14"/>
@@ -2487,12 +2516,12 @@
     </row>
     <row r="42" spans="1:7" ht="17.25" thickBot="1">
       <c r="A42" s="20"/>
-      <c r="B42" s="53"/>
-      <c r="C42" s="54"/>
-      <c r="D42" s="54"/>
-      <c r="E42" s="54"/>
-      <c r="F42" s="54"/>
-      <c r="G42" s="55"/>
+      <c r="B42" s="55"/>
+      <c r="C42" s="56"/>
+      <c r="D42" s="56"/>
+      <c r="E42" s="56"/>
+      <c r="F42" s="56"/>
+      <c r="G42" s="57"/>
     </row>
     <row r="43" spans="1:7" ht="17.25" thickBot="1">
       <c r="A43" s="14"/>
@@ -2532,12 +2561,12 @@
     </row>
     <row r="47" spans="1:7" ht="17.25" thickBot="1">
       <c r="A47" s="20"/>
-      <c r="B47" s="44"/>
-      <c r="C47" s="45"/>
-      <c r="D47" s="45"/>
-      <c r="E47" s="45"/>
-      <c r="F47" s="45"/>
-      <c r="G47" s="46"/>
+      <c r="B47" s="46"/>
+      <c r="C47" s="47"/>
+      <c r="D47" s="47"/>
+      <c r="E47" s="47"/>
+      <c r="F47" s="47"/>
+      <c r="G47" s="48"/>
     </row>
     <row r="48" spans="1:7" ht="17.25" thickBot="1">
       <c r="A48" s="14"/>
@@ -2568,12 +2597,12 @@
     </row>
     <row r="51" spans="1:7" ht="17.25" thickBot="1">
       <c r="A51" s="20"/>
-      <c r="B51" s="44"/>
-      <c r="C51" s="45"/>
-      <c r="D51" s="45"/>
-      <c r="E51" s="45"/>
-      <c r="F51" s="45"/>
-      <c r="G51" s="46"/>
+      <c r="B51" s="46"/>
+      <c r="C51" s="47"/>
+      <c r="D51" s="47"/>
+      <c r="E51" s="47"/>
+      <c r="F51" s="47"/>
+      <c r="G51" s="48"/>
     </row>
     <row r="52" spans="1:7" ht="17.25" thickBot="1">
       <c r="A52" s="14"/>
@@ -2604,12 +2633,12 @@
     </row>
     <row r="55" spans="1:7" ht="17.25" thickBot="1">
       <c r="A55" s="20"/>
-      <c r="B55" s="44"/>
-      <c r="C55" s="45"/>
-      <c r="D55" s="45"/>
-      <c r="E55" s="45"/>
-      <c r="F55" s="45"/>
-      <c r="G55" s="46"/>
+      <c r="B55" s="46"/>
+      <c r="C55" s="47"/>
+      <c r="D55" s="47"/>
+      <c r="E55" s="47"/>
+      <c r="F55" s="47"/>
+      <c r="G55" s="48"/>
     </row>
     <row r="56" spans="1:7" ht="17.25" thickBot="1">
       <c r="A56" s="14"/>
@@ -2640,12 +2669,12 @@
     </row>
     <row r="59" spans="1:7" ht="17.25" thickBot="1">
       <c r="A59" s="20"/>
-      <c r="B59" s="44"/>
-      <c r="C59" s="45"/>
-      <c r="D59" s="45"/>
-      <c r="E59" s="45"/>
-      <c r="F59" s="45"/>
-      <c r="G59" s="46"/>
+      <c r="B59" s="46"/>
+      <c r="C59" s="47"/>
+      <c r="D59" s="47"/>
+      <c r="E59" s="47"/>
+      <c r="F59" s="47"/>
+      <c r="G59" s="48"/>
     </row>
     <row r="60" spans="1:7" ht="17.25" thickBot="1">
       <c r="A60" s="14"/>
@@ -2685,12 +2714,12 @@
     </row>
     <row r="64" spans="1:7" ht="17.25" thickBot="1">
       <c r="A64" s="20"/>
-      <c r="B64" s="44"/>
-      <c r="C64" s="45"/>
-      <c r="D64" s="45"/>
-      <c r="E64" s="45"/>
-      <c r="F64" s="45"/>
-      <c r="G64" s="46"/>
+      <c r="B64" s="46"/>
+      <c r="C64" s="47"/>
+      <c r="D64" s="47"/>
+      <c r="E64" s="47"/>
+      <c r="F64" s="47"/>
+      <c r="G64" s="48"/>
     </row>
     <row r="65" spans="1:7" ht="17.25" thickBot="1">
       <c r="A65" s="14"/>
@@ -2703,12 +2732,12 @@
     </row>
     <row r="66" spans="1:7" ht="17.25" thickBot="1">
       <c r="A66" s="20"/>
-      <c r="B66" s="44"/>
-      <c r="C66" s="45"/>
-      <c r="D66" s="45"/>
-      <c r="E66" s="45"/>
-      <c r="F66" s="45"/>
-      <c r="G66" s="46"/>
+      <c r="B66" s="46"/>
+      <c r="C66" s="47"/>
+      <c r="D66" s="47"/>
+      <c r="E66" s="47"/>
+      <c r="F66" s="47"/>
+      <c r="G66" s="48"/>
     </row>
     <row r="67" spans="1:7" ht="17.25" thickBot="1">
       <c r="A67" s="14"/>
@@ -2730,12 +2759,12 @@
     </row>
     <row r="69" spans="1:7" ht="17.25" thickBot="1">
       <c r="A69" s="20"/>
-      <c r="B69" s="44"/>
-      <c r="C69" s="45"/>
-      <c r="D69" s="45"/>
-      <c r="E69" s="45"/>
-      <c r="F69" s="45"/>
-      <c r="G69" s="46"/>
+      <c r="B69" s="46"/>
+      <c r="C69" s="47"/>
+      <c r="D69" s="47"/>
+      <c r="E69" s="47"/>
+      <c r="F69" s="47"/>
+      <c r="G69" s="48"/>
     </row>
     <row r="70" spans="1:7" ht="17.25" thickBot="1">
       <c r="A70" s="14"/>
@@ -2784,12 +2813,12 @@
     </row>
     <row r="75" spans="1:7" ht="17.25" thickBot="1">
       <c r="A75" s="20"/>
-      <c r="B75" s="44"/>
-      <c r="C75" s="45"/>
-      <c r="D75" s="45"/>
-      <c r="E75" s="45"/>
-      <c r="F75" s="45"/>
-      <c r="G75" s="46"/>
+      <c r="B75" s="46"/>
+      <c r="C75" s="47"/>
+      <c r="D75" s="47"/>
+      <c r="E75" s="47"/>
+      <c r="F75" s="47"/>
+      <c r="G75" s="48"/>
     </row>
     <row r="76" spans="1:7" ht="17.25" thickBot="1">
       <c r="A76" s="14"/>
@@ -2811,12 +2840,12 @@
     </row>
     <row r="78" spans="1:7" ht="17.25" thickBot="1">
       <c r="A78" s="20"/>
-      <c r="B78" s="44"/>
-      <c r="C78" s="45"/>
-      <c r="D78" s="45"/>
-      <c r="E78" s="45"/>
-      <c r="F78" s="45"/>
-      <c r="G78" s="46"/>
+      <c r="B78" s="46"/>
+      <c r="C78" s="47"/>
+      <c r="D78" s="47"/>
+      <c r="E78" s="47"/>
+      <c r="F78" s="47"/>
+      <c r="G78" s="48"/>
     </row>
     <row r="79" spans="1:7" ht="17.25" thickBot="1">
       <c r="A79" s="14"/>
@@ -2856,12 +2885,12 @@
     </row>
     <row r="83" spans="1:7" ht="17.25" thickBot="1">
       <c r="A83" s="25"/>
-      <c r="B83" s="41"/>
-      <c r="C83" s="42"/>
-      <c r="D83" s="42"/>
-      <c r="E83" s="42"/>
-      <c r="F83" s="42"/>
-      <c r="G83" s="43"/>
+      <c r="B83" s="43"/>
+      <c r="C83" s="44"/>
+      <c r="D83" s="44"/>
+      <c r="E83" s="44"/>
+      <c r="F83" s="44"/>
+      <c r="G83" s="45"/>
     </row>
     <row r="84" spans="1:7" ht="17.25" thickBot="1">
       <c r="A84" s="9"/>

</xml_diff>

<commit_message>
* Updated Graphs.xlsx and Time spent per member per week and activity.docx * Modified Time Management Account.docx : Added description on the last graph, only graphs needed to be finalize * Added the CommitsByDate.jpg : Commits by date graph from TortoiseSVN
</commit_message>
<xml_diff>
--- a/doc/End of Project Report/Graphs.xlsx
+++ b/doc/End of Project Report/Graphs.xlsx
@@ -11,12 +11,15 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+  </externalReferences>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>Edward</t>
     <phoneticPr fontId="10" type="noConversion"/>
@@ -99,6 +102,60 @@
   </si>
   <si>
     <t>Week 10</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Actual time spent and expected time spent</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Week 1</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Week 2</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Week 3</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Week 4</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Week 5</t>
+  </si>
+  <si>
+    <t>Week 6</t>
+  </si>
+  <si>
+    <t>Week 7 (11)</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Week 8 (12)</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Week 9 (13)</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Week 10 (14)</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Actual time spent</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Expected time spent</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
 </sst>
@@ -309,7 +366,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -439,6 +496,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -484,13 +550,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -812,7 +878,7 @@
                   <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.25</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -907,7 +973,7 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.5</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1013,31 +1079,31 @@
                   <c:v>16.25</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.75</c:v>
+                  <c:v>6.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="58925440"/>
-        <c:axId val="58926976"/>
+        <c:axId val="41898368"/>
+        <c:axId val="41899904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="58925440"/>
+        <c:axId val="41898368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58926976"/>
+        <c:crossAx val="41899904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58926976"/>
+        <c:axId val="41899904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1045,7 +1111,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0_);\(#,##0\)" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58925440"/>
+        <c:crossAx val="41898368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1058,7 +1124,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1278,19 +1344,19 @@
                   <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>8.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18</c:v>
+                  <c:v>23.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.75</c:v>
+                  <c:v>1.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1352,13 +1418,13 @@
                   <c:v>19.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.5</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1426,32 +1492,32 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15.5</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="58975744"/>
-        <c:axId val="58977280"/>
+        <c:axId val="41940480"/>
+        <c:axId val="41942016"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="58975744"/>
+        <c:axId val="41940480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58977280"/>
+        <c:crossAx val="41942016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58977280"/>
+        <c:axId val="41942016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1459,7 +1525,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58975744"/>
+        <c:crossAx val="41940480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1472,7 +1538,361 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="zh-TW"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" altLang="zh-TW" sz="1800" b="1" i="0" baseline="0"/>
+              <a:t>Actual time spent against expected time spent</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-TW" altLang="zh-TW" sz="1800" b="1" i="0" baseline="0"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="4.4664249736624841E-2"/>
+          <c:y val="0.10486619079157161"/>
+          <c:w val="0.81388711766905097"/>
+          <c:h val="0.80228243432187796"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$38</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual time spent</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$J$37:$S$37</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Week 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Week 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Week 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Week 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Week 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Week 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Week 7 (11)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Week 8 (12)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Week 9 (13)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Week 10 (14)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$38:$S$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>19.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>67.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>106.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>112.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>149.25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>224</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>261</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$39</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Expected time spent</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.3904982618771726E-2"/>
+                  <c:y val="-2.9906542056074768E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showVal val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.0899961375048281E-3"/>
+                  <c:y val="1.7445482866043614E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showVal val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.6349942062572421E-3"/>
+                  <c:y val="1.4953271028037384E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showVal val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.4804943993820005E-2"/>
+                  <c:y val="-3.4890965732087137E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showVal val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.544998068752414E-3"/>
+                  <c:y val="1.4953271028037384E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showVal val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="6.1799922750096561E-3"/>
+                  <c:y val="7.4766355140186919E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showVal val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="8"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.6349942062572421E-3"/>
+                  <c:y val="2.2429906542056073E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showVal val="1"/>
+            </c:dLbl>
+            <c:showVal val="1"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$J$37:$S$37</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Week 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Week 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Week 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Week 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Week 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Week 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Week 7 (11)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Week 8 (12)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Week 9 (13)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Week 10 (14)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$39:$S$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>276</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>314</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>347</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>356</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="65803008"/>
+        <c:axId val="65810816"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="65803008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="65810816"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="65810816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="65803008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.87588695948246509"/>
+          <c:y val="0.42374979763043641"/>
+          <c:w val="0.11185563500170241"/>
+          <c:h val="0.18982137513184683"/>
+        </c:manualLayout>
+      </c:layout>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1482,16 +1902,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>57149</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>219074</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1512,16 +1932,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>647701</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>28576</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>200025</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>95249</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1540,7 +1960,157 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>200024</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="圖表 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+      <sheetName val="Sheet2"/>
+      <sheetName val="Sheet3"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="C2" t="str">
+            <v>Week 1</v>
+          </cell>
+          <cell r="D2" t="str">
+            <v>Week 2</v>
+          </cell>
+          <cell r="E2" t="str">
+            <v>Week 3</v>
+          </cell>
+          <cell r="F2" t="str">
+            <v>Week 4</v>
+          </cell>
+          <cell r="G2" t="str">
+            <v>Week 5</v>
+          </cell>
+          <cell r="H2" t="str">
+            <v>Week 6</v>
+          </cell>
+          <cell r="I2" t="str">
+            <v>Week 7 (11)</v>
+          </cell>
+          <cell r="J2" t="str">
+            <v>Week 8 (12)</v>
+          </cell>
+          <cell r="K2" t="str">
+            <v>Week 9 (13)</v>
+          </cell>
+          <cell r="L2" t="str">
+            <v>Week 10 (14)</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="B3" t="str">
+            <v>Actual time spent</v>
+          </cell>
+          <cell r="C3">
+            <v>19.5</v>
+          </cell>
+          <cell r="D3">
+            <v>26</v>
+          </cell>
+          <cell r="E3">
+            <v>52</v>
+          </cell>
+          <cell r="F3">
+            <v>67.5</v>
+          </cell>
+          <cell r="G3">
+            <v>106.5</v>
+          </cell>
+          <cell r="H3">
+            <v>112.5</v>
+          </cell>
+          <cell r="I3">
+            <v>122</v>
+          </cell>
+          <cell r="J3">
+            <v>149.25</v>
+          </cell>
+          <cell r="K3">
+            <v>224</v>
+          </cell>
+          <cell r="L3">
+            <v>248.25</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="B4" t="str">
+            <v>Expected time spent</v>
+          </cell>
+          <cell r="C4">
+            <v>21</v>
+          </cell>
+          <cell r="D4">
+            <v>21.5</v>
+          </cell>
+          <cell r="E4">
+            <v>33</v>
+          </cell>
+          <cell r="F4">
+            <v>66</v>
+          </cell>
+          <cell r="G4">
+            <v>97</v>
+          </cell>
+          <cell r="H4">
+            <v>119</v>
+          </cell>
+          <cell r="I4">
+            <v>276</v>
+          </cell>
+          <cell r="J4">
+            <v>314</v>
+          </cell>
+          <cell r="K4">
+            <v>347</v>
+          </cell>
+          <cell r="L4">
+            <v>356</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1830,8 +2400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I16" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView tabSelected="1" topLeftCell="D43" workbookViewId="0">
+      <selection activeCell="S47" sqref="S47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1911,6 +2481,10 @@
       <c r="N3" s="35">
         <v>3</v>
       </c>
+      <c r="O3">
+        <f>SUM(J3:N3)</f>
+        <v>19.5</v>
+      </c>
       <c r="P3" s="34" t="s">
         <v>14</v>
       </c>
@@ -1932,12 +2506,12 @@
     </row>
     <row r="4" spans="1:21" ht="17.25" thickBot="1">
       <c r="A4" s="9"/>
-      <c r="B4" s="49"/>
-      <c r="C4" s="50"/>
-      <c r="D4" s="50"/>
-      <c r="E4" s="50"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="51"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="54"/>
       <c r="I4" s="34" t="s">
         <v>2</v>
       </c>
@@ -1956,6 +2530,10 @@
       <c r="N4" s="41">
         <v>1</v>
       </c>
+      <c r="O4">
+        <f t="shared" ref="O4:O11" si="0">SUM(J4:N4)</f>
+        <v>6.5</v>
+      </c>
       <c r="P4" s="34" t="s">
         <v>15</v>
       </c>
@@ -1966,7 +2544,7 @@
         <v>4.5</v>
       </c>
       <c r="S4" s="31">
-        <v>8</v>
+        <v>8.75</v>
       </c>
       <c r="T4" s="31">
         <v>8.5</v>
@@ -2001,6 +2579,10 @@
       <c r="N5" s="41">
         <v>5.25</v>
       </c>
+      <c r="O5">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
       <c r="P5" s="34" t="s">
         <v>17</v>
       </c>
@@ -2011,7 +2593,7 @@
         <v>23</v>
       </c>
       <c r="S5" s="28">
-        <v>18</v>
+        <v>23.5</v>
       </c>
       <c r="T5" s="28">
         <v>19.5</v>
@@ -2046,6 +2628,10 @@
       <c r="N6" s="41">
         <v>3.5</v>
       </c>
+      <c r="O6">
+        <f t="shared" si="0"/>
+        <v>15.5</v>
+      </c>
       <c r="P6" s="34" t="s">
         <v>18</v>
       </c>
@@ -2054,10 +2640,10 @@
       </c>
       <c r="R6" s="27"/>
       <c r="S6" s="28">
-        <v>0.75</v>
+        <v>1.25</v>
       </c>
       <c r="T6" s="28">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="U6" s="28">
         <v>6</v>
@@ -2089,6 +2675,10 @@
       <c r="N7" s="41">
         <v>7.25</v>
       </c>
+      <c r="O7">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
       <c r="P7" s="34" t="s">
         <v>16</v>
       </c>
@@ -2134,6 +2724,10 @@
       <c r="N8" s="41">
         <v>0</v>
       </c>
+      <c r="O8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
       <c r="P8" s="34" t="s">
         <v>19</v>
       </c>
@@ -2142,13 +2736,13 @@
       </c>
       <c r="R8" s="27"/>
       <c r="S8" s="28">
-        <v>5.5</v>
+        <v>8</v>
       </c>
       <c r="T8" s="28">
-        <v>7.5</v>
+        <v>8.5</v>
       </c>
       <c r="U8" s="28">
-        <v>15.5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="17.25" thickBot="1">
@@ -2177,6 +2771,10 @@
       <c r="N9" s="41">
         <v>0</v>
       </c>
+      <c r="O9">
+        <f t="shared" si="0"/>
+        <v>9.5</v>
+      </c>
     </row>
     <row r="10" spans="1:21" ht="17.25" thickBot="1">
       <c r="A10" s="17"/>
@@ -2204,15 +2802,19 @@
       <c r="N10" s="35">
         <v>8</v>
       </c>
+      <c r="O10">
+        <f t="shared" si="0"/>
+        <v>27.25</v>
+      </c>
     </row>
     <row r="11" spans="1:21" ht="17.25" thickBot="1">
       <c r="A11" s="20"/>
-      <c r="B11" s="46"/>
-      <c r="C11" s="47"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="48"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="51"/>
       <c r="I11" s="34" t="s">
         <v>9</v>
       </c>
@@ -2230,6 +2832,10 @@
       </c>
       <c r="N11" s="35">
         <v>16.25</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="0"/>
+        <v>74.75</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="17.25" thickBot="1">
@@ -2243,20 +2849,24 @@
       <c r="I12" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="J12" s="58">
+      <c r="J12" s="43">
         <v>11.75</v>
       </c>
-      <c r="K12" s="59">
+      <c r="K12" s="44">
         <v>0</v>
       </c>
-      <c r="L12" s="60">
-        <v>1.25</v>
-      </c>
-      <c r="M12" s="60">
-        <v>5.5</v>
-      </c>
-      <c r="N12" s="60">
-        <v>5.75</v>
+      <c r="L12" s="45">
+        <v>10.5</v>
+      </c>
+      <c r="M12" s="45">
+        <v>8.5</v>
+      </c>
+      <c r="N12" s="45">
+        <v>6.25</v>
+      </c>
+      <c r="O12">
+        <f>SUM(J12:N12)</f>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="17.25" thickBot="1">
@@ -2297,12 +2907,12 @@
     </row>
     <row r="17" spans="1:7" ht="17.25" thickBot="1">
       <c r="A17" s="20"/>
-      <c r="B17" s="46"/>
-      <c r="C17" s="47"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="48"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="51"/>
     </row>
     <row r="18" spans="1:7" ht="17.25" thickBot="1">
       <c r="A18" s="14"/>
@@ -2351,12 +2961,12 @@
     </row>
     <row r="23" spans="1:7" ht="17.25" thickBot="1">
       <c r="A23" s="20"/>
-      <c r="B23" s="46"/>
-      <c r="C23" s="47"/>
-      <c r="D23" s="47"/>
-      <c r="E23" s="47"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="48"/>
+      <c r="B23" s="49"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="51"/>
     </row>
     <row r="24" spans="1:7" ht="17.25" thickBot="1">
       <c r="A24" s="14"/>
@@ -2387,12 +2997,12 @@
     </row>
     <row r="27" spans="1:7" ht="17.25" thickBot="1">
       <c r="A27" s="20"/>
-      <c r="B27" s="46"/>
-      <c r="C27" s="47"/>
-      <c r="D27" s="47"/>
-      <c r="E27" s="47"/>
-      <c r="F27" s="47"/>
-      <c r="G27" s="48"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="50"/>
+      <c r="E27" s="50"/>
+      <c r="F27" s="50"/>
+      <c r="G27" s="51"/>
     </row>
     <row r="28" spans="1:7" ht="17.25" thickBot="1">
       <c r="A28" s="14"/>
@@ -2414,12 +3024,12 @@
     </row>
     <row r="30" spans="1:7" ht="17.25" thickBot="1">
       <c r="A30" s="20"/>
-      <c r="B30" s="46"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="48"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="50"/>
+      <c r="D30" s="50"/>
+      <c r="E30" s="50"/>
+      <c r="F30" s="50"/>
+      <c r="G30" s="51"/>
     </row>
     <row r="31" spans="1:7" ht="17.25" thickBot="1">
       <c r="A31" s="14"/>
@@ -2439,7 +3049,7 @@
       <c r="F32" s="13"/>
       <c r="G32" s="13"/>
     </row>
-    <row r="33" spans="1:7" ht="17.25" thickBot="1">
+    <row r="33" spans="1:19" ht="17.25" thickBot="1">
       <c r="A33" s="17"/>
       <c r="B33" s="22"/>
       <c r="C33" s="19"/>
@@ -2448,10 +3058,10 @@
       <c r="F33" s="8"/>
       <c r="G33" s="8"/>
     </row>
-    <row r="34" spans="1:7" ht="17.25" thickBot="1">
+    <row r="34" spans="1:19" ht="17.25" thickBot="1">
       <c r="A34" s="2"/>
     </row>
-    <row r="35" spans="1:7" ht="17.25" thickBot="1">
+    <row r="35" spans="1:19" ht="17.25" thickBot="1">
       <c r="A35" s="3"/>
       <c r="B35" s="4"/>
       <c r="C35" s="5"/>
@@ -2460,7 +3070,7 @@
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
     </row>
-    <row r="36" spans="1:7" ht="17.25" thickBot="1">
+    <row r="36" spans="1:19" ht="17.25" thickBot="1">
       <c r="A36" s="6"/>
       <c r="B36" s="7"/>
       <c r="C36" s="8"/>
@@ -2468,17 +3078,53 @@
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
       <c r="G36" s="8"/>
-    </row>
-    <row r="37" spans="1:7" ht="17.25" thickBot="1">
+      <c r="I36" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" ht="17.25" thickBot="1">
       <c r="A37" s="23"/>
-      <c r="B37" s="52"/>
-      <c r="C37" s="53"/>
-      <c r="D37" s="53"/>
-      <c r="E37" s="53"/>
-      <c r="F37" s="53"/>
-      <c r="G37" s="54"/>
-    </row>
-    <row r="38" spans="1:7" ht="17.25" thickBot="1">
+      <c r="B37" s="55"/>
+      <c r="C37" s="56"/>
+      <c r="D37" s="56"/>
+      <c r="E37" s="56"/>
+      <c r="F37" s="56"/>
+      <c r="G37" s="57"/>
+      <c r="I37" t="s">
+        <v>22</v>
+      </c>
+      <c r="J37" s="61" t="s">
+        <v>23</v>
+      </c>
+      <c r="K37" s="61" t="s">
+        <v>24</v>
+      </c>
+      <c r="L37" s="61" t="s">
+        <v>25</v>
+      </c>
+      <c r="M37" s="61" t="s">
+        <v>26</v>
+      </c>
+      <c r="N37" s="61" t="s">
+        <v>27</v>
+      </c>
+      <c r="O37" s="61" t="s">
+        <v>28</v>
+      </c>
+      <c r="P37" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q37" s="61" t="s">
+        <v>30</v>
+      </c>
+      <c r="R37" s="61" t="s">
+        <v>31</v>
+      </c>
+      <c r="S37" s="61" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" ht="17.25" thickBot="1">
       <c r="A38" s="14"/>
       <c r="B38" s="15"/>
       <c r="C38" s="12"/>
@@ -2486,17 +3132,98 @@
       <c r="E38" s="13"/>
       <c r="F38" s="13"/>
       <c r="G38" s="13"/>
-    </row>
-    <row r="39" spans="1:7" ht="17.25" thickBot="1">
+      <c r="I38" t="s">
+        <v>33</v>
+      </c>
+      <c r="J38" s="62">
+        <v>19.5</v>
+      </c>
+      <c r="K38" s="62">
+        <f>19.5+6.5</f>
+        <v>26</v>
+      </c>
+      <c r="L38" s="62">
+        <f>26+26</f>
+        <v>52</v>
+      </c>
+      <c r="M38" s="62">
+        <f>52+15.5</f>
+        <v>67.5</v>
+      </c>
+      <c r="N38" s="62">
+        <f>67.5+39</f>
+        <v>106.5</v>
+      </c>
+      <c r="O38" s="62">
+        <f>106.5+6</f>
+        <v>112.5</v>
+      </c>
+      <c r="P38" s="62">
+        <f>112.5+9.5</f>
+        <v>122</v>
+      </c>
+      <c r="Q38" s="62">
+        <f>122+27.25</f>
+        <v>149.25</v>
+      </c>
+      <c r="R38" s="62">
+        <f>149.25+74.75</f>
+        <v>224</v>
+      </c>
+      <c r="S38" s="62">
+        <f>224+37</f>
+        <v>261</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" ht="17.25" thickBot="1">
       <c r="A39" s="20"/>
-      <c r="B39" s="46"/>
-      <c r="C39" s="47"/>
-      <c r="D39" s="47"/>
-      <c r="E39" s="47"/>
-      <c r="F39" s="47"/>
-      <c r="G39" s="48"/>
-    </row>
-    <row r="40" spans="1:7" ht="17.25" thickBot="1">
+      <c r="B39" s="49"/>
+      <c r="C39" s="50"/>
+      <c r="D39" s="50"/>
+      <c r="E39" s="50"/>
+      <c r="F39" s="50"/>
+      <c r="G39" s="51"/>
+      <c r="I39" t="s">
+        <v>34</v>
+      </c>
+      <c r="J39" s="62">
+        <v>21</v>
+      </c>
+      <c r="K39" s="63">
+        <v>21.5</v>
+      </c>
+      <c r="L39" s="62">
+        <v>33</v>
+      </c>
+      <c r="M39" s="62">
+        <v>66</v>
+      </c>
+      <c r="N39" s="62">
+        <f>66+31</f>
+        <v>97</v>
+      </c>
+      <c r="O39" s="62">
+        <f>97+22</f>
+        <v>119</v>
+      </c>
+      <c r="P39" s="62">
+        <f>119+19+19+46+46+27</f>
+        <v>276</v>
+      </c>
+      <c r="Q39" s="62">
+        <f>276+38</f>
+        <v>314</v>
+      </c>
+      <c r="R39" s="62">
+        <f>314+33</f>
+        <v>347</v>
+      </c>
+      <c r="S39" s="62">
+        <f>347+9</f>
+        <v>356</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" ht="17.25" thickBot="1">
       <c r="A40" s="14"/>
       <c r="B40" s="15"/>
       <c r="C40" s="12"/>
@@ -2505,7 +3232,7 @@
       <c r="F40" s="16"/>
       <c r="G40" s="16"/>
     </row>
-    <row r="41" spans="1:7" ht="17.25" thickBot="1">
+    <row r="41" spans="1:19" ht="17.25" thickBot="1">
       <c r="A41" s="14"/>
       <c r="B41" s="15"/>
       <c r="C41" s="12"/>
@@ -2514,16 +3241,16 @@
       <c r="F41" s="16"/>
       <c r="G41" s="16"/>
     </row>
-    <row r="42" spans="1:7" ht="17.25" thickBot="1">
+    <row r="42" spans="1:19" ht="17.25" thickBot="1">
       <c r="A42" s="20"/>
-      <c r="B42" s="55"/>
-      <c r="C42" s="56"/>
-      <c r="D42" s="56"/>
-      <c r="E42" s="56"/>
-      <c r="F42" s="56"/>
-      <c r="G42" s="57"/>
-    </row>
-    <row r="43" spans="1:7" ht="17.25" thickBot="1">
+      <c r="B42" s="58"/>
+      <c r="C42" s="59"/>
+      <c r="D42" s="59"/>
+      <c r="E42" s="59"/>
+      <c r="F42" s="59"/>
+      <c r="G42" s="60"/>
+    </row>
+    <row r="43" spans="1:19" ht="17.25" thickBot="1">
       <c r="A43" s="14"/>
       <c r="B43" s="15"/>
       <c r="C43" s="12"/>
@@ -2532,7 +3259,7 @@
       <c r="F43" s="16"/>
       <c r="G43" s="16"/>
     </row>
-    <row r="44" spans="1:7" ht="17.25" thickBot="1">
+    <row r="44" spans="1:19" ht="17.25" thickBot="1">
       <c r="A44" s="14"/>
       <c r="B44" s="15"/>
       <c r="C44" s="12"/>
@@ -2541,7 +3268,7 @@
       <c r="F44" s="16"/>
       <c r="G44" s="16"/>
     </row>
-    <row r="45" spans="1:7" ht="17.25" thickBot="1">
+    <row r="45" spans="1:19" ht="17.25" thickBot="1">
       <c r="A45" s="14"/>
       <c r="B45" s="15"/>
       <c r="C45" s="12"/>
@@ -2550,7 +3277,7 @@
       <c r="F45" s="16"/>
       <c r="G45" s="16"/>
     </row>
-    <row r="46" spans="1:7" ht="17.25" thickBot="1">
+    <row r="46" spans="1:19" ht="17.25" thickBot="1">
       <c r="A46" s="17"/>
       <c r="B46" s="18"/>
       <c r="C46" s="19"/>
@@ -2559,16 +3286,16 @@
       <c r="F46" s="8"/>
       <c r="G46" s="8"/>
     </row>
-    <row r="47" spans="1:7" ht="17.25" thickBot="1">
+    <row r="47" spans="1:19" ht="17.25" thickBot="1">
       <c r="A47" s="20"/>
-      <c r="B47" s="46"/>
-      <c r="C47" s="47"/>
-      <c r="D47" s="47"/>
-      <c r="E47" s="47"/>
-      <c r="F47" s="47"/>
-      <c r="G47" s="48"/>
-    </row>
-    <row r="48" spans="1:7" ht="17.25" thickBot="1">
+      <c r="B47" s="49"/>
+      <c r="C47" s="50"/>
+      <c r="D47" s="50"/>
+      <c r="E47" s="50"/>
+      <c r="F47" s="50"/>
+      <c r="G47" s="51"/>
+    </row>
+    <row r="48" spans="1:19" ht="17.25" thickBot="1">
       <c r="A48" s="14"/>
       <c r="B48" s="15"/>
       <c r="C48" s="12"/>
@@ -2597,12 +3324,12 @@
     </row>
     <row r="51" spans="1:7" ht="17.25" thickBot="1">
       <c r="A51" s="20"/>
-      <c r="B51" s="46"/>
-      <c r="C51" s="47"/>
-      <c r="D51" s="47"/>
-      <c r="E51" s="47"/>
-      <c r="F51" s="47"/>
-      <c r="G51" s="48"/>
+      <c r="B51" s="49"/>
+      <c r="C51" s="50"/>
+      <c r="D51" s="50"/>
+      <c r="E51" s="50"/>
+      <c r="F51" s="50"/>
+      <c r="G51" s="51"/>
     </row>
     <row r="52" spans="1:7" ht="17.25" thickBot="1">
       <c r="A52" s="14"/>
@@ -2633,12 +3360,12 @@
     </row>
     <row r="55" spans="1:7" ht="17.25" thickBot="1">
       <c r="A55" s="20"/>
-      <c r="B55" s="46"/>
-      <c r="C55" s="47"/>
-      <c r="D55" s="47"/>
-      <c r="E55" s="47"/>
-      <c r="F55" s="47"/>
-      <c r="G55" s="48"/>
+      <c r="B55" s="49"/>
+      <c r="C55" s="50"/>
+      <c r="D55" s="50"/>
+      <c r="E55" s="50"/>
+      <c r="F55" s="50"/>
+      <c r="G55" s="51"/>
     </row>
     <row r="56" spans="1:7" ht="17.25" thickBot="1">
       <c r="A56" s="14"/>
@@ -2669,12 +3396,12 @@
     </row>
     <row r="59" spans="1:7" ht="17.25" thickBot="1">
       <c r="A59" s="20"/>
-      <c r="B59" s="46"/>
-      <c r="C59" s="47"/>
-      <c r="D59" s="47"/>
-      <c r="E59" s="47"/>
-      <c r="F59" s="47"/>
-      <c r="G59" s="48"/>
+      <c r="B59" s="49"/>
+      <c r="C59" s="50"/>
+      <c r="D59" s="50"/>
+      <c r="E59" s="50"/>
+      <c r="F59" s="50"/>
+      <c r="G59" s="51"/>
     </row>
     <row r="60" spans="1:7" ht="17.25" thickBot="1">
       <c r="A60" s="14"/>
@@ -2714,12 +3441,12 @@
     </row>
     <row r="64" spans="1:7" ht="17.25" thickBot="1">
       <c r="A64" s="20"/>
-      <c r="B64" s="46"/>
-      <c r="C64" s="47"/>
-      <c r="D64" s="47"/>
-      <c r="E64" s="47"/>
-      <c r="F64" s="47"/>
-      <c r="G64" s="48"/>
+      <c r="B64" s="49"/>
+      <c r="C64" s="50"/>
+      <c r="D64" s="50"/>
+      <c r="E64" s="50"/>
+      <c r="F64" s="50"/>
+      <c r="G64" s="51"/>
     </row>
     <row r="65" spans="1:7" ht="17.25" thickBot="1">
       <c r="A65" s="14"/>
@@ -2732,12 +3459,12 @@
     </row>
     <row r="66" spans="1:7" ht="17.25" thickBot="1">
       <c r="A66" s="20"/>
-      <c r="B66" s="46"/>
-      <c r="C66" s="47"/>
-      <c r="D66" s="47"/>
-      <c r="E66" s="47"/>
-      <c r="F66" s="47"/>
-      <c r="G66" s="48"/>
+      <c r="B66" s="49"/>
+      <c r="C66" s="50"/>
+      <c r="D66" s="50"/>
+      <c r="E66" s="50"/>
+      <c r="F66" s="50"/>
+      <c r="G66" s="51"/>
     </row>
     <row r="67" spans="1:7" ht="17.25" thickBot="1">
       <c r="A67" s="14"/>
@@ -2759,12 +3486,12 @@
     </row>
     <row r="69" spans="1:7" ht="17.25" thickBot="1">
       <c r="A69" s="20"/>
-      <c r="B69" s="46"/>
-      <c r="C69" s="47"/>
-      <c r="D69" s="47"/>
-      <c r="E69" s="47"/>
-      <c r="F69" s="47"/>
-      <c r="G69" s="48"/>
+      <c r="B69" s="49"/>
+      <c r="C69" s="50"/>
+      <c r="D69" s="50"/>
+      <c r="E69" s="50"/>
+      <c r="F69" s="50"/>
+      <c r="G69" s="51"/>
     </row>
     <row r="70" spans="1:7" ht="17.25" thickBot="1">
       <c r="A70" s="14"/>
@@ -2813,12 +3540,12 @@
     </row>
     <row r="75" spans="1:7" ht="17.25" thickBot="1">
       <c r="A75" s="20"/>
-      <c r="B75" s="46"/>
-      <c r="C75" s="47"/>
-      <c r="D75" s="47"/>
-      <c r="E75" s="47"/>
-      <c r="F75" s="47"/>
-      <c r="G75" s="48"/>
+      <c r="B75" s="49"/>
+      <c r="C75" s="50"/>
+      <c r="D75" s="50"/>
+      <c r="E75" s="50"/>
+      <c r="F75" s="50"/>
+      <c r="G75" s="51"/>
     </row>
     <row r="76" spans="1:7" ht="17.25" thickBot="1">
       <c r="A76" s="14"/>
@@ -2840,12 +3567,12 @@
     </row>
     <row r="78" spans="1:7" ht="17.25" thickBot="1">
       <c r="A78" s="20"/>
-      <c r="B78" s="46"/>
-      <c r="C78" s="47"/>
-      <c r="D78" s="47"/>
-      <c r="E78" s="47"/>
-      <c r="F78" s="47"/>
-      <c r="G78" s="48"/>
+      <c r="B78" s="49"/>
+      <c r="C78" s="50"/>
+      <c r="D78" s="50"/>
+      <c r="E78" s="50"/>
+      <c r="F78" s="50"/>
+      <c r="G78" s="51"/>
     </row>
     <row r="79" spans="1:7" ht="17.25" thickBot="1">
       <c r="A79" s="14"/>
@@ -2885,12 +3612,12 @@
     </row>
     <row r="83" spans="1:7" ht="17.25" thickBot="1">
       <c r="A83" s="25"/>
-      <c r="B83" s="43"/>
-      <c r="C83" s="44"/>
-      <c r="D83" s="44"/>
-      <c r="E83" s="44"/>
-      <c r="F83" s="44"/>
-      <c r="G83" s="45"/>
+      <c r="B83" s="46"/>
+      <c r="C83" s="47"/>
+      <c r="D83" s="47"/>
+      <c r="E83" s="47"/>
+      <c r="F83" s="47"/>
+      <c r="G83" s="48"/>
     </row>
     <row r="84" spans="1:7" ht="17.25" thickBot="1">
       <c r="A84" s="9"/>

</xml_diff>

<commit_message>
* Updated Graphs.xlsx, Time Management Account.docx, Time spent per member per week and activity.docx * Added Time spent per member per week and activity_2PageVersion.docx * Updated CommitsByDate graph
</commit_message>
<xml_diff>
--- a/doc/End of Project Report/Graphs.xlsx
+++ b/doc/End of Project Report/Graphs.xlsx
@@ -11,15 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
   <si>
     <t>Edward</t>
     <phoneticPr fontId="10" type="noConversion"/>
@@ -158,6 +155,10 @@
     <t>Expected time spent</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
+  <si>
+    <t>Second Presentation</t>
+    <phoneticPr fontId="10" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -261,7 +262,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -360,6 +361,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -490,20 +502,50 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
@@ -514,49 +556,19 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -583,7 +595,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" altLang="zh-TW"/>
-              <a:t>Working</a:t>
+              <a:t>4.2.3 Working</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" altLang="zh-TW" baseline="0"/>
@@ -688,7 +700,7 @@
                   <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11.75</c:v>
+                  <c:v>22.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -783,7 +795,7 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -878,7 +890,7 @@
                   <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10.5</c:v>
+                  <c:v>18.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -952,7 +964,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.75</c:v>
+                  <c:v>10.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2.5</c:v>
@@ -973,7 +985,7 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.5</c:v>
+                  <c:v>25.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1064,13 +1076,13 @@
                   <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.25</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>8</c:v>
@@ -1079,31 +1091,31 @@
                   <c:v>16.25</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.25</c:v>
+                  <c:v>12.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="41898368"/>
-        <c:axId val="41899904"/>
+        <c:axId val="57901440"/>
+        <c:axId val="57902976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="41898368"/>
+        <c:axId val="57901440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41899904"/>
+        <c:crossAx val="57902976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="41899904"/>
+        <c:axId val="57902976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1111,7 +1123,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0_);\(#,##0\)" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41898368"/>
+        <c:crossAx val="57901440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1124,7 +1136,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1145,7 +1157,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US" altLang="zh-TW"/>
-              <a:t>Distribution</a:t>
+              <a:t>4.2.1 Distribution</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" altLang="zh-TW" baseline="0"/>
@@ -1180,9 +1192,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$P$3:$P$8</c:f>
+              <c:f>Sheet1!$P$3:$P$9</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>Project Plan</c:v>
                 </c:pt>
@@ -1199,6 +1211,9 @@
                   <c:v>First Presentation</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>Second Presentation</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>Final Report</c:v>
                 </c:pt>
               </c:strCache>
@@ -1206,18 +1221,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$3:$Q$8</c:f>
+              <c:f>Sheet1!$Q$3:$Q$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>35.5</c:v>
+                  <c:v>36.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>3</c:v>
@@ -1226,7 +1241,10 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.75</c:v>
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1248,9 +1266,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$P$3:$P$8</c:f>
+              <c:f>Sheet1!$P$3:$P$9</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>Project Plan</c:v>
                 </c:pt>
@@ -1267,6 +1285,9 @@
                   <c:v>First Presentation</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>Second Presentation</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>Final Report</c:v>
                 </c:pt>
               </c:strCache>
@@ -1274,10 +1295,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$R$3:$R$8</c:f>
+              <c:f>Sheet1!$R$3:$R$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>5</c:v>
                 </c:pt>
@@ -1285,10 +1306,19 @@
                   <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23</c:v>
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1310,9 +1340,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$P$3:$P$8</c:f>
+              <c:f>Sheet1!$P$3:$P$9</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>Project Plan</c:v>
                 </c:pt>
@@ -1329,6 +1359,9 @@
                   <c:v>First Presentation</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>Second Presentation</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>Final Report</c:v>
                 </c:pt>
               </c:strCache>
@@ -1336,10 +1369,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$S$3:$S$8</c:f>
+              <c:f>Sheet1!$S$3:$S$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>3.5</c:v>
                 </c:pt>
@@ -1347,16 +1380,19 @@
                   <c:v>8.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23.5</c:v>
+                  <c:v>24.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.25</c:v>
+                  <c:v>1.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1378,9 +1414,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$P$3:$P$8</c:f>
+              <c:f>Sheet1!$P$3:$P$9</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>Project Plan</c:v>
                 </c:pt>
@@ -1397,6 +1433,9 @@
                   <c:v>First Presentation</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>Second Presentation</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>Final Report</c:v>
                 </c:pt>
               </c:strCache>
@@ -1404,10 +1443,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$T$3:$T$8</c:f>
+              <c:f>Sheet1!$T$3:$T$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -1424,7 +1463,10 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.5</c:v>
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1446,9 +1488,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$P$3:$P$8</c:f>
+              <c:f>Sheet1!$P$3:$P$9</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>Project Plan</c:v>
                 </c:pt>
@@ -1465,6 +1507,9 @@
                   <c:v>First Presentation</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>Second Presentation</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>Final Report</c:v>
                 </c:pt>
               </c:strCache>
@@ -1472,10 +1517,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$U$3:$U$8</c:f>
+              <c:f>Sheet1!$U$3:$U$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -1492,32 +1537,35 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16</c:v>
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="41940480"/>
-        <c:axId val="41942016"/>
+        <c:axId val="63063552"/>
+        <c:axId val="63065088"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="41940480"/>
+        <c:axId val="63063552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41942016"/>
+        <c:crossAx val="63065088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="41942016"/>
+        <c:axId val="63065088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1525,7 +1573,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41940480"/>
+        <c:crossAx val="63063552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1538,7 +1586,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1573,10 +1621,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.4664249736624841E-2"/>
-          <c:y val="0.10486619079157161"/>
-          <c:w val="0.81388711766905097"/>
-          <c:h val="0.80228243432187796"/>
+          <c:x val="4.4664249736624848E-2"/>
+          <c:y val="0.10486619079157163"/>
+          <c:w val="0.81388711766905109"/>
+          <c:h val="0.80228243432187807"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1598,6 +1646,89 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.6994978756276556E-2"/>
+                  <c:y val="2.2429906542056073E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showVal val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.0899961375048281E-3"/>
+                  <c:y val="-3.7383177570093455E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showVal val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.0899961375048563E-3"/>
+                  <c:y val="-3.4890965732087137E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showVal val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.1629972962533797E-2"/>
+                  <c:y val="-4.7352024922118381E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showVal val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="4"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.3174971031286212E-2"/>
+                  <c:y val="-3.7383177570093552E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showVal val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="2.2429906542056073E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showVal val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="6"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.6349942062572421E-3"/>
+                  <c:y val="2.2429906542056073E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showVal val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="7"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="9.2699884125144842E-3"/>
+                  <c:y val="-1.4953271028037384E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showVal val="1"/>
+            </c:dLbl>
+            <c:showVal val="1"/>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$J$37:$S$37</c:f>
@@ -1649,28 +1780,28 @@
                   <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>52</c:v>
+                  <c:v>53.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>67.5</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>106.5</c:v>
+                  <c:v>107.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>112.5</c:v>
+                  <c:v>113.25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>122</c:v>
+                  <c:v>123.75</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>149.25</c:v>
+                  <c:v>151</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>224</c:v>
+                  <c:v>225.75</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>261</c:v>
+                  <c:v>316</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1698,8 +1829,8 @@
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-1.3904982618771726E-2"/>
-                  <c:y val="-2.9906542056074768E-2"/>
+                  <c:x val="-1.3904982618771728E-2"/>
+                  <c:y val="-2.9906542056074778E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showVal val="1"/>
@@ -1709,7 +1840,17 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="-3.0899961375048281E-3"/>
-                  <c:y val="1.7445482866043614E-2"/>
+                  <c:y val="1.7445482866043617E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showVal val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.544998068752414E-3"/>
+                  <c:y val="9.9688473520249225E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:showVal val="1"/>
@@ -1718,8 +1859,8 @@
               <c:idx val="4"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="4.6349942062572421E-3"/>
-                  <c:y val="1.4953271028037384E-2"/>
+                  <c:x val="4.6349942062572404E-3"/>
+                  <c:y val="1.4953271028037387E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showVal val="1"/>
@@ -1728,8 +1869,8 @@
               <c:idx val="5"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-4.4804943993820005E-2"/>
-                  <c:y val="-3.4890965732087137E-2"/>
+                  <c:x val="-4.4804943993820019E-2"/>
+                  <c:y val="-3.4890965732087144E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showVal val="1"/>
@@ -1739,7 +1880,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="1.544998068752414E-3"/>
-                  <c:y val="1.4953271028037384E-2"/>
+                  <c:y val="1.4953271028037387E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showVal val="1"/>
@@ -1748,8 +1889,8 @@
               <c:idx val="7"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="6.1799922750096561E-3"/>
-                  <c:y val="7.4766355140186919E-3"/>
+                  <c:x val="6.179992275009657E-3"/>
+                  <c:y val="7.4766355140186936E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:showVal val="1"/>
@@ -1758,8 +1899,8 @@
               <c:idx val="8"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="4.6349942062572421E-3"/>
-                  <c:y val="2.2429906542056073E-2"/>
+                  <c:x val="4.6349942062572404E-3"/>
+                  <c:y val="2.242990654205608E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showVal val="1"/>
@@ -1845,24 +1986,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="65803008"/>
-        <c:axId val="65810816"/>
+        <c:axId val="63102976"/>
+        <c:axId val="63104512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="65803008"/>
+        <c:axId val="63102976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65810816"/>
+        <c:crossAx val="63104512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="65810816"/>
+        <c:axId val="63104512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1870,7 +2011,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65803008"/>
+        <c:crossAx val="63102976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1884,7 +2025,7 @@
           <c:x val="0.87588695948246509"/>
           <c:y val="0.42374979763043641"/>
           <c:w val="0.11185563500170241"/>
-          <c:h val="0.18982137513184683"/>
+          <c:h val="0.18982137513184685"/>
         </c:manualLayout>
       </c:layout>
     </c:legend>
@@ -1892,7 +2033,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1991,126 +2132,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-      <sheetName val="Sheet2"/>
-      <sheetName val="Sheet3"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="2">
-          <cell r="C2" t="str">
-            <v>Week 1</v>
-          </cell>
-          <cell r="D2" t="str">
-            <v>Week 2</v>
-          </cell>
-          <cell r="E2" t="str">
-            <v>Week 3</v>
-          </cell>
-          <cell r="F2" t="str">
-            <v>Week 4</v>
-          </cell>
-          <cell r="G2" t="str">
-            <v>Week 5</v>
-          </cell>
-          <cell r="H2" t="str">
-            <v>Week 6</v>
-          </cell>
-          <cell r="I2" t="str">
-            <v>Week 7 (11)</v>
-          </cell>
-          <cell r="J2" t="str">
-            <v>Week 8 (12)</v>
-          </cell>
-          <cell r="K2" t="str">
-            <v>Week 9 (13)</v>
-          </cell>
-          <cell r="L2" t="str">
-            <v>Week 10 (14)</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="B3" t="str">
-            <v>Actual time spent</v>
-          </cell>
-          <cell r="C3">
-            <v>19.5</v>
-          </cell>
-          <cell r="D3">
-            <v>26</v>
-          </cell>
-          <cell r="E3">
-            <v>52</v>
-          </cell>
-          <cell r="F3">
-            <v>67.5</v>
-          </cell>
-          <cell r="G3">
-            <v>106.5</v>
-          </cell>
-          <cell r="H3">
-            <v>112.5</v>
-          </cell>
-          <cell r="I3">
-            <v>122</v>
-          </cell>
-          <cell r="J3">
-            <v>149.25</v>
-          </cell>
-          <cell r="K3">
-            <v>224</v>
-          </cell>
-          <cell r="L3">
-            <v>248.25</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="B4" t="str">
-            <v>Expected time spent</v>
-          </cell>
-          <cell r="C4">
-            <v>21</v>
-          </cell>
-          <cell r="D4">
-            <v>21.5</v>
-          </cell>
-          <cell r="E4">
-            <v>33</v>
-          </cell>
-          <cell r="F4">
-            <v>66</v>
-          </cell>
-          <cell r="G4">
-            <v>97</v>
-          </cell>
-          <cell r="H4">
-            <v>119</v>
-          </cell>
-          <cell r="I4">
-            <v>276</v>
-          </cell>
-          <cell r="J4">
-            <v>314</v>
-          </cell>
-          <cell r="K4">
-            <v>347</v>
-          </cell>
-          <cell r="L4">
-            <v>356</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2400,8 +2421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D43" workbookViewId="0">
-      <selection activeCell="S47" sqref="S47"/>
+    <sheetView tabSelected="1" topLeftCell="D37" workbookViewId="0">
+      <selection activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2466,19 +2487,19 @@
       <c r="I3" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="35">
+      <c r="J3" s="63">
         <v>5</v>
       </c>
-      <c r="K3" s="35">
+      <c r="K3" s="62">
         <v>5</v>
       </c>
-      <c r="L3" s="35">
+      <c r="L3" s="62">
         <v>3.5</v>
       </c>
-      <c r="M3" s="35">
+      <c r="M3" s="62">
         <v>3</v>
       </c>
-      <c r="N3" s="35">
+      <c r="N3" s="62">
         <v>3</v>
       </c>
       <c r="O3">
@@ -2506,28 +2527,28 @@
     </row>
     <row r="4" spans="1:21" ht="17.25" thickBot="1">
       <c r="A4" s="9"/>
-      <c r="B4" s="52"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="54"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="49"/>
       <c r="I4" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="41">
+      <c r="J4" s="60">
         <v>1</v>
       </c>
-      <c r="K4" s="41">
+      <c r="K4" s="61">
         <v>1.5</v>
       </c>
-      <c r="L4" s="41">
+      <c r="L4" s="62">
         <v>1</v>
       </c>
-      <c r="M4" s="41">
+      <c r="M4" s="62">
         <v>2</v>
       </c>
-      <c r="N4" s="41">
+      <c r="N4" s="62">
         <v>1</v>
       </c>
       <c r="O4">
@@ -2538,7 +2559,7 @@
         <v>15</v>
       </c>
       <c r="Q4" s="39">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="R4" s="30">
         <v>4.5</v>
@@ -2564,36 +2585,36 @@
       <c r="I5" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="41">
+      <c r="J5" s="60">
         <v>7</v>
       </c>
-      <c r="K5" s="41">
+      <c r="K5" s="61">
         <v>3</v>
       </c>
-      <c r="L5" s="41">
+      <c r="L5" s="62">
         <v>2</v>
       </c>
-      <c r="M5" s="41">
-        <v>8.75</v>
-      </c>
-      <c r="N5" s="41">
+      <c r="M5" s="62">
+        <v>10.25</v>
+      </c>
+      <c r="N5" s="62">
         <v>5.25</v>
       </c>
       <c r="O5">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>27.5</v>
       </c>
       <c r="P5" s="34" t="s">
         <v>17</v>
       </c>
       <c r="Q5" s="40">
-        <v>35.5</v>
+        <v>36.25</v>
       </c>
       <c r="R5" s="27">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S5" s="28">
-        <v>23.5</v>
+        <v>24.5</v>
       </c>
       <c r="T5" s="28">
         <v>19.5</v>
@@ -2613,19 +2634,19 @@
       <c r="I6" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="41">
+      <c r="J6" s="60">
         <v>1</v>
       </c>
-      <c r="K6" s="41">
+      <c r="K6" s="61">
         <v>7</v>
       </c>
-      <c r="L6" s="41">
+      <c r="L6" s="62">
         <v>1.5</v>
       </c>
-      <c r="M6" s="41">
+      <c r="M6" s="62">
         <v>2.5</v>
       </c>
-      <c r="N6" s="41">
+      <c r="N6" s="62">
         <v>3.5</v>
       </c>
       <c r="O6">
@@ -2638,9 +2659,11 @@
       <c r="Q6" s="40">
         <v>3</v>
       </c>
-      <c r="R6" s="27"/>
+      <c r="R6" s="27">
+        <v>4</v>
+      </c>
       <c r="S6" s="28">
-        <v>1.25</v>
+        <v>1.75</v>
       </c>
       <c r="T6" s="28">
         <v>6</v>
@@ -2660,24 +2683,24 @@
       <c r="I7" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="41">
+      <c r="J7" s="63">
         <v>11</v>
       </c>
-      <c r="K7" s="41">
+      <c r="K7" s="62">
         <v>7</v>
       </c>
-      <c r="L7" s="41">
+      <c r="L7" s="62">
         <v>6</v>
       </c>
-      <c r="M7" s="41">
+      <c r="M7" s="62">
         <v>7.75</v>
       </c>
-      <c r="N7" s="41">
-        <v>7.25</v>
+      <c r="N7" s="62">
+        <v>6.5</v>
       </c>
       <c r="O7">
         <f t="shared" si="0"/>
-        <v>39</v>
+        <v>38.25</v>
       </c>
       <c r="P7" s="34" t="s">
         <v>16</v>
@@ -2709,40 +2732,42 @@
       <c r="I8" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="J8" s="41">
+      <c r="J8" s="60">
         <v>0</v>
       </c>
-      <c r="K8" s="41">
+      <c r="K8" s="61">
         <v>0</v>
       </c>
-      <c r="L8" s="41">
+      <c r="L8" s="62">
         <v>6</v>
       </c>
-      <c r="M8" s="41">
+      <c r="M8" s="62">
         <v>0</v>
       </c>
-      <c r="N8" s="41">
+      <c r="N8" s="62">
         <v>0</v>
       </c>
       <c r="O8">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="P8" s="34" t="s">
-        <v>19</v>
+      <c r="P8" s="59" t="s">
+        <v>35</v>
       </c>
       <c r="Q8" s="40">
-        <v>5.75</v>
-      </c>
-      <c r="R8" s="27"/>
+        <v>6</v>
+      </c>
+      <c r="R8" s="27">
+        <v>6</v>
+      </c>
       <c r="S8" s="28">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="T8" s="28">
-        <v>8.5</v>
+        <v>6</v>
       </c>
       <c r="U8" s="28">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:21" ht="17.25" thickBot="1">
@@ -2756,24 +2781,42 @@
       <c r="I9" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="35">
+      <c r="J9" s="60">
         <v>0</v>
       </c>
-      <c r="K9" s="41">
+      <c r="K9" s="61">
         <v>0</v>
       </c>
-      <c r="L9" s="41">
+      <c r="L9" s="62">
         <v>6</v>
       </c>
-      <c r="M9" s="41">
+      <c r="M9" s="62">
         <v>3.5</v>
       </c>
-      <c r="N9" s="41">
-        <v>0</v>
+      <c r="N9" s="62">
+        <v>1</v>
       </c>
       <c r="O9">
         <f t="shared" si="0"/>
-        <v>9.5</v>
+        <v>10.5</v>
+      </c>
+      <c r="P9" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q9" s="40">
+        <v>7.75</v>
+      </c>
+      <c r="R9" s="27">
+        <v>0</v>
+      </c>
+      <c r="S9" s="28">
+        <v>8.5</v>
+      </c>
+      <c r="T9" s="28">
+        <v>19.75</v>
+      </c>
+      <c r="U9" s="28">
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="17.25" thickBot="1">
@@ -2787,19 +2830,19 @@
       <c r="I10" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="J10" s="35">
+      <c r="J10" s="60">
         <v>12.25</v>
       </c>
-      <c r="K10" s="35">
+      <c r="K10" s="61">
         <v>0</v>
       </c>
-      <c r="L10" s="35">
+      <c r="L10" s="62">
         <v>2</v>
       </c>
-      <c r="M10" s="35">
+      <c r="M10" s="62">
         <v>5</v>
       </c>
-      <c r="N10" s="35">
+      <c r="N10" s="62">
         <v>8</v>
       </c>
       <c r="O10">
@@ -2809,28 +2852,28 @@
     </row>
     <row r="11" spans="1:21" ht="17.25" thickBot="1">
       <c r="A11" s="20"/>
-      <c r="B11" s="49"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="50"/>
-      <c r="F11" s="50"/>
-      <c r="G11" s="51"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="46"/>
       <c r="I11" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="J11" s="42">
+      <c r="J11" s="60">
         <v>22</v>
       </c>
-      <c r="K11" s="42">
+      <c r="K11" s="61">
         <v>15</v>
       </c>
-      <c r="L11" s="35">
+      <c r="L11" s="62">
         <v>12.5</v>
       </c>
-      <c r="M11" s="35">
+      <c r="M11" s="62">
         <v>9</v>
       </c>
-      <c r="N11" s="35">
+      <c r="N11" s="62">
         <v>16.25</v>
       </c>
       <c r="O11">
@@ -2849,24 +2892,24 @@
       <c r="I12" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="J12" s="43">
-        <v>11.75</v>
-      </c>
-      <c r="K12" s="44">
-        <v>0</v>
-      </c>
-      <c r="L12" s="45">
-        <v>10.5</v>
-      </c>
-      <c r="M12" s="45">
-        <v>8.5</v>
-      </c>
-      <c r="N12" s="45">
-        <v>6.25</v>
+      <c r="J12" s="60">
+        <v>22.75</v>
+      </c>
+      <c r="K12" s="61">
+        <v>11</v>
+      </c>
+      <c r="L12" s="62">
+        <v>18.5</v>
+      </c>
+      <c r="M12" s="62">
+        <v>25.75</v>
+      </c>
+      <c r="N12" s="62">
+        <v>12.25</v>
       </c>
       <c r="O12">
         <f>SUM(J12:N12)</f>
-        <v>37</v>
+        <v>90.25</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="17.25" thickBot="1">
@@ -2907,12 +2950,12 @@
     </row>
     <row r="17" spans="1:7" ht="17.25" thickBot="1">
       <c r="A17" s="20"/>
-      <c r="B17" s="49"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="50"/>
-      <c r="E17" s="50"/>
-      <c r="F17" s="50"/>
-      <c r="G17" s="51"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="46"/>
     </row>
     <row r="18" spans="1:7" ht="17.25" thickBot="1">
       <c r="A18" s="14"/>
@@ -2961,12 +3004,12 @@
     </row>
     <row r="23" spans="1:7" ht="17.25" thickBot="1">
       <c r="A23" s="20"/>
-      <c r="B23" s="49"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="50"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="50"/>
-      <c r="G23" s="51"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="46"/>
     </row>
     <row r="24" spans="1:7" ht="17.25" thickBot="1">
       <c r="A24" s="14"/>
@@ -2997,12 +3040,12 @@
     </row>
     <row r="27" spans="1:7" ht="17.25" thickBot="1">
       <c r="A27" s="20"/>
-      <c r="B27" s="49"/>
-      <c r="C27" s="50"/>
-      <c r="D27" s="50"/>
-      <c r="E27" s="50"/>
-      <c r="F27" s="50"/>
-      <c r="G27" s="51"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="45"/>
+      <c r="D27" s="45"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="46"/>
     </row>
     <row r="28" spans="1:7" ht="17.25" thickBot="1">
       <c r="A28" s="14"/>
@@ -3024,12 +3067,12 @@
     </row>
     <row r="30" spans="1:7" ht="17.25" thickBot="1">
       <c r="A30" s="20"/>
-      <c r="B30" s="49"/>
-      <c r="C30" s="50"/>
-      <c r="D30" s="50"/>
-      <c r="E30" s="50"/>
-      <c r="F30" s="50"/>
-      <c r="G30" s="51"/>
+      <c r="B30" s="44"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="46"/>
     </row>
     <row r="31" spans="1:7" ht="17.25" thickBot="1">
       <c r="A31" s="14"/>
@@ -3084,43 +3127,43 @@
     </row>
     <row r="37" spans="1:19" ht="17.25" thickBot="1">
       <c r="A37" s="23"/>
-      <c r="B37" s="55"/>
-      <c r="C37" s="56"/>
-      <c r="D37" s="56"/>
-      <c r="E37" s="56"/>
-      <c r="F37" s="56"/>
-      <c r="G37" s="57"/>
+      <c r="B37" s="50"/>
+      <c r="C37" s="51"/>
+      <c r="D37" s="51"/>
+      <c r="E37" s="51"/>
+      <c r="F37" s="51"/>
+      <c r="G37" s="52"/>
       <c r="I37" t="s">
         <v>22</v>
       </c>
-      <c r="J37" s="61" t="s">
+      <c r="J37" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="K37" s="61" t="s">
+      <c r="K37" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="L37" s="61" t="s">
+      <c r="L37" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="M37" s="61" t="s">
+      <c r="M37" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="N37" s="61" t="s">
+      <c r="N37" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="O37" s="61" t="s">
+      <c r="O37" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="P37" s="61" t="s">
+      <c r="P37" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="Q37" s="61" t="s">
+      <c r="Q37" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="R37" s="61" t="s">
+      <c r="R37" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="S37" s="61" t="s">
+      <c r="S37" s="41" t="s">
         <v>32</v>
       </c>
     </row>
@@ -3135,90 +3178,90 @@
       <c r="I38" t="s">
         <v>33</v>
       </c>
-      <c r="J38" s="62">
+      <c r="J38" s="42">
         <v>19.5</v>
       </c>
-      <c r="K38" s="62">
+      <c r="K38" s="42">
         <f>19.5+6.5</f>
         <v>26</v>
       </c>
-      <c r="L38" s="62">
-        <f>26+26</f>
-        <v>52</v>
-      </c>
-      <c r="M38" s="62">
-        <f>52+15.5</f>
-        <v>67.5</v>
-      </c>
-      <c r="N38" s="62">
-        <f>67.5+39</f>
-        <v>106.5</v>
-      </c>
-      <c r="O38" s="62">
-        <f>106.5+6</f>
-        <v>112.5</v>
-      </c>
-      <c r="P38" s="62">
-        <f>112.5+9.5</f>
-        <v>122</v>
-      </c>
-      <c r="Q38" s="62">
-        <f>122+27.25</f>
-        <v>149.25</v>
-      </c>
-      <c r="R38" s="62">
-        <f>149.25+74.75</f>
-        <v>224</v>
-      </c>
-      <c r="S38" s="62">
-        <f>224+37</f>
-        <v>261</v>
+      <c r="L38" s="42">
+        <f>26+27.5</f>
+        <v>53.5</v>
+      </c>
+      <c r="M38" s="42">
+        <f>53.5+15.5</f>
+        <v>69</v>
+      </c>
+      <c r="N38" s="42">
+        <f>69+38.25</f>
+        <v>107.25</v>
+      </c>
+      <c r="O38" s="42">
+        <f>107.25+6</f>
+        <v>113.25</v>
+      </c>
+      <c r="P38" s="42">
+        <f>113.25+10.5</f>
+        <v>123.75</v>
+      </c>
+      <c r="Q38" s="42">
+        <f>123.75+27.25</f>
+        <v>151</v>
+      </c>
+      <c r="R38" s="42">
+        <f>151+74.75</f>
+        <v>225.75</v>
+      </c>
+      <c r="S38" s="42">
+        <f>225.75+90.25</f>
+        <v>316</v>
       </c>
     </row>
     <row r="39" spans="1:19" ht="17.25" thickBot="1">
       <c r="A39" s="20"/>
-      <c r="B39" s="49"/>
-      <c r="C39" s="50"/>
-      <c r="D39" s="50"/>
-      <c r="E39" s="50"/>
-      <c r="F39" s="50"/>
-      <c r="G39" s="51"/>
+      <c r="B39" s="44"/>
+      <c r="C39" s="45"/>
+      <c r="D39" s="45"/>
+      <c r="E39" s="45"/>
+      <c r="F39" s="45"/>
+      <c r="G39" s="46"/>
       <c r="I39" t="s">
         <v>34</v>
       </c>
-      <c r="J39" s="62">
+      <c r="J39" s="42">
         <v>21</v>
       </c>
-      <c r="K39" s="63">
+      <c r="K39" s="43">
         <v>21.5</v>
       </c>
-      <c r="L39" s="62">
+      <c r="L39" s="42">
         <v>33</v>
       </c>
-      <c r="M39" s="62">
+      <c r="M39" s="42">
         <v>66</v>
       </c>
-      <c r="N39" s="62">
+      <c r="N39" s="42">
         <f>66+31</f>
         <v>97</v>
       </c>
-      <c r="O39" s="62">
+      <c r="O39" s="42">
         <f>97+22</f>
         <v>119</v>
       </c>
-      <c r="P39" s="62">
+      <c r="P39" s="42">
         <f>119+19+19+46+46+27</f>
         <v>276</v>
       </c>
-      <c r="Q39" s="62">
+      <c r="Q39" s="42">
         <f>276+38</f>
         <v>314</v>
       </c>
-      <c r="R39" s="62">
+      <c r="R39" s="42">
         <f>314+33</f>
         <v>347</v>
       </c>
-      <c r="S39" s="62">
+      <c r="S39" s="42">
         <f>347+9</f>
         <v>356</v>
       </c>
@@ -3243,12 +3286,12 @@
     </row>
     <row r="42" spans="1:19" ht="17.25" thickBot="1">
       <c r="A42" s="20"/>
-      <c r="B42" s="58"/>
-      <c r="C42" s="59"/>
-      <c r="D42" s="59"/>
-      <c r="E42" s="59"/>
-      <c r="F42" s="59"/>
-      <c r="G42" s="60"/>
+      <c r="B42" s="53"/>
+      <c r="C42" s="54"/>
+      <c r="D42" s="54"/>
+      <c r="E42" s="54"/>
+      <c r="F42" s="54"/>
+      <c r="G42" s="55"/>
     </row>
     <row r="43" spans="1:19" ht="17.25" thickBot="1">
       <c r="A43" s="14"/>
@@ -3288,12 +3331,12 @@
     </row>
     <row r="47" spans="1:19" ht="17.25" thickBot="1">
       <c r="A47" s="20"/>
-      <c r="B47" s="49"/>
-      <c r="C47" s="50"/>
-      <c r="D47" s="50"/>
-      <c r="E47" s="50"/>
-      <c r="F47" s="50"/>
-      <c r="G47" s="51"/>
+      <c r="B47" s="44"/>
+      <c r="C47" s="45"/>
+      <c r="D47" s="45"/>
+      <c r="E47" s="45"/>
+      <c r="F47" s="45"/>
+      <c r="G47" s="46"/>
     </row>
     <row r="48" spans="1:19" ht="17.25" thickBot="1">
       <c r="A48" s="14"/>
@@ -3324,12 +3367,12 @@
     </row>
     <row r="51" spans="1:7" ht="17.25" thickBot="1">
       <c r="A51" s="20"/>
-      <c r="B51" s="49"/>
-      <c r="C51" s="50"/>
-      <c r="D51" s="50"/>
-      <c r="E51" s="50"/>
-      <c r="F51" s="50"/>
-      <c r="G51" s="51"/>
+      <c r="B51" s="44"/>
+      <c r="C51" s="45"/>
+      <c r="D51" s="45"/>
+      <c r="E51" s="45"/>
+      <c r="F51" s="45"/>
+      <c r="G51" s="46"/>
     </row>
     <row r="52" spans="1:7" ht="17.25" thickBot="1">
       <c r="A52" s="14"/>
@@ -3360,12 +3403,12 @@
     </row>
     <row r="55" spans="1:7" ht="17.25" thickBot="1">
       <c r="A55" s="20"/>
-      <c r="B55" s="49"/>
-      <c r="C55" s="50"/>
-      <c r="D55" s="50"/>
-      <c r="E55" s="50"/>
-      <c r="F55" s="50"/>
-      <c r="G55" s="51"/>
+      <c r="B55" s="44"/>
+      <c r="C55" s="45"/>
+      <c r="D55" s="45"/>
+      <c r="E55" s="45"/>
+      <c r="F55" s="45"/>
+      <c r="G55" s="46"/>
     </row>
     <row r="56" spans="1:7" ht="17.25" thickBot="1">
       <c r="A56" s="14"/>
@@ -3396,12 +3439,12 @@
     </row>
     <row r="59" spans="1:7" ht="17.25" thickBot="1">
       <c r="A59" s="20"/>
-      <c r="B59" s="49"/>
-      <c r="C59" s="50"/>
-      <c r="D59" s="50"/>
-      <c r="E59" s="50"/>
-      <c r="F59" s="50"/>
-      <c r="G59" s="51"/>
+      <c r="B59" s="44"/>
+      <c r="C59" s="45"/>
+      <c r="D59" s="45"/>
+      <c r="E59" s="45"/>
+      <c r="F59" s="45"/>
+      <c r="G59" s="46"/>
     </row>
     <row r="60" spans="1:7" ht="17.25" thickBot="1">
       <c r="A60" s="14"/>
@@ -3441,12 +3484,12 @@
     </row>
     <row r="64" spans="1:7" ht="17.25" thickBot="1">
       <c r="A64" s="20"/>
-      <c r="B64" s="49"/>
-      <c r="C64" s="50"/>
-      <c r="D64" s="50"/>
-      <c r="E64" s="50"/>
-      <c r="F64" s="50"/>
-      <c r="G64" s="51"/>
+      <c r="B64" s="44"/>
+      <c r="C64" s="45"/>
+      <c r="D64" s="45"/>
+      <c r="E64" s="45"/>
+      <c r="F64" s="45"/>
+      <c r="G64" s="46"/>
     </row>
     <row r="65" spans="1:7" ht="17.25" thickBot="1">
       <c r="A65" s="14"/>
@@ -3459,12 +3502,12 @@
     </row>
     <row r="66" spans="1:7" ht="17.25" thickBot="1">
       <c r="A66" s="20"/>
-      <c r="B66" s="49"/>
-      <c r="C66" s="50"/>
-      <c r="D66" s="50"/>
-      <c r="E66" s="50"/>
-      <c r="F66" s="50"/>
-      <c r="G66" s="51"/>
+      <c r="B66" s="44"/>
+      <c r="C66" s="45"/>
+      <c r="D66" s="45"/>
+      <c r="E66" s="45"/>
+      <c r="F66" s="45"/>
+      <c r="G66" s="46"/>
     </row>
     <row r="67" spans="1:7" ht="17.25" thickBot="1">
       <c r="A67" s="14"/>
@@ -3486,12 +3529,12 @@
     </row>
     <row r="69" spans="1:7" ht="17.25" thickBot="1">
       <c r="A69" s="20"/>
-      <c r="B69" s="49"/>
-      <c r="C69" s="50"/>
-      <c r="D69" s="50"/>
-      <c r="E69" s="50"/>
-      <c r="F69" s="50"/>
-      <c r="G69" s="51"/>
+      <c r="B69" s="44"/>
+      <c r="C69" s="45"/>
+      <c r="D69" s="45"/>
+      <c r="E69" s="45"/>
+      <c r="F69" s="45"/>
+      <c r="G69" s="46"/>
     </row>
     <row r="70" spans="1:7" ht="17.25" thickBot="1">
       <c r="A70" s="14"/>
@@ -3540,12 +3583,12 @@
     </row>
     <row r="75" spans="1:7" ht="17.25" thickBot="1">
       <c r="A75" s="20"/>
-      <c r="B75" s="49"/>
-      <c r="C75" s="50"/>
-      <c r="D75" s="50"/>
-      <c r="E75" s="50"/>
-      <c r="F75" s="50"/>
-      <c r="G75" s="51"/>
+      <c r="B75" s="44"/>
+      <c r="C75" s="45"/>
+      <c r="D75" s="45"/>
+      <c r="E75" s="45"/>
+      <c r="F75" s="45"/>
+      <c r="G75" s="46"/>
     </row>
     <row r="76" spans="1:7" ht="17.25" thickBot="1">
       <c r="A76" s="14"/>
@@ -3567,12 +3610,12 @@
     </row>
     <row r="78" spans="1:7" ht="17.25" thickBot="1">
       <c r="A78" s="20"/>
-      <c r="B78" s="49"/>
-      <c r="C78" s="50"/>
-      <c r="D78" s="50"/>
-      <c r="E78" s="50"/>
-      <c r="F78" s="50"/>
-      <c r="G78" s="51"/>
+      <c r="B78" s="44"/>
+      <c r="C78" s="45"/>
+      <c r="D78" s="45"/>
+      <c r="E78" s="45"/>
+      <c r="F78" s="45"/>
+      <c r="G78" s="46"/>
     </row>
     <row r="79" spans="1:7" ht="17.25" thickBot="1">
       <c r="A79" s="14"/>
@@ -3612,12 +3655,12 @@
     </row>
     <row r="83" spans="1:7" ht="17.25" thickBot="1">
       <c r="A83" s="25"/>
-      <c r="B83" s="46"/>
-      <c r="C83" s="47"/>
-      <c r="D83" s="47"/>
-      <c r="E83" s="47"/>
-      <c r="F83" s="47"/>
-      <c r="G83" s="48"/>
+      <c r="B83" s="56"/>
+      <c r="C83" s="57"/>
+      <c r="D83" s="57"/>
+      <c r="E83" s="57"/>
+      <c r="F83" s="57"/>
+      <c r="G83" s="58"/>
     </row>
     <row r="84" spans="1:7" ht="17.25" thickBot="1">
       <c r="A84" s="9"/>
@@ -3678,6 +3721,13 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B83:G83"/>
+    <mergeCell ref="B59:G59"/>
+    <mergeCell ref="B64:G64"/>
+    <mergeCell ref="B66:G66"/>
+    <mergeCell ref="B69:G69"/>
+    <mergeCell ref="B75:G75"/>
+    <mergeCell ref="B78:G78"/>
     <mergeCell ref="B55:G55"/>
     <mergeCell ref="B4:G4"/>
     <mergeCell ref="B11:G11"/>
@@ -3690,13 +3740,6 @@
     <mergeCell ref="B42:G42"/>
     <mergeCell ref="B47:G47"/>
     <mergeCell ref="B51:G51"/>
-    <mergeCell ref="B83:G83"/>
-    <mergeCell ref="B59:G59"/>
-    <mergeCell ref="B64:G64"/>
-    <mergeCell ref="B66:G66"/>
-    <mergeCell ref="B69:G69"/>
-    <mergeCell ref="B75:G75"/>
-    <mergeCell ref="B78:G78"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
* Updated Graphs.xlsx, Time Management Account.docx and Time spent per member per week and activity_2PageVersion.docx
</commit_message>
<xml_diff>
--- a/doc/End of Project Report/Graphs.xlsx
+++ b/doc/End of Project Report/Graphs.xlsx
@@ -511,6 +511,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -546,30 +570,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -694,13 +694,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12.25</c:v>
+                  <c:v>13.25</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>22.75</c:v>
+                  <c:v>24.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -789,13 +789,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11</c:v>
+                  <c:v>15.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -884,13 +884,13 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>18.5</c:v>
+                  <c:v>20.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -979,13 +979,13 @@
                   <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>25.75</c:v>
+                  <c:v>27.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1085,37 +1085,37 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>16.25</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12.25</c:v>
+                  <c:v>15.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="57901440"/>
-        <c:axId val="57902976"/>
+        <c:axId val="53223808"/>
+        <c:axId val="53225344"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="57901440"/>
+        <c:axId val="53223808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57902976"/>
+        <c:crossAx val="53225344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="57902976"/>
+        <c:axId val="53225344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1123,7 +1123,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0_);\(#,##0\)" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57901440"/>
+        <c:crossAx val="53223808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1136,7 +1136,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1235,7 +1235,7 @@
                   <c:v>36.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>6</c:v>
@@ -1303,13 +1303,13 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>6</c:v>
@@ -1383,7 +1383,7 @@
                   <c:v>24.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.75</c:v>
+                  <c:v>4.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>6</c:v>
@@ -1457,7 +1457,7 @@
                   <c:v>19.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>6</c:v>
@@ -1531,7 +1531,7 @@
                   <c:v>18.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>6</c:v>
@@ -1540,32 +1540,32 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:shape val="box"/>
-        <c:axId val="63063552"/>
-        <c:axId val="63065088"/>
+        <c:axId val="53278208"/>
+        <c:axId val="53279744"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="63063552"/>
+        <c:axId val="53278208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63065088"/>
+        <c:crossAx val="53279744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63065088"/>
+        <c:axId val="53279744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1573,7 +1573,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63063552"/>
+        <c:crossAx val="53278208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1586,7 +1586,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1621,10 +1621,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.4664249736624848E-2"/>
-          <c:y val="0.10486619079157163"/>
-          <c:w val="0.81388711766905109"/>
-          <c:h val="0.80228243432187807"/>
+          <c:x val="4.4664249736624854E-2"/>
+          <c:y val="0.10486619079157164"/>
+          <c:w val="0.8138871176690512"/>
+          <c:h val="0.80228243432187818"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1651,8 +1651,8 @@
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-1.6994978756276556E-2"/>
-                  <c:y val="2.2429906542056073E-2"/>
+                  <c:x val="-1.699497875627656E-2"/>
+                  <c:y val="2.242990654205608E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showVal val="1"/>
@@ -1662,7 +1662,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="-3.0899961375048281E-3"/>
-                  <c:y val="-3.7383177570093455E-2"/>
+                  <c:y val="-3.7383177570093469E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showVal val="1"/>
@@ -1671,8 +1671,8 @@
               <c:idx val="2"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-3.0899961375048563E-3"/>
-                  <c:y val="-3.4890965732087137E-2"/>
+                  <c:x val="-3.0899961375048571E-3"/>
+                  <c:y val="-3.4890965732087144E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showVal val="1"/>
@@ -1681,8 +1681,8 @@
               <c:idx val="3"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-2.1629972962533797E-2"/>
-                  <c:y val="-4.7352024922118381E-2"/>
+                  <c:x val="-2.1629972962533807E-2"/>
+                  <c:y val="-4.7352024922118409E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showVal val="1"/>
@@ -1691,8 +1691,8 @@
               <c:idx val="4"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-2.3174971031286212E-2"/>
-                  <c:y val="-3.7383177570093552E-2"/>
+                  <c:x val="-2.3174971031286205E-2"/>
+                  <c:y val="-3.7383177570093566E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showVal val="1"/>
@@ -1702,7 +1702,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="0"/>
-                  <c:y val="2.2429906542056073E-2"/>
+                  <c:y val="2.242990654205608E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showVal val="1"/>
@@ -1711,8 +1711,8 @@
               <c:idx val="6"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="4.6349942062572421E-3"/>
-                  <c:y val="2.2429906542056073E-2"/>
+                  <c:x val="4.6349942062572404E-3"/>
+                  <c:y val="2.242990654205608E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showVal val="1"/>
@@ -1722,7 +1722,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="9.2699884125144842E-3"/>
-                  <c:y val="-1.4953271028037384E-2"/>
+                  <c:y val="-1.4953271028037387E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showVal val="1"/>
@@ -1795,13 +1795,13 @@
                   <c:v>123.75</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>151</c:v>
+                  <c:v>156</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>225.75</c:v>
+                  <c:v>230.75</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>316</c:v>
+                  <c:v>334.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1829,8 +1829,8 @@
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-1.3904982618771728E-2"/>
-                  <c:y val="-2.9906542056074778E-2"/>
+                  <c:x val="-1.390498261877173E-2"/>
+                  <c:y val="-2.9906542056074785E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showVal val="1"/>
@@ -1850,7 +1850,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="1.544998068752414E-3"/>
-                  <c:y val="9.9688473520249225E-3"/>
+                  <c:y val="9.9688473520249243E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:showVal val="1"/>
@@ -1859,8 +1859,8 @@
               <c:idx val="4"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="4.6349942062572404E-3"/>
-                  <c:y val="1.4953271028037387E-2"/>
+                  <c:x val="4.6349942062572386E-3"/>
+                  <c:y val="1.4953271028037389E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showVal val="1"/>
@@ -1869,7 +1869,7 @@
               <c:idx val="5"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-4.4804943993820019E-2"/>
+                  <c:x val="-4.4804943993820026E-2"/>
                   <c:y val="-3.4890965732087144E-2"/>
                 </c:manualLayout>
               </c:layout>
@@ -1880,7 +1880,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="1.544998068752414E-3"/>
-                  <c:y val="1.4953271028037387E-2"/>
+                  <c:y val="1.4953271028037389E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showVal val="1"/>
@@ -1889,8 +1889,8 @@
               <c:idx val="7"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="6.179992275009657E-3"/>
-                  <c:y val="7.4766355140186936E-3"/>
+                  <c:x val="6.1799922750096579E-3"/>
+                  <c:y val="7.4766355140186954E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:showVal val="1"/>
@@ -1899,8 +1899,8 @@
               <c:idx val="8"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="4.6349942062572404E-3"/>
-                  <c:y val="2.242990654205608E-2"/>
+                  <c:x val="4.6349942062572386E-3"/>
+                  <c:y val="2.2429906542056084E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showVal val="1"/>
@@ -1986,24 +1986,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="63102976"/>
-        <c:axId val="63104512"/>
+        <c:axId val="54768000"/>
+        <c:axId val="54769536"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="63102976"/>
+        <c:axId val="54768000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63104512"/>
+        <c:crossAx val="54769536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63104512"/>
+        <c:axId val="54769536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2011,7 +2011,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63102976"/>
+        <c:crossAx val="54768000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2025,7 +2025,7 @@
           <c:x val="0.87588695948246509"/>
           <c:y val="0.42374979763043641"/>
           <c:w val="0.11185563500170241"/>
-          <c:h val="0.18982137513184685"/>
+          <c:h val="0.18982137513184688"/>
         </c:manualLayout>
       </c:layout>
     </c:legend>
@@ -2033,7 +2033,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2421,8 +2421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D37" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+    <sheetView tabSelected="1" topLeftCell="F34" workbookViewId="0">
+      <selection activeCell="T39" sqref="T39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2487,19 +2487,19 @@
       <c r="I3" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="63">
+      <c r="J3" s="48">
         <v>5</v>
       </c>
-      <c r="K3" s="62">
+      <c r="K3" s="47">
         <v>5</v>
       </c>
-      <c r="L3" s="62">
+      <c r="L3" s="47">
         <v>3.5</v>
       </c>
-      <c r="M3" s="62">
+      <c r="M3" s="47">
         <v>3</v>
       </c>
-      <c r="N3" s="62">
+      <c r="N3" s="47">
         <v>3</v>
       </c>
       <c r="O3">
@@ -2527,28 +2527,28 @@
     </row>
     <row r="4" spans="1:21" ht="17.25" thickBot="1">
       <c r="A4" s="9"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="48"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="49"/>
+      <c r="B4" s="55"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="57"/>
       <c r="I4" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="J4" s="60">
+      <c r="J4" s="45">
         <v>1</v>
       </c>
-      <c r="K4" s="61">
+      <c r="K4" s="46">
         <v>1.5</v>
       </c>
-      <c r="L4" s="62">
+      <c r="L4" s="47">
         <v>1</v>
       </c>
-      <c r="M4" s="62">
+      <c r="M4" s="47">
         <v>2</v>
       </c>
-      <c r="N4" s="62">
+      <c r="N4" s="47">
         <v>1</v>
       </c>
       <c r="O4">
@@ -2562,7 +2562,7 @@
         <v>18</v>
       </c>
       <c r="R4" s="30">
-        <v>4.5</v>
+        <v>7</v>
       </c>
       <c r="S4" s="31">
         <v>8.75</v>
@@ -2585,19 +2585,19 @@
       <c r="I5" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="J5" s="60">
+      <c r="J5" s="45">
         <v>7</v>
       </c>
-      <c r="K5" s="61">
+      <c r="K5" s="46">
         <v>3</v>
       </c>
-      <c r="L5" s="62">
+      <c r="L5" s="47">
         <v>2</v>
       </c>
-      <c r="M5" s="62">
+      <c r="M5" s="47">
         <v>10.25</v>
       </c>
-      <c r="N5" s="62">
+      <c r="N5" s="47">
         <v>5.25</v>
       </c>
       <c r="O5">
@@ -2634,19 +2634,19 @@
       <c r="I6" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="60">
+      <c r="J6" s="45">
         <v>1</v>
       </c>
-      <c r="K6" s="61">
+      <c r="K6" s="46">
         <v>7</v>
       </c>
-      <c r="L6" s="62">
+      <c r="L6" s="47">
         <v>1.5</v>
       </c>
-      <c r="M6" s="62">
+      <c r="M6" s="47">
         <v>2.5</v>
       </c>
-      <c r="N6" s="62">
+      <c r="N6" s="47">
         <v>3.5</v>
       </c>
       <c r="O6">
@@ -2657,19 +2657,19 @@
         <v>18</v>
       </c>
       <c r="Q6" s="40">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="R6" s="27">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="S6" s="28">
-        <v>1.75</v>
+        <v>4.75</v>
       </c>
       <c r="T6" s="28">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="U6" s="28">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="17.25" thickBot="1">
@@ -2683,19 +2683,19 @@
       <c r="I7" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="63">
+      <c r="J7" s="48">
         <v>11</v>
       </c>
-      <c r="K7" s="62">
+      <c r="K7" s="47">
         <v>7</v>
       </c>
-      <c r="L7" s="62">
+      <c r="L7" s="47">
         <v>6</v>
       </c>
-      <c r="M7" s="62">
+      <c r="M7" s="47">
         <v>7.75</v>
       </c>
-      <c r="N7" s="62">
+      <c r="N7" s="47">
         <v>6.5</v>
       </c>
       <c r="O7">
@@ -2732,26 +2732,26 @@
       <c r="I8" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="J8" s="60">
+      <c r="J8" s="45">
         <v>0</v>
       </c>
-      <c r="K8" s="61">
+      <c r="K8" s="46">
         <v>0</v>
       </c>
-      <c r="L8" s="62">
+      <c r="L8" s="47">
         <v>6</v>
       </c>
-      <c r="M8" s="62">
+      <c r="M8" s="47">
         <v>0</v>
       </c>
-      <c r="N8" s="62">
+      <c r="N8" s="47">
         <v>0</v>
       </c>
       <c r="O8">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="P8" s="59" t="s">
+      <c r="P8" s="44" t="s">
         <v>35</v>
       </c>
       <c r="Q8" s="40">
@@ -2781,19 +2781,19 @@
       <c r="I9" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="60">
+      <c r="J9" s="45">
         <v>0</v>
       </c>
-      <c r="K9" s="61">
+      <c r="K9" s="46">
         <v>0</v>
       </c>
-      <c r="L9" s="62">
+      <c r="L9" s="47">
         <v>6</v>
       </c>
-      <c r="M9" s="62">
+      <c r="M9" s="47">
         <v>3.5</v>
       </c>
-      <c r="N9" s="62">
+      <c r="N9" s="47">
         <v>1</v>
       </c>
       <c r="O9">
@@ -2816,7 +2816,7 @@
         <v>19.75</v>
       </c>
       <c r="U9" s="28">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="17.25" thickBot="1">
@@ -2830,50 +2830,50 @@
       <c r="I10" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="J10" s="60">
-        <v>12.25</v>
-      </c>
-      <c r="K10" s="61">
-        <v>0</v>
-      </c>
-      <c r="L10" s="62">
-        <v>2</v>
-      </c>
-      <c r="M10" s="62">
-        <v>5</v>
-      </c>
-      <c r="N10" s="62">
-        <v>8</v>
+      <c r="J10" s="45">
+        <v>13.25</v>
+      </c>
+      <c r="K10" s="46">
+        <v>1</v>
+      </c>
+      <c r="L10" s="47">
+        <v>3</v>
+      </c>
+      <c r="M10" s="47">
+        <v>6</v>
+      </c>
+      <c r="N10" s="47">
+        <v>9</v>
       </c>
       <c r="O10">
         <f t="shared" si="0"/>
-        <v>27.25</v>
+        <v>32.25</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="17.25" thickBot="1">
       <c r="A11" s="20"/>
-      <c r="B11" s="44"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="46"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="54"/>
       <c r="I11" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="J11" s="60">
+      <c r="J11" s="45">
         <v>22</v>
       </c>
-      <c r="K11" s="61">
+      <c r="K11" s="46">
         <v>15</v>
       </c>
-      <c r="L11" s="62">
+      <c r="L11" s="47">
         <v>12.5</v>
       </c>
-      <c r="M11" s="62">
+      <c r="M11" s="47">
         <v>9</v>
       </c>
-      <c r="N11" s="62">
+      <c r="N11" s="47">
         <v>16.25</v>
       </c>
       <c r="O11">
@@ -2892,24 +2892,24 @@
       <c r="I12" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="J12" s="60">
-        <v>22.75</v>
-      </c>
-      <c r="K12" s="61">
-        <v>11</v>
-      </c>
-      <c r="L12" s="62">
-        <v>18.5</v>
-      </c>
-      <c r="M12" s="62">
-        <v>25.75</v>
-      </c>
-      <c r="N12" s="62">
-        <v>12.25</v>
+      <c r="J12" s="45">
+        <v>24.75</v>
+      </c>
+      <c r="K12" s="46">
+        <v>15.5</v>
+      </c>
+      <c r="L12" s="47">
+        <v>20.5</v>
+      </c>
+      <c r="M12" s="47">
+        <v>27.75</v>
+      </c>
+      <c r="N12" s="47">
+        <v>15.25</v>
       </c>
       <c r="O12">
         <f>SUM(J12:N12)</f>
-        <v>90.25</v>
+        <v>103.75</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="17.25" thickBot="1">
@@ -2950,12 +2950,12 @@
     </row>
     <row r="17" spans="1:7" ht="17.25" thickBot="1">
       <c r="A17" s="20"/>
-      <c r="B17" s="44"/>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="46"/>
+      <c r="B17" s="52"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="54"/>
     </row>
     <row r="18" spans="1:7" ht="17.25" thickBot="1">
       <c r="A18" s="14"/>
@@ -3004,12 +3004,12 @@
     </row>
     <row r="23" spans="1:7" ht="17.25" thickBot="1">
       <c r="A23" s="20"/>
-      <c r="B23" s="44"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="45"/>
-      <c r="G23" s="46"/>
+      <c r="B23" s="52"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="54"/>
     </row>
     <row r="24" spans="1:7" ht="17.25" thickBot="1">
       <c r="A24" s="14"/>
@@ -3040,12 +3040,12 @@
     </row>
     <row r="27" spans="1:7" ht="17.25" thickBot="1">
       <c r="A27" s="20"/>
-      <c r="B27" s="44"/>
-      <c r="C27" s="45"/>
-      <c r="D27" s="45"/>
-      <c r="E27" s="45"/>
-      <c r="F27" s="45"/>
-      <c r="G27" s="46"/>
+      <c r="B27" s="52"/>
+      <c r="C27" s="53"/>
+      <c r="D27" s="53"/>
+      <c r="E27" s="53"/>
+      <c r="F27" s="53"/>
+      <c r="G27" s="54"/>
     </row>
     <row r="28" spans="1:7" ht="17.25" thickBot="1">
       <c r="A28" s="14"/>
@@ -3067,12 +3067,12 @@
     </row>
     <row r="30" spans="1:7" ht="17.25" thickBot="1">
       <c r="A30" s="20"/>
-      <c r="B30" s="44"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="46"/>
+      <c r="B30" s="52"/>
+      <c r="C30" s="53"/>
+      <c r="D30" s="53"/>
+      <c r="E30" s="53"/>
+      <c r="F30" s="53"/>
+      <c r="G30" s="54"/>
     </row>
     <row r="31" spans="1:7" ht="17.25" thickBot="1">
       <c r="A31" s="14"/>
@@ -3127,12 +3127,12 @@
     </row>
     <row r="37" spans="1:19" ht="17.25" thickBot="1">
       <c r="A37" s="23"/>
-      <c r="B37" s="50"/>
-      <c r="C37" s="51"/>
-      <c r="D37" s="51"/>
-      <c r="E37" s="51"/>
-      <c r="F37" s="51"/>
-      <c r="G37" s="52"/>
+      <c r="B37" s="58"/>
+      <c r="C37" s="59"/>
+      <c r="D37" s="59"/>
+      <c r="E37" s="59"/>
+      <c r="F37" s="59"/>
+      <c r="G37" s="60"/>
       <c r="I37" t="s">
         <v>22</v>
       </c>
@@ -3206,26 +3206,26 @@
         <v>123.75</v>
       </c>
       <c r="Q38" s="42">
-        <f>123.75+27.25</f>
-        <v>151</v>
+        <f>123.75+32.25</f>
+        <v>156</v>
       </c>
       <c r="R38" s="42">
-        <f>151+74.75</f>
-        <v>225.75</v>
+        <f>156+74.75</f>
+        <v>230.75</v>
       </c>
       <c r="S38" s="42">
-        <f>225.75+90.25</f>
-        <v>316</v>
+        <f>230.75+103.75</f>
+        <v>334.5</v>
       </c>
     </row>
     <row r="39" spans="1:19" ht="17.25" thickBot="1">
       <c r="A39" s="20"/>
-      <c r="B39" s="44"/>
-      <c r="C39" s="45"/>
-      <c r="D39" s="45"/>
-      <c r="E39" s="45"/>
-      <c r="F39" s="45"/>
-      <c r="G39" s="46"/>
+      <c r="B39" s="52"/>
+      <c r="C39" s="53"/>
+      <c r="D39" s="53"/>
+      <c r="E39" s="53"/>
+      <c r="F39" s="53"/>
+      <c r="G39" s="54"/>
       <c r="I39" t="s">
         <v>34</v>
       </c>
@@ -3286,12 +3286,12 @@
     </row>
     <row r="42" spans="1:19" ht="17.25" thickBot="1">
       <c r="A42" s="20"/>
-      <c r="B42" s="53"/>
-      <c r="C42" s="54"/>
-      <c r="D42" s="54"/>
-      <c r="E42" s="54"/>
-      <c r="F42" s="54"/>
-      <c r="G42" s="55"/>
+      <c r="B42" s="61"/>
+      <c r="C42" s="62"/>
+      <c r="D42" s="62"/>
+      <c r="E42" s="62"/>
+      <c r="F42" s="62"/>
+      <c r="G42" s="63"/>
     </row>
     <row r="43" spans="1:19" ht="17.25" thickBot="1">
       <c r="A43" s="14"/>
@@ -3331,12 +3331,12 @@
     </row>
     <row r="47" spans="1:19" ht="17.25" thickBot="1">
       <c r="A47" s="20"/>
-      <c r="B47" s="44"/>
-      <c r="C47" s="45"/>
-      <c r="D47" s="45"/>
-      <c r="E47" s="45"/>
-      <c r="F47" s="45"/>
-      <c r="G47" s="46"/>
+      <c r="B47" s="52"/>
+      <c r="C47" s="53"/>
+      <c r="D47" s="53"/>
+      <c r="E47" s="53"/>
+      <c r="F47" s="53"/>
+      <c r="G47" s="54"/>
     </row>
     <row r="48" spans="1:19" ht="17.25" thickBot="1">
       <c r="A48" s="14"/>
@@ -3367,12 +3367,12 @@
     </row>
     <row r="51" spans="1:7" ht="17.25" thickBot="1">
       <c r="A51" s="20"/>
-      <c r="B51" s="44"/>
-      <c r="C51" s="45"/>
-      <c r="D51" s="45"/>
-      <c r="E51" s="45"/>
-      <c r="F51" s="45"/>
-      <c r="G51" s="46"/>
+      <c r="B51" s="52"/>
+      <c r="C51" s="53"/>
+      <c r="D51" s="53"/>
+      <c r="E51" s="53"/>
+      <c r="F51" s="53"/>
+      <c r="G51" s="54"/>
     </row>
     <row r="52" spans="1:7" ht="17.25" thickBot="1">
       <c r="A52" s="14"/>
@@ -3403,12 +3403,12 @@
     </row>
     <row r="55" spans="1:7" ht="17.25" thickBot="1">
       <c r="A55" s="20"/>
-      <c r="B55" s="44"/>
-      <c r="C55" s="45"/>
-      <c r="D55" s="45"/>
-      <c r="E55" s="45"/>
-      <c r="F55" s="45"/>
-      <c r="G55" s="46"/>
+      <c r="B55" s="52"/>
+      <c r="C55" s="53"/>
+      <c r="D55" s="53"/>
+      <c r="E55" s="53"/>
+      <c r="F55" s="53"/>
+      <c r="G55" s="54"/>
     </row>
     <row r="56" spans="1:7" ht="17.25" thickBot="1">
       <c r="A56" s="14"/>
@@ -3439,12 +3439,12 @@
     </row>
     <row r="59" spans="1:7" ht="17.25" thickBot="1">
       <c r="A59" s="20"/>
-      <c r="B59" s="44"/>
-      <c r="C59" s="45"/>
-      <c r="D59" s="45"/>
-      <c r="E59" s="45"/>
-      <c r="F59" s="45"/>
-      <c r="G59" s="46"/>
+      <c r="B59" s="52"/>
+      <c r="C59" s="53"/>
+      <c r="D59" s="53"/>
+      <c r="E59" s="53"/>
+      <c r="F59" s="53"/>
+      <c r="G59" s="54"/>
     </row>
     <row r="60" spans="1:7" ht="17.25" thickBot="1">
       <c r="A60" s="14"/>
@@ -3484,12 +3484,12 @@
     </row>
     <row r="64" spans="1:7" ht="17.25" thickBot="1">
       <c r="A64" s="20"/>
-      <c r="B64" s="44"/>
-      <c r="C64" s="45"/>
-      <c r="D64" s="45"/>
-      <c r="E64" s="45"/>
-      <c r="F64" s="45"/>
-      <c r="G64" s="46"/>
+      <c r="B64" s="52"/>
+      <c r="C64" s="53"/>
+      <c r="D64" s="53"/>
+      <c r="E64" s="53"/>
+      <c r="F64" s="53"/>
+      <c r="G64" s="54"/>
     </row>
     <row r="65" spans="1:7" ht="17.25" thickBot="1">
       <c r="A65" s="14"/>
@@ -3502,12 +3502,12 @@
     </row>
     <row r="66" spans="1:7" ht="17.25" thickBot="1">
       <c r="A66" s="20"/>
-      <c r="B66" s="44"/>
-      <c r="C66" s="45"/>
-      <c r="D66" s="45"/>
-      <c r="E66" s="45"/>
-      <c r="F66" s="45"/>
-      <c r="G66" s="46"/>
+      <c r="B66" s="52"/>
+      <c r="C66" s="53"/>
+      <c r="D66" s="53"/>
+      <c r="E66" s="53"/>
+      <c r="F66" s="53"/>
+      <c r="G66" s="54"/>
     </row>
     <row r="67" spans="1:7" ht="17.25" thickBot="1">
       <c r="A67" s="14"/>
@@ -3529,12 +3529,12 @@
     </row>
     <row r="69" spans="1:7" ht="17.25" thickBot="1">
       <c r="A69" s="20"/>
-      <c r="B69" s="44"/>
-      <c r="C69" s="45"/>
-      <c r="D69" s="45"/>
-      <c r="E69" s="45"/>
-      <c r="F69" s="45"/>
-      <c r="G69" s="46"/>
+      <c r="B69" s="52"/>
+      <c r="C69" s="53"/>
+      <c r="D69" s="53"/>
+      <c r="E69" s="53"/>
+      <c r="F69" s="53"/>
+      <c r="G69" s="54"/>
     </row>
     <row r="70" spans="1:7" ht="17.25" thickBot="1">
       <c r="A70" s="14"/>
@@ -3583,12 +3583,12 @@
     </row>
     <row r="75" spans="1:7" ht="17.25" thickBot="1">
       <c r="A75" s="20"/>
-      <c r="B75" s="44"/>
-      <c r="C75" s="45"/>
-      <c r="D75" s="45"/>
-      <c r="E75" s="45"/>
-      <c r="F75" s="45"/>
-      <c r="G75" s="46"/>
+      <c r="B75" s="52"/>
+      <c r="C75" s="53"/>
+      <c r="D75" s="53"/>
+      <c r="E75" s="53"/>
+      <c r="F75" s="53"/>
+      <c r="G75" s="54"/>
     </row>
     <row r="76" spans="1:7" ht="17.25" thickBot="1">
       <c r="A76" s="14"/>
@@ -3610,12 +3610,12 @@
     </row>
     <row r="78" spans="1:7" ht="17.25" thickBot="1">
       <c r="A78" s="20"/>
-      <c r="B78" s="44"/>
-      <c r="C78" s="45"/>
-      <c r="D78" s="45"/>
-      <c r="E78" s="45"/>
-      <c r="F78" s="45"/>
-      <c r="G78" s="46"/>
+      <c r="B78" s="52"/>
+      <c r="C78" s="53"/>
+      <c r="D78" s="53"/>
+      <c r="E78" s="53"/>
+      <c r="F78" s="53"/>
+      <c r="G78" s="54"/>
     </row>
     <row r="79" spans="1:7" ht="17.25" thickBot="1">
       <c r="A79" s="14"/>
@@ -3655,12 +3655,12 @@
     </row>
     <row r="83" spans="1:7" ht="17.25" thickBot="1">
       <c r="A83" s="25"/>
-      <c r="B83" s="56"/>
-      <c r="C83" s="57"/>
-      <c r="D83" s="57"/>
-      <c r="E83" s="57"/>
-      <c r="F83" s="57"/>
-      <c r="G83" s="58"/>
+      <c r="B83" s="49"/>
+      <c r="C83" s="50"/>
+      <c r="D83" s="50"/>
+      <c r="E83" s="50"/>
+      <c r="F83" s="50"/>
+      <c r="G83" s="51"/>
     </row>
     <row r="84" spans="1:7" ht="17.25" thickBot="1">
       <c r="A84" s="9"/>
@@ -3721,13 +3721,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B83:G83"/>
-    <mergeCell ref="B59:G59"/>
-    <mergeCell ref="B64:G64"/>
-    <mergeCell ref="B66:G66"/>
-    <mergeCell ref="B69:G69"/>
-    <mergeCell ref="B75:G75"/>
-    <mergeCell ref="B78:G78"/>
     <mergeCell ref="B55:G55"/>
     <mergeCell ref="B4:G4"/>
     <mergeCell ref="B11:G11"/>
@@ -3740,6 +3733,13 @@
     <mergeCell ref="B42:G42"/>
     <mergeCell ref="B47:G47"/>
     <mergeCell ref="B51:G51"/>
+    <mergeCell ref="B83:G83"/>
+    <mergeCell ref="B59:G59"/>
+    <mergeCell ref="B64:G64"/>
+    <mergeCell ref="B66:G66"/>
+    <mergeCell ref="B69:G69"/>
+    <mergeCell ref="B75:G75"/>
+    <mergeCell ref="B78:G78"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
*Compiled the End of Project Report
</commit_message>
<xml_diff>
--- a/doc/End of Project Report/Graphs.xlsx
+++ b/doc/End of Project Report/Graphs.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="30" windowWidth="19395" windowHeight="7830"/>
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -163,15 +163,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="m&quot;月&quot;d&quot;日&quot;"/>
+    <numFmt numFmtId="164" formatCode="m&quot;月&quot;d&quot;日&quot;"/>
   </numFmts>
   <fonts count="11">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -236,7 +236,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -451,7 +451,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -526,6 +526,42 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -535,54 +571,33 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="zh-TW"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -606,11 +621,14 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -694,17 +712,18 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>13.25</c:v>
+                  <c:v>14.25</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>24.75</c:v>
+                  <c:v>27.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -800,6 +819,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -895,6 +915,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -990,6 +1011,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -1096,34 +1118,51 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="53223808"/>
-        <c:axId val="53225344"/>
+        <c:smooth val="0"/>
+        <c:axId val="64789888"/>
+        <c:axId val="64803968"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="53223808"/>
+        <c:axId val="64789888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53225344"/>
+        <c:crossAx val="64803968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53225344"/>
+        <c:axId val="64803968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0_);\(#,##0\)" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53223808"/>
+        <c:crossAx val="64789888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1131,8 +1170,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1144,7 +1186,17 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="zh-TW"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1167,15 +1219,29 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:view3D>
+      <c:rotX val="15"/>
+      <c:rotY val="20"/>
       <c:rAngAx val="1"/>
     </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+    </c:backWall>
     <c:plotArea>
       <c:layout/>
       <c:bar3DChart>
         <c:barDir val="col"/>
         <c:grouping val="percentStacked"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1190,6 +1256,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$P$3:$P$9</c:f>
@@ -1229,13 +1296,13 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>36.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>6</c:v>
@@ -1244,7 +1311,7 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.75</c:v>
+                  <c:v>9.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1264,6 +1331,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$P$3:$P$9</c:f>
@@ -1338,6 +1406,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$P$3:$P$9</c:f>
@@ -1412,6 +1481,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$P$3:$P$9</c:f>
@@ -1486,6 +1556,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$P$3:$P$9</c:f>
@@ -1546,34 +1617,50 @@
             </c:numRef>
           </c:val>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="53278208"/>
-        <c:axId val="53279744"/>
+        <c:axId val="66028288"/>
+        <c:axId val="66029824"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="53278208"/>
+        <c:axId val="66028288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53279744"/>
+        <c:crossAx val="66029824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53279744"/>
+        <c:axId val="66029824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53278208"/>
+        <c:crossAx val="66028288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1581,8 +1668,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1594,7 +1684,17 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="zh-TW"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1614,7 +1714,9 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -1629,6 +1731,7 @@
       </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1655,7 +1758,12 @@
                   <c:y val="2.242990654205608E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
@@ -1665,7 +1773,12 @@
                   <c:y val="-3.7383177570093469E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
@@ -1675,7 +1788,12 @@
                   <c:y val="-3.4890965732087144E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
@@ -1685,7 +1803,12 @@
                   <c:y val="-4.7352024922118409E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
@@ -1695,7 +1818,12 @@
                   <c:y val="-3.7383177570093566E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="5"/>
@@ -1705,7 +1833,12 @@
                   <c:y val="2.242990654205608E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="6"/>
@@ -1715,7 +1848,12 @@
                   <c:y val="2.242990654205608E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="7"/>
@@ -1725,9 +1863,20 @@
                   <c:y val="-1.4953271028037387E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
             </c:dLbl>
+            <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -1801,11 +1950,12 @@
                   <c:v>230.75</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>334.5</c:v>
+                  <c:v>337</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1833,7 +1983,12 @@
                   <c:y val="-2.9906542056074785E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
@@ -1843,7 +1998,12 @@
                   <c:y val="1.7445482866043617E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
@@ -1853,7 +2013,12 @@
                   <c:y val="9.9688473520249243E-3"/>
                 </c:manualLayout>
               </c:layout>
+              <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
@@ -1863,7 +2028,12 @@
                   <c:y val="1.4953271028037389E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="5"/>
@@ -1873,7 +2043,12 @@
                   <c:y val="-3.4890965732087144E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="6"/>
@@ -1883,7 +2058,12 @@
                   <c:y val="1.4953271028037389E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="7"/>
@@ -1893,7 +2073,12 @@
                   <c:y val="7.4766355140186954E-3"/>
                 </c:manualLayout>
               </c:layout>
+              <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="8"/>
@@ -1903,9 +2088,20 @@
                   <c:y val="2.2429906542056084E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
             </c:dLbl>
+            <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -1984,34 +2180,51 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="54768000"/>
-        <c:axId val="54769536"/>
+        <c:smooth val="0"/>
+        <c:axId val="66080768"/>
+        <c:axId val="66082304"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="54768000"/>
+        <c:axId val="66080768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54769536"/>
+        <c:crossAx val="66082304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="54769536"/>
+        <c:axId val="66082304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54768000"/>
+        <c:crossAx val="66080768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2028,8 +2241,11 @@
           <c:h val="0.18982137513184688"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -2135,7 +2351,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2209,6 +2425,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -2243,6 +2460,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2418,14 +2636,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F34" workbookViewId="0">
-      <selection activeCell="T39" sqref="T39"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="T42" sqref="T42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="2" max="2" width="30.5" customWidth="1"/>
     <col min="3" max="3" width="9.75" customWidth="1"/>
@@ -2435,7 +2653,7 @@
     <row r="1" spans="1:21" ht="21" thickBot="1">
       <c r="A1" s="1"/>
     </row>
-    <row r="2" spans="1:21" ht="17.25" thickBot="1">
+    <row r="2" spans="1:21" ht="16.5" thickBot="1">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
       <c r="C2" s="5"/>
@@ -2476,7 +2694,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="17.25" thickBot="1">
+    <row r="3" spans="1:21" ht="16.5" thickBot="1">
       <c r="A3" s="6"/>
       <c r="B3" s="7"/>
       <c r="C3" s="8"/>
@@ -2525,14 +2743,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="17.25" thickBot="1">
+    <row r="4" spans="1:21" ht="16.5" thickBot="1">
       <c r="A4" s="9"/>
-      <c r="B4" s="55"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="57"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="54"/>
       <c r="I4" s="34" t="s">
         <v>2</v>
       </c>
@@ -2559,7 +2777,7 @@
         <v>15</v>
       </c>
       <c r="Q4" s="39">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="R4" s="30">
         <v>7</v>
@@ -2574,7 +2792,7 @@
         <v>3.25</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="17.25" thickBot="1">
+    <row r="5" spans="1:21" ht="16.5" thickBot="1">
       <c r="A5" s="10"/>
       <c r="B5" s="11"/>
       <c r="C5" s="12"/>
@@ -2623,7 +2841,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="17.25" thickBot="1">
+    <row r="6" spans="1:21" ht="16.5" thickBot="1">
       <c r="A6" s="14"/>
       <c r="B6" s="15"/>
       <c r="C6" s="12"/>
@@ -2657,7 +2875,7 @@
         <v>18</v>
       </c>
       <c r="Q6" s="40">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R6" s="27">
         <v>7</v>
@@ -2672,7 +2890,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="17.25" thickBot="1">
+    <row r="7" spans="1:21" ht="16.5" thickBot="1">
       <c r="A7" s="14"/>
       <c r="B7" s="15"/>
       <c r="C7" s="12"/>
@@ -2721,7 +2939,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="17.25" thickBot="1">
+    <row r="8" spans="1:21" ht="16.5" thickBot="1">
       <c r="A8" s="14"/>
       <c r="B8" s="15"/>
       <c r="C8" s="12"/>
@@ -2770,7 +2988,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="17.25" thickBot="1">
+    <row r="9" spans="1:21" ht="16.5" thickBot="1">
       <c r="A9" s="14"/>
       <c r="B9" s="15"/>
       <c r="C9" s="12"/>
@@ -2804,7 +3022,7 @@
         <v>19</v>
       </c>
       <c r="Q9" s="40">
-        <v>7.75</v>
+        <v>9.25</v>
       </c>
       <c r="R9" s="27">
         <v>0</v>
@@ -2819,7 +3037,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="17.25" thickBot="1">
+    <row r="10" spans="1:21" ht="16.5" thickBot="1">
       <c r="A10" s="17"/>
       <c r="B10" s="18"/>
       <c r="C10" s="19"/>
@@ -2831,7 +3049,7 @@
         <v>8</v>
       </c>
       <c r="J10" s="45">
-        <v>13.25</v>
+        <v>14.25</v>
       </c>
       <c r="K10" s="46">
         <v>1</v>
@@ -2847,17 +3065,17 @@
       </c>
       <c r="O10">
         <f t="shared" si="0"/>
-        <v>32.25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" ht="17.25" thickBot="1">
+        <v>33.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="16.5" thickBot="1">
       <c r="A11" s="20"/>
-      <c r="B11" s="52"/>
-      <c r="C11" s="53"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="54"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="51"/>
       <c r="I11" s="34" t="s">
         <v>9</v>
       </c>
@@ -2881,7 +3099,7 @@
         <v>74.75</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="17.25" thickBot="1">
+    <row r="12" spans="1:21" ht="16.5" thickBot="1">
       <c r="A12" s="14"/>
       <c r="B12" s="15"/>
       <c r="C12" s="12"/>
@@ -2893,7 +3111,7 @@
         <v>20</v>
       </c>
       <c r="J12" s="45">
-        <v>24.75</v>
+        <v>27.25</v>
       </c>
       <c r="K12" s="46">
         <v>15.5</v>
@@ -2909,10 +3127,10 @@
       </c>
       <c r="O12">
         <f>SUM(J12:N12)</f>
-        <v>103.75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" ht="17.25" thickBot="1">
+        <v>106.25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="16.5" thickBot="1">
       <c r="A13" s="14"/>
       <c r="B13" s="15"/>
       <c r="C13" s="12"/>
@@ -2921,7 +3139,7 @@
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
     </row>
-    <row r="14" spans="1:21" ht="17.25" thickBot="1">
+    <row r="14" spans="1:21" ht="16.5" thickBot="1">
       <c r="A14" s="14"/>
       <c r="B14" s="15"/>
       <c r="C14" s="12"/>
@@ -2930,7 +3148,7 @@
       <c r="F14" s="13"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="1:21" ht="17.25" thickBot="1">
+    <row r="15" spans="1:21" ht="16.5" thickBot="1">
       <c r="A15" s="14"/>
       <c r="B15" s="15"/>
       <c r="C15" s="12"/>
@@ -2939,7 +3157,7 @@
       <c r="F15" s="16"/>
       <c r="G15" s="13"/>
     </row>
-    <row r="16" spans="1:21" ht="17.25" thickBot="1">
+    <row r="16" spans="1:21" ht="16.5" thickBot="1">
       <c r="A16" s="17"/>
       <c r="B16" s="18"/>
       <c r="C16" s="19"/>
@@ -2948,16 +3166,16 @@
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="1:7" ht="17.25" thickBot="1">
+    <row r="17" spans="1:7" ht="16.5" thickBot="1">
       <c r="A17" s="20"/>
-      <c r="B17" s="52"/>
-      <c r="C17" s="53"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="53"/>
-      <c r="G17" s="54"/>
-    </row>
-    <row r="18" spans="1:7" ht="17.25" thickBot="1">
+      <c r="B17" s="49"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="51"/>
+    </row>
+    <row r="18" spans="1:7" ht="16.5" thickBot="1">
       <c r="A18" s="14"/>
       <c r="B18" s="15"/>
       <c r="C18" s="12"/>
@@ -2966,7 +3184,7 @@
       <c r="F18" s="13"/>
       <c r="G18" s="16"/>
     </row>
-    <row r="19" spans="1:7" ht="17.25" thickBot="1">
+    <row r="19" spans="1:7" ht="16.5" thickBot="1">
       <c r="A19" s="14"/>
       <c r="B19" s="15"/>
       <c r="C19" s="12"/>
@@ -2975,7 +3193,7 @@
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
     </row>
-    <row r="20" spans="1:7" ht="17.25" thickBot="1">
+    <row r="20" spans="1:7" ht="16.5" thickBot="1">
       <c r="A20" s="14"/>
       <c r="B20" s="15"/>
       <c r="C20" s="12"/>
@@ -2984,7 +3202,7 @@
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
     </row>
-    <row r="21" spans="1:7" ht="17.25" thickBot="1">
+    <row r="21" spans="1:7" ht="16.5" thickBot="1">
       <c r="A21" s="14"/>
       <c r="B21" s="15"/>
       <c r="C21" s="12"/>
@@ -2993,7 +3211,7 @@
       <c r="F21" s="16"/>
       <c r="G21" s="13"/>
     </row>
-    <row r="22" spans="1:7" ht="17.25" thickBot="1">
+    <row r="22" spans="1:7" ht="16.5" thickBot="1">
       <c r="A22" s="14"/>
       <c r="B22" s="15"/>
       <c r="C22" s="12"/>
@@ -3002,16 +3220,16 @@
       <c r="F22" s="16"/>
       <c r="G22" s="16"/>
     </row>
-    <row r="23" spans="1:7" ht="17.25" thickBot="1">
+    <row r="23" spans="1:7" ht="16.5" thickBot="1">
       <c r="A23" s="20"/>
-      <c r="B23" s="52"/>
-      <c r="C23" s="53"/>
-      <c r="D23" s="53"/>
-      <c r="E23" s="53"/>
-      <c r="F23" s="53"/>
-      <c r="G23" s="54"/>
-    </row>
-    <row r="24" spans="1:7" ht="17.25" thickBot="1">
+      <c r="B23" s="49"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="51"/>
+    </row>
+    <row r="24" spans="1:7" ht="16.5" thickBot="1">
       <c r="A24" s="14"/>
       <c r="B24" s="15"/>
       <c r="C24" s="12"/>
@@ -3020,7 +3238,7 @@
       <c r="F24" s="16"/>
       <c r="G24" s="16"/>
     </row>
-    <row r="25" spans="1:7" ht="17.25" thickBot="1">
+    <row r="25" spans="1:7" ht="16.5" thickBot="1">
       <c r="A25" s="14"/>
       <c r="B25" s="15"/>
       <c r="C25" s="12"/>
@@ -3029,7 +3247,7 @@
       <c r="F25" s="13"/>
       <c r="G25" s="13"/>
     </row>
-    <row r="26" spans="1:7" ht="17.25" thickBot="1">
+    <row r="26" spans="1:7" ht="16.5" thickBot="1">
       <c r="A26" s="17"/>
       <c r="B26" s="18"/>
       <c r="C26" s="19"/>
@@ -3038,16 +3256,16 @@
       <c r="F26" s="8"/>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" spans="1:7" ht="17.25" thickBot="1">
+    <row r="27" spans="1:7" ht="16.5" thickBot="1">
       <c r="A27" s="20"/>
-      <c r="B27" s="52"/>
-      <c r="C27" s="53"/>
-      <c r="D27" s="53"/>
-      <c r="E27" s="53"/>
-      <c r="F27" s="53"/>
-      <c r="G27" s="54"/>
-    </row>
-    <row r="28" spans="1:7" ht="17.25" thickBot="1">
+      <c r="B27" s="49"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="50"/>
+      <c r="E27" s="50"/>
+      <c r="F27" s="50"/>
+      <c r="G27" s="51"/>
+    </row>
+    <row r="28" spans="1:7" ht="16.5" thickBot="1">
       <c r="A28" s="14"/>
       <c r="B28" s="15"/>
       <c r="C28" s="12"/>
@@ -3056,7 +3274,7 @@
       <c r="F28" s="13"/>
       <c r="G28" s="13"/>
     </row>
-    <row r="29" spans="1:7" ht="17.25" thickBot="1">
+    <row r="29" spans="1:7" ht="16.5" thickBot="1">
       <c r="A29" s="14"/>
       <c r="B29" s="21"/>
       <c r="C29" s="12"/>
@@ -3065,16 +3283,16 @@
       <c r="F29" s="13"/>
       <c r="G29" s="13"/>
     </row>
-    <row r="30" spans="1:7" ht="17.25" thickBot="1">
+    <row r="30" spans="1:7" ht="16.5" thickBot="1">
       <c r="A30" s="20"/>
-      <c r="B30" s="52"/>
-      <c r="C30" s="53"/>
-      <c r="D30" s="53"/>
-      <c r="E30" s="53"/>
-      <c r="F30" s="53"/>
-      <c r="G30" s="54"/>
-    </row>
-    <row r="31" spans="1:7" ht="17.25" thickBot="1">
+      <c r="B30" s="49"/>
+      <c r="C30" s="50"/>
+      <c r="D30" s="50"/>
+      <c r="E30" s="50"/>
+      <c r="F30" s="50"/>
+      <c r="G30" s="51"/>
+    </row>
+    <row r="31" spans="1:7" ht="16.5" thickBot="1">
       <c r="A31" s="14"/>
       <c r="B31" s="15"/>
       <c r="C31" s="12"/>
@@ -3083,7 +3301,7 @@
       <c r="F31" s="16"/>
       <c r="G31" s="16"/>
     </row>
-    <row r="32" spans="1:7" ht="17.25" thickBot="1">
+    <row r="32" spans="1:7" ht="16.5" thickBot="1">
       <c r="A32" s="14"/>
       <c r="B32" s="15"/>
       <c r="C32" s="12"/>
@@ -3092,7 +3310,7 @@
       <c r="F32" s="13"/>
       <c r="G32" s="13"/>
     </row>
-    <row r="33" spans="1:19" ht="17.25" thickBot="1">
+    <row r="33" spans="1:19" ht="16.5" thickBot="1">
       <c r="A33" s="17"/>
       <c r="B33" s="22"/>
       <c r="C33" s="19"/>
@@ -3101,10 +3319,10 @@
       <c r="F33" s="8"/>
       <c r="G33" s="8"/>
     </row>
-    <row r="34" spans="1:19" ht="17.25" thickBot="1">
+    <row r="34" spans="1:19" ht="16.5" thickBot="1">
       <c r="A34" s="2"/>
     </row>
-    <row r="35" spans="1:19" ht="17.25" thickBot="1">
+    <row r="35" spans="1:19" ht="16.5" thickBot="1">
       <c r="A35" s="3"/>
       <c r="B35" s="4"/>
       <c r="C35" s="5"/>
@@ -3113,7 +3331,7 @@
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
     </row>
-    <row r="36" spans="1:19" ht="17.25" thickBot="1">
+    <row r="36" spans="1:19" ht="16.5" thickBot="1">
       <c r="A36" s="6"/>
       <c r="B36" s="7"/>
       <c r="C36" s="8"/>
@@ -3125,14 +3343,14 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:19" ht="17.25" thickBot="1">
+    <row r="37" spans="1:19" ht="16.5" thickBot="1">
       <c r="A37" s="23"/>
-      <c r="B37" s="58"/>
-      <c r="C37" s="59"/>
-      <c r="D37" s="59"/>
-      <c r="E37" s="59"/>
-      <c r="F37" s="59"/>
-      <c r="G37" s="60"/>
+      <c r="B37" s="55"/>
+      <c r="C37" s="56"/>
+      <c r="D37" s="56"/>
+      <c r="E37" s="56"/>
+      <c r="F37" s="56"/>
+      <c r="G37" s="57"/>
       <c r="I37" t="s">
         <v>22</v>
       </c>
@@ -3167,7 +3385,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="17.25" thickBot="1">
+    <row r="38" spans="1:19" ht="16.5" thickBot="1">
       <c r="A38" s="14"/>
       <c r="B38" s="15"/>
       <c r="C38" s="12"/>
@@ -3214,18 +3432,18 @@
         <v>230.75</v>
       </c>
       <c r="S38" s="42">
-        <f>230.75+103.75</f>
-        <v>334.5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:19" ht="17.25" thickBot="1">
+        <f>230.75+103.75+2.5</f>
+        <v>337</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" ht="16.5" thickBot="1">
       <c r="A39" s="20"/>
-      <c r="B39" s="52"/>
-      <c r="C39" s="53"/>
-      <c r="D39" s="53"/>
-      <c r="E39" s="53"/>
-      <c r="F39" s="53"/>
-      <c r="G39" s="54"/>
+      <c r="B39" s="49"/>
+      <c r="C39" s="50"/>
+      <c r="D39" s="50"/>
+      <c r="E39" s="50"/>
+      <c r="F39" s="50"/>
+      <c r="G39" s="51"/>
       <c r="I39" t="s">
         <v>34</v>
       </c>
@@ -3266,7 +3484,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="17.25" thickBot="1">
+    <row r="40" spans="1:19" ht="16.5" thickBot="1">
       <c r="A40" s="14"/>
       <c r="B40" s="15"/>
       <c r="C40" s="12"/>
@@ -3275,7 +3493,7 @@
       <c r="F40" s="16"/>
       <c r="G40" s="16"/>
     </row>
-    <row r="41" spans="1:19" ht="17.25" thickBot="1">
+    <row r="41" spans="1:19" ht="16.5" thickBot="1">
       <c r="A41" s="14"/>
       <c r="B41" s="15"/>
       <c r="C41" s="12"/>
@@ -3284,16 +3502,16 @@
       <c r="F41" s="16"/>
       <c r="G41" s="16"/>
     </row>
-    <row r="42" spans="1:19" ht="17.25" thickBot="1">
+    <row r="42" spans="1:19" ht="16.5" thickBot="1">
       <c r="A42" s="20"/>
-      <c r="B42" s="61"/>
-      <c r="C42" s="62"/>
-      <c r="D42" s="62"/>
-      <c r="E42" s="62"/>
-      <c r="F42" s="62"/>
-      <c r="G42" s="63"/>
-    </row>
-    <row r="43" spans="1:19" ht="17.25" thickBot="1">
+      <c r="B42" s="58"/>
+      <c r="C42" s="59"/>
+      <c r="D42" s="59"/>
+      <c r="E42" s="59"/>
+      <c r="F42" s="59"/>
+      <c r="G42" s="60"/>
+    </row>
+    <row r="43" spans="1:19" ht="16.5" thickBot="1">
       <c r="A43" s="14"/>
       <c r="B43" s="15"/>
       <c r="C43" s="12"/>
@@ -3302,7 +3520,7 @@
       <c r="F43" s="16"/>
       <c r="G43" s="16"/>
     </row>
-    <row r="44" spans="1:19" ht="17.25" thickBot="1">
+    <row r="44" spans="1:19" ht="16.5" thickBot="1">
       <c r="A44" s="14"/>
       <c r="B44" s="15"/>
       <c r="C44" s="12"/>
@@ -3311,7 +3529,7 @@
       <c r="F44" s="16"/>
       <c r="G44" s="16"/>
     </row>
-    <row r="45" spans="1:19" ht="17.25" thickBot="1">
+    <row r="45" spans="1:19" ht="16.5" thickBot="1">
       <c r="A45" s="14"/>
       <c r="B45" s="15"/>
       <c r="C45" s="12"/>
@@ -3320,7 +3538,7 @@
       <c r="F45" s="16"/>
       <c r="G45" s="16"/>
     </row>
-    <row r="46" spans="1:19" ht="17.25" thickBot="1">
+    <row r="46" spans="1:19" ht="16.5" thickBot="1">
       <c r="A46" s="17"/>
       <c r="B46" s="18"/>
       <c r="C46" s="19"/>
@@ -3329,16 +3547,16 @@
       <c r="F46" s="8"/>
       <c r="G46" s="8"/>
     </row>
-    <row r="47" spans="1:19" ht="17.25" thickBot="1">
+    <row r="47" spans="1:19" ht="16.5" thickBot="1">
       <c r="A47" s="20"/>
-      <c r="B47" s="52"/>
-      <c r="C47" s="53"/>
-      <c r="D47" s="53"/>
-      <c r="E47" s="53"/>
-      <c r="F47" s="53"/>
-      <c r="G47" s="54"/>
-    </row>
-    <row r="48" spans="1:19" ht="17.25" thickBot="1">
+      <c r="B47" s="49"/>
+      <c r="C47" s="50"/>
+      <c r="D47" s="50"/>
+      <c r="E47" s="50"/>
+      <c r="F47" s="50"/>
+      <c r="G47" s="51"/>
+    </row>
+    <row r="48" spans="1:19" ht="16.5" thickBot="1">
       <c r="A48" s="14"/>
       <c r="B48" s="15"/>
       <c r="C48" s="12"/>
@@ -3347,7 +3565,7 @@
       <c r="F48" s="16"/>
       <c r="G48" s="16"/>
     </row>
-    <row r="49" spans="1:7" ht="17.25" thickBot="1">
+    <row r="49" spans="1:7" ht="16.5" thickBot="1">
       <c r="A49" s="14"/>
       <c r="B49" s="15"/>
       <c r="C49" s="12"/>
@@ -3356,7 +3574,7 @@
       <c r="F49" s="16"/>
       <c r="G49" s="16"/>
     </row>
-    <row r="50" spans="1:7" ht="17.25" thickBot="1">
+    <row r="50" spans="1:7" ht="16.5" thickBot="1">
       <c r="A50" s="17"/>
       <c r="B50" s="18"/>
       <c r="C50" s="19"/>
@@ -3365,16 +3583,16 @@
       <c r="F50" s="8"/>
       <c r="G50" s="8"/>
     </row>
-    <row r="51" spans="1:7" ht="17.25" thickBot="1">
+    <row r="51" spans="1:7" ht="16.5" thickBot="1">
       <c r="A51" s="20"/>
-      <c r="B51" s="52"/>
-      <c r="C51" s="53"/>
-      <c r="D51" s="53"/>
-      <c r="E51" s="53"/>
-      <c r="F51" s="53"/>
-      <c r="G51" s="54"/>
-    </row>
-    <row r="52" spans="1:7" ht="17.25" thickBot="1">
+      <c r="B51" s="49"/>
+      <c r="C51" s="50"/>
+      <c r="D51" s="50"/>
+      <c r="E51" s="50"/>
+      <c r="F51" s="50"/>
+      <c r="G51" s="51"/>
+    </row>
+    <row r="52" spans="1:7" ht="16.5" thickBot="1">
       <c r="A52" s="14"/>
       <c r="B52" s="15"/>
       <c r="C52" s="12"/>
@@ -3383,7 +3601,7 @@
       <c r="F52" s="16"/>
       <c r="G52" s="16"/>
     </row>
-    <row r="53" spans="1:7" ht="17.25" thickBot="1">
+    <row r="53" spans="1:7" ht="16.5" thickBot="1">
       <c r="A53" s="14"/>
       <c r="B53" s="15"/>
       <c r="C53" s="12"/>
@@ -3392,7 +3610,7 @@
       <c r="F53" s="16"/>
       <c r="G53" s="16"/>
     </row>
-    <row r="54" spans="1:7" ht="17.25" thickBot="1">
+    <row r="54" spans="1:7" ht="16.5" thickBot="1">
       <c r="A54" s="17"/>
       <c r="B54" s="18"/>
       <c r="C54" s="19"/>
@@ -3401,16 +3619,16 @@
       <c r="F54" s="8"/>
       <c r="G54" s="8"/>
     </row>
-    <row r="55" spans="1:7" ht="17.25" thickBot="1">
+    <row r="55" spans="1:7" ht="16.5" thickBot="1">
       <c r="A55" s="20"/>
-      <c r="B55" s="52"/>
-      <c r="C55" s="53"/>
-      <c r="D55" s="53"/>
-      <c r="E55" s="53"/>
-      <c r="F55" s="53"/>
-      <c r="G55" s="54"/>
-    </row>
-    <row r="56" spans="1:7" ht="17.25" thickBot="1">
+      <c r="B55" s="49"/>
+      <c r="C55" s="50"/>
+      <c r="D55" s="50"/>
+      <c r="E55" s="50"/>
+      <c r="F55" s="50"/>
+      <c r="G55" s="51"/>
+    </row>
+    <row r="56" spans="1:7" ht="16.5" thickBot="1">
       <c r="A56" s="14"/>
       <c r="B56" s="15"/>
       <c r="C56" s="12"/>
@@ -3419,7 +3637,7 @@
       <c r="F56" s="16"/>
       <c r="G56" s="16"/>
     </row>
-    <row r="57" spans="1:7" ht="17.25" thickBot="1">
+    <row r="57" spans="1:7" ht="16.5" thickBot="1">
       <c r="A57" s="24"/>
       <c r="B57" s="15"/>
       <c r="C57" s="12"/>
@@ -3428,7 +3646,7 @@
       <c r="F57" s="16"/>
       <c r="G57" s="16"/>
     </row>
-    <row r="58" spans="1:7" ht="17.25" thickBot="1">
+    <row r="58" spans="1:7" ht="16.5" thickBot="1">
       <c r="A58" s="14"/>
       <c r="B58" s="15"/>
       <c r="C58" s="12"/>
@@ -3437,16 +3655,16 @@
       <c r="F58" s="16"/>
       <c r="G58" s="16"/>
     </row>
-    <row r="59" spans="1:7" ht="17.25" thickBot="1">
+    <row r="59" spans="1:7" ht="16.5" thickBot="1">
       <c r="A59" s="20"/>
-      <c r="B59" s="52"/>
-      <c r="C59" s="53"/>
-      <c r="D59" s="53"/>
-      <c r="E59" s="53"/>
-      <c r="F59" s="53"/>
-      <c r="G59" s="54"/>
-    </row>
-    <row r="60" spans="1:7" ht="17.25" thickBot="1">
+      <c r="B59" s="49"/>
+      <c r="C59" s="50"/>
+      <c r="D59" s="50"/>
+      <c r="E59" s="50"/>
+      <c r="F59" s="50"/>
+      <c r="G59" s="51"/>
+    </row>
+    <row r="60" spans="1:7" ht="16.5" thickBot="1">
       <c r="A60" s="14"/>
       <c r="B60" s="15"/>
       <c r="C60" s="12"/>
@@ -3455,7 +3673,7 @@
       <c r="F60" s="16"/>
       <c r="G60" s="16"/>
     </row>
-    <row r="61" spans="1:7" ht="17.25" thickBot="1">
+    <row r="61" spans="1:7" ht="16.5" thickBot="1">
       <c r="A61" s="14"/>
       <c r="B61" s="15"/>
       <c r="C61" s="12"/>
@@ -3464,7 +3682,7 @@
       <c r="F61" s="16"/>
       <c r="G61" s="16"/>
     </row>
-    <row r="62" spans="1:7" ht="17.25" thickBot="1">
+    <row r="62" spans="1:7" ht="16.5" thickBot="1">
       <c r="A62" s="14"/>
       <c r="B62" s="15"/>
       <c r="C62" s="12"/>
@@ -3473,7 +3691,7 @@
       <c r="F62" s="16"/>
       <c r="G62" s="16"/>
     </row>
-    <row r="63" spans="1:7" ht="17.25" thickBot="1">
+    <row r="63" spans="1:7" ht="16.5" thickBot="1">
       <c r="A63" s="14"/>
       <c r="B63" s="15"/>
       <c r="C63" s="12"/>
@@ -3482,16 +3700,16 @@
       <c r="F63" s="16"/>
       <c r="G63" s="16"/>
     </row>
-    <row r="64" spans="1:7" ht="17.25" thickBot="1">
+    <row r="64" spans="1:7" ht="16.5" thickBot="1">
       <c r="A64" s="20"/>
-      <c r="B64" s="52"/>
-      <c r="C64" s="53"/>
-      <c r="D64" s="53"/>
-      <c r="E64" s="53"/>
-      <c r="F64" s="53"/>
-      <c r="G64" s="54"/>
-    </row>
-    <row r="65" spans="1:7" ht="17.25" thickBot="1">
+      <c r="B64" s="49"/>
+      <c r="C64" s="50"/>
+      <c r="D64" s="50"/>
+      <c r="E64" s="50"/>
+      <c r="F64" s="50"/>
+      <c r="G64" s="51"/>
+    </row>
+    <row r="65" spans="1:7" ht="16.5" thickBot="1">
       <c r="A65" s="14"/>
       <c r="B65" s="15"/>
       <c r="C65" s="12"/>
@@ -3500,16 +3718,16 @@
       <c r="F65" s="16"/>
       <c r="G65" s="16"/>
     </row>
-    <row r="66" spans="1:7" ht="17.25" thickBot="1">
+    <row r="66" spans="1:7" ht="16.5" thickBot="1">
       <c r="A66" s="20"/>
-      <c r="B66" s="52"/>
-      <c r="C66" s="53"/>
-      <c r="D66" s="53"/>
-      <c r="E66" s="53"/>
-      <c r="F66" s="53"/>
-      <c r="G66" s="54"/>
-    </row>
-    <row r="67" spans="1:7" ht="17.25" thickBot="1">
+      <c r="B66" s="49"/>
+      <c r="C66" s="50"/>
+      <c r="D66" s="50"/>
+      <c r="E66" s="50"/>
+      <c r="F66" s="50"/>
+      <c r="G66" s="51"/>
+    </row>
+    <row r="67" spans="1:7" ht="16.5" thickBot="1">
       <c r="A67" s="14"/>
       <c r="B67" s="15"/>
       <c r="C67" s="12"/>
@@ -3518,7 +3736,7 @@
       <c r="F67" s="16"/>
       <c r="G67" s="16"/>
     </row>
-    <row r="68" spans="1:7" ht="17.25" thickBot="1">
+    <row r="68" spans="1:7" ht="16.5" thickBot="1">
       <c r="A68" s="17"/>
       <c r="B68" s="18"/>
       <c r="C68" s="19"/>
@@ -3527,16 +3745,16 @@
       <c r="F68" s="8"/>
       <c r="G68" s="8"/>
     </row>
-    <row r="69" spans="1:7" ht="17.25" thickBot="1">
+    <row r="69" spans="1:7" ht="16.5" thickBot="1">
       <c r="A69" s="20"/>
-      <c r="B69" s="52"/>
-      <c r="C69" s="53"/>
-      <c r="D69" s="53"/>
-      <c r="E69" s="53"/>
-      <c r="F69" s="53"/>
-      <c r="G69" s="54"/>
-    </row>
-    <row r="70" spans="1:7" ht="17.25" thickBot="1">
+      <c r="B69" s="49"/>
+      <c r="C69" s="50"/>
+      <c r="D69" s="50"/>
+      <c r="E69" s="50"/>
+      <c r="F69" s="50"/>
+      <c r="G69" s="51"/>
+    </row>
+    <row r="70" spans="1:7" ht="16.5" thickBot="1">
       <c r="A70" s="14"/>
       <c r="B70" s="15"/>
       <c r="C70" s="12"/>
@@ -3545,7 +3763,7 @@
       <c r="F70" s="16"/>
       <c r="G70" s="16"/>
     </row>
-    <row r="71" spans="1:7" ht="17.25" thickBot="1">
+    <row r="71" spans="1:7" ht="16.5" thickBot="1">
       <c r="A71" s="14"/>
       <c r="B71" s="15"/>
       <c r="C71" s="12"/>
@@ -3554,7 +3772,7 @@
       <c r="F71" s="16"/>
       <c r="G71" s="16"/>
     </row>
-    <row r="72" spans="1:7" ht="17.25" thickBot="1">
+    <row r="72" spans="1:7" ht="16.5" thickBot="1">
       <c r="A72" s="14"/>
       <c r="B72" s="15"/>
       <c r="C72" s="12"/>
@@ -3563,7 +3781,7 @@
       <c r="F72" s="16"/>
       <c r="G72" s="16"/>
     </row>
-    <row r="73" spans="1:7" ht="17.25" thickBot="1">
+    <row r="73" spans="1:7" ht="16.5" thickBot="1">
       <c r="A73" s="14"/>
       <c r="B73" s="15"/>
       <c r="C73" s="12"/>
@@ -3572,7 +3790,7 @@
       <c r="F73" s="16"/>
       <c r="G73" s="16"/>
     </row>
-    <row r="74" spans="1:7" ht="17.25" thickBot="1">
+    <row r="74" spans="1:7" ht="16.5" thickBot="1">
       <c r="A74" s="14"/>
       <c r="B74" s="15"/>
       <c r="C74" s="12"/>
@@ -3581,16 +3799,16 @@
       <c r="F74" s="16"/>
       <c r="G74" s="16"/>
     </row>
-    <row r="75" spans="1:7" ht="17.25" thickBot="1">
+    <row r="75" spans="1:7" ht="16.5" thickBot="1">
       <c r="A75" s="20"/>
-      <c r="B75" s="52"/>
-      <c r="C75" s="53"/>
-      <c r="D75" s="53"/>
-      <c r="E75" s="53"/>
-      <c r="F75" s="53"/>
-      <c r="G75" s="54"/>
-    </row>
-    <row r="76" spans="1:7" ht="17.25" thickBot="1">
+      <c r="B75" s="49"/>
+      <c r="C75" s="50"/>
+      <c r="D75" s="50"/>
+      <c r="E75" s="50"/>
+      <c r="F75" s="50"/>
+      <c r="G75" s="51"/>
+    </row>
+    <row r="76" spans="1:7" ht="16.5" thickBot="1">
       <c r="A76" s="14"/>
       <c r="B76" s="15"/>
       <c r="C76" s="12"/>
@@ -3599,7 +3817,7 @@
       <c r="F76" s="16"/>
       <c r="G76" s="16"/>
     </row>
-    <row r="77" spans="1:7" ht="17.25" thickBot="1">
+    <row r="77" spans="1:7" ht="16.5" thickBot="1">
       <c r="A77" s="14"/>
       <c r="B77" s="15"/>
       <c r="C77" s="12"/>
@@ -3608,16 +3826,16 @@
       <c r="F77" s="16"/>
       <c r="G77" s="16"/>
     </row>
-    <row r="78" spans="1:7" ht="17.25" thickBot="1">
+    <row r="78" spans="1:7" ht="16.5" thickBot="1">
       <c r="A78" s="20"/>
-      <c r="B78" s="52"/>
-      <c r="C78" s="53"/>
-      <c r="D78" s="53"/>
-      <c r="E78" s="53"/>
-      <c r="F78" s="53"/>
-      <c r="G78" s="54"/>
-    </row>
-    <row r="79" spans="1:7" ht="17.25" thickBot="1">
+      <c r="B78" s="49"/>
+      <c r="C78" s="50"/>
+      <c r="D78" s="50"/>
+      <c r="E78" s="50"/>
+      <c r="F78" s="50"/>
+      <c r="G78" s="51"/>
+    </row>
+    <row r="79" spans="1:7" ht="16.5" thickBot="1">
       <c r="A79" s="14"/>
       <c r="B79" s="15"/>
       <c r="C79" s="12"/>
@@ -3626,7 +3844,7 @@
       <c r="F79" s="16"/>
       <c r="G79" s="16"/>
     </row>
-    <row r="80" spans="1:7" ht="17.25" thickBot="1">
+    <row r="80" spans="1:7" ht="16.5" thickBot="1">
       <c r="A80" s="17"/>
       <c r="B80" s="22"/>
       <c r="C80" s="19"/>
@@ -3635,7 +3853,7 @@
       <c r="F80" s="8"/>
       <c r="G80" s="8"/>
     </row>
-    <row r="81" spans="1:7" ht="17.25" thickBot="1">
+    <row r="81" spans="1:7" ht="16.5" thickBot="1">
       <c r="A81" s="25"/>
       <c r="B81" s="26"/>
       <c r="C81" s="27"/>
@@ -3644,7 +3862,7 @@
       <c r="F81" s="28"/>
       <c r="G81" s="28"/>
     </row>
-    <row r="82" spans="1:7" ht="17.25" thickBot="1">
+    <row r="82" spans="1:7" ht="16.5" thickBot="1">
       <c r="A82" s="25"/>
       <c r="B82" s="29"/>
       <c r="C82" s="27"/>
@@ -3653,16 +3871,16 @@
       <c r="F82" s="28"/>
       <c r="G82" s="28"/>
     </row>
-    <row r="83" spans="1:7" ht="17.25" thickBot="1">
+    <row r="83" spans="1:7" ht="16.5" thickBot="1">
       <c r="A83" s="25"/>
-      <c r="B83" s="49"/>
-      <c r="C83" s="50"/>
-      <c r="D83" s="50"/>
-      <c r="E83" s="50"/>
-      <c r="F83" s="50"/>
-      <c r="G83" s="51"/>
-    </row>
-    <row r="84" spans="1:7" ht="17.25" thickBot="1">
+      <c r="B83" s="61"/>
+      <c r="C83" s="62"/>
+      <c r="D83" s="62"/>
+      <c r="E83" s="62"/>
+      <c r="F83" s="62"/>
+      <c r="G83" s="63"/>
+    </row>
+    <row r="84" spans="1:7" ht="16.5" thickBot="1">
       <c r="A84" s="9"/>
       <c r="B84" s="29"/>
       <c r="C84" s="30"/>
@@ -3671,7 +3889,7 @@
       <c r="F84" s="31"/>
       <c r="G84" s="31"/>
     </row>
-    <row r="85" spans="1:7" ht="17.25" thickBot="1">
+    <row r="85" spans="1:7" ht="16.5" thickBot="1">
       <c r="A85" s="23"/>
       <c r="B85" s="32"/>
       <c r="C85" s="30"/>
@@ -3680,7 +3898,7 @@
       <c r="F85" s="31"/>
       <c r="G85" s="31"/>
     </row>
-    <row r="86" spans="1:7" ht="17.25" thickBot="1">
+    <row r="86" spans="1:7" ht="16.5" thickBot="1">
       <c r="A86" s="23"/>
       <c r="B86" s="32"/>
       <c r="C86" s="27"/>
@@ -3689,7 +3907,7 @@
       <c r="F86" s="28"/>
       <c r="G86" s="28"/>
     </row>
-    <row r="87" spans="1:7" ht="17.25" thickBot="1">
+    <row r="87" spans="1:7" ht="16.5" thickBot="1">
       <c r="A87" s="23"/>
       <c r="B87" s="32"/>
       <c r="C87" s="27"/>
@@ -3698,7 +3916,7 @@
       <c r="F87" s="28"/>
       <c r="G87" s="28"/>
     </row>
-    <row r="88" spans="1:7" ht="17.25" thickBot="1">
+    <row r="88" spans="1:7" ht="16.5" thickBot="1">
       <c r="A88" s="23"/>
       <c r="B88" s="33"/>
       <c r="C88" s="27"/>
@@ -3707,7 +3925,7 @@
       <c r="F88" s="28"/>
       <c r="G88" s="28"/>
     </row>
-    <row r="89" spans="1:7" ht="17.25" thickBot="1">
+    <row r="89" spans="1:7" ht="16.5" thickBot="1">
       <c r="A89" s="23"/>
       <c r="B89" s="32"/>
       <c r="C89" s="27"/>
@@ -3721,6 +3939,13 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B83:G83"/>
+    <mergeCell ref="B59:G59"/>
+    <mergeCell ref="B64:G64"/>
+    <mergeCell ref="B66:G66"/>
+    <mergeCell ref="B69:G69"/>
+    <mergeCell ref="B75:G75"/>
+    <mergeCell ref="B78:G78"/>
     <mergeCell ref="B55:G55"/>
     <mergeCell ref="B4:G4"/>
     <mergeCell ref="B11:G11"/>
@@ -3733,13 +3958,6 @@
     <mergeCell ref="B42:G42"/>
     <mergeCell ref="B47:G47"/>
     <mergeCell ref="B51:G51"/>
-    <mergeCell ref="B83:G83"/>
-    <mergeCell ref="B59:G59"/>
-    <mergeCell ref="B64:G64"/>
-    <mergeCell ref="B66:G66"/>
-    <mergeCell ref="B69:G69"/>
-    <mergeCell ref="B75:G75"/>
-    <mergeCell ref="B78:G78"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3749,12 +3967,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData/>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3762,12 +3980,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData/>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>